<commit_message>
<UI, Feature> Icons, Refactoring Attributes
Started implementing gear system.
Gear has attribute modifiers.
Characters have gear slots.
Gear types affect which slot they take up.
Gear can only be equipped if there is enough space in the character's
inventory.
Updated weapon names- no more placeholders.
Icon design based around medieval imagery.
Refactored some classes so they can be reused in later projects.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13200" firstSheet="1" activeTab="9"/>
+    <workbookView windowWidth="28695" windowHeight="13200" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="WeightData" sheetId="1" r:id="rId1"/>
@@ -202,7 +202,7 @@
     <t>Handsnapper</t>
   </si>
   <si>
-    <t>T4Pistol</t>
+    <t>Saltscraper</t>
   </si>
   <si>
     <t>Deathgrip</t>
@@ -211,15 +211,15 @@
     <t>Rifle</t>
   </si>
   <si>
-    <t>Snipper</t>
-  </si>
-  <si>
     <t>Groundrider</t>
   </si>
   <si>
     <t>Longstrider</t>
   </si>
   <si>
+    <t>Deepdriver</t>
+  </si>
+  <si>
     <t>Shoulderbreaker</t>
   </si>
   <si>
@@ -229,16 +229,16 @@
     <t>Shotgun</t>
   </si>
   <si>
-    <t>Banger</t>
-  </si>
-  <si>
     <t>Leadspreader</t>
   </si>
   <si>
-    <t>T3Shotgun</t>
-  </si>
-  <si>
-    <t>T4Shotgun</t>
+    <t>Steelsweeper</t>
+  </si>
+  <si>
+    <t>Bonebreaker</t>
+  </si>
+  <si>
+    <t>Skullcrusher</t>
   </si>
   <si>
     <t>Hellsmasher</t>
@@ -250,13 +250,13 @@
     <t>Rattler</t>
   </si>
   <si>
-    <t>Saltscraper</t>
-  </si>
-  <si>
-    <t>T3SMG</t>
-  </si>
-  <si>
-    <t>T4SMG</t>
+    <t>Gripshaker</t>
+  </si>
+  <si>
+    <t>Fulminator</t>
+  </si>
+  <si>
+    <t>Skyscatterer</t>
   </si>
   <si>
     <t>Beastbreaker</t>
@@ -265,16 +265,16 @@
     <t>LMG</t>
   </si>
   <si>
+    <t>Spitter</t>
+  </si>
+  <si>
+    <t>Spewer</t>
+  </si>
+  <si>
     <t>Gouger</t>
   </si>
   <si>
-    <t>Eruptor</t>
-  </si>
-  <si>
-    <t>T3LMG</t>
-  </si>
-  <si>
-    <t>T4LMG</t>
+    <t>Annihilator</t>
   </si>
   <si>
     <t>Godgrinder</t>
@@ -283,16 +283,16 @@
     <t>Explosive</t>
   </si>
   <si>
-    <t>Boomer</t>
-  </si>
-  <si>
-    <t>Earsplitter</t>
-  </si>
-  <si>
-    <t>T3Explosive</t>
-  </si>
-  <si>
-    <t>T4Explosive</t>
+    <t>Splitter</t>
+  </si>
+  <si>
+    <t>Breacher</t>
+  </si>
+  <si>
+    <t>Rupturer</t>
+  </si>
+  <si>
+    <t>Divider</t>
   </si>
   <si>
     <t>Heavencracker</t>
@@ -723,11 +723,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="0.0"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -781,14 +781,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -803,8 +795,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -835,7 +836,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -843,7 +844,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -865,9 +866,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -882,21 +889,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -910,16 +903,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1000,7 +1000,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1012,25 +1078,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1042,91 +1096,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1144,7 +1120,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1156,31 +1168,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1500,13 +1500,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1529,17 +1533,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1548,7 +1548,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1566,40 +1566,40 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1608,88 +1608,88 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="43" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2427,8 +2427,8 @@
   <sheetPr/>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -2539,7 +2539,7 @@
   <dimension ref="A1:AJ75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.7142857142857" defaultRowHeight="15"/>
@@ -7054,8 +7054,8 @@
   <sheetPr/>
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -7293,7 +7293,7 @@
       </c>
       <c r="C4" t="str">
         <f>WeaponData!C7</f>
-        <v>T4Pistol</v>
+        <v>Saltscraper</v>
       </c>
       <c r="D4">
         <f>WeaponData!D7</f>
@@ -7441,7 +7441,7 @@
       </c>
       <c r="C6" t="str">
         <f>WeaponData!C10</f>
-        <v>Snipper</v>
+        <v>Groundrider</v>
       </c>
       <c r="D6">
         <f>WeaponData!D10</f>
@@ -7515,7 +7515,7 @@
       </c>
       <c r="C7" t="str">
         <f>WeaponData!C11</f>
-        <v>Groundrider</v>
+        <v>Longstrider</v>
       </c>
       <c r="D7">
         <f>WeaponData!D11</f>
@@ -7589,7 +7589,7 @@
       </c>
       <c r="C8" t="str">
         <f>WeaponData!C12</f>
-        <v>Longstrider</v>
+        <v>Deepdriver</v>
       </c>
       <c r="D8">
         <f>WeaponData!D12</f>
@@ -7811,7 +7811,7 @@
       </c>
       <c r="C11" t="str">
         <f>WeaponData!C16</f>
-        <v>Banger</v>
+        <v>Leadspreader</v>
       </c>
       <c r="D11">
         <f>WeaponData!D16</f>
@@ -7885,7 +7885,7 @@
       </c>
       <c r="C12" t="str">
         <f>WeaponData!C17</f>
-        <v>Leadspreader</v>
+        <v>Steelsweeper</v>
       </c>
       <c r="D12">
         <f>WeaponData!D17</f>
@@ -7959,7 +7959,7 @@
       </c>
       <c r="C13" t="str">
         <f>WeaponData!C18</f>
-        <v>T3Shotgun</v>
+        <v>Bonebreaker</v>
       </c>
       <c r="D13">
         <f>WeaponData!D18</f>
@@ -8033,7 +8033,7 @@
       </c>
       <c r="C14" t="str">
         <f>WeaponData!C19</f>
-        <v>T4Shotgun</v>
+        <v>Skullcrusher</v>
       </c>
       <c r="D14">
         <f>WeaponData!D19</f>
@@ -8255,7 +8255,7 @@
       </c>
       <c r="C17" t="str">
         <f>WeaponData!C23</f>
-        <v>Saltscraper</v>
+        <v>Gripshaker</v>
       </c>
       <c r="D17">
         <f>WeaponData!D23</f>
@@ -8329,7 +8329,7 @@
       </c>
       <c r="C18" t="str">
         <f>WeaponData!C24</f>
-        <v>T3SMG</v>
+        <v>Fulminator</v>
       </c>
       <c r="D18">
         <f>WeaponData!D24</f>
@@ -8403,7 +8403,7 @@
       </c>
       <c r="C19" t="str">
         <f>WeaponData!C25</f>
-        <v>T4SMG</v>
+        <v>Skyscatterer</v>
       </c>
       <c r="D19">
         <f>WeaponData!D25</f>
@@ -8551,7 +8551,7 @@
       </c>
       <c r="C21" t="str">
         <f>WeaponData!C28</f>
-        <v>Gouger</v>
+        <v>Spitter</v>
       </c>
       <c r="D21">
         <f>WeaponData!D28</f>
@@ -8625,7 +8625,7 @@
       </c>
       <c r="C22" t="str">
         <f>WeaponData!C29</f>
-        <v>Eruptor</v>
+        <v>Spewer</v>
       </c>
       <c r="D22">
         <f>WeaponData!D29</f>
@@ -8699,7 +8699,7 @@
       </c>
       <c r="C23" t="str">
         <f>WeaponData!C30</f>
-        <v>T3LMG</v>
+        <v>Gouger</v>
       </c>
       <c r="D23">
         <f>WeaponData!D30</f>
@@ -8773,7 +8773,7 @@
       </c>
       <c r="C24" t="str">
         <f>WeaponData!C31</f>
-        <v>T4LMG</v>
+        <v>Annihilator</v>
       </c>
       <c r="D24">
         <f>WeaponData!D31</f>
@@ -8921,7 +8921,7 @@
       </c>
       <c r="C26" t="str">
         <f>WeaponData!C34</f>
-        <v>Boomer</v>
+        <v>Splitter</v>
       </c>
       <c r="D26">
         <f>WeaponData!D34</f>
@@ -8995,7 +8995,7 @@
       </c>
       <c r="C27" t="str">
         <f>WeaponData!C35</f>
-        <v>Earsplitter</v>
+        <v>Breacher</v>
       </c>
       <c r="D27">
         <f>WeaponData!D35</f>
@@ -9069,7 +9069,7 @@
       </c>
       <c r="C28" t="str">
         <f>WeaponData!C36</f>
-        <v>T3Explosive</v>
+        <v>Rupturer</v>
       </c>
       <c r="D28">
         <f>WeaponData!D36</f>
@@ -9143,7 +9143,7 @@
       </c>
       <c r="C29" t="str">
         <f>WeaponData!C37</f>
-        <v>T4Explosive</v>
+        <v>Divider</v>
       </c>
       <c r="D29">
         <f>WeaponData!D37</f>

</xml_diff>

<commit_message>
<Feature, Bugfixes> Healing, Powershot, Knockback
Healer now heals enemies (including self).
Heal animation.
Sniper uses powershot.
Sort of put knockback in.
Removed knockdown.
Changed the enemyui to use one ui for the target rather than one ui for
each enemy.
Enemies now selected based on orientation from  player rather than on
distance.
Moved recoilmanager to character combat and updated.
Included blocked cells as well as reachable cells. Now pathfinding won't
include unreachable cells, whilst the block algorithm will only look
return true if the cell is blocked not unreachable.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="813">
   <si>
     <t>Type</t>
   </si>
@@ -2093,24 +2093,39 @@
     <t>Sniper</t>
   </si>
   <si>
+    <t>powershot</t>
+  </si>
+  <si>
     <t>Brawler</t>
   </si>
   <si>
+    <t>knockdown</t>
+  </si>
+  <si>
     <t>Medic</t>
   </si>
   <si>
     <t>SMG, Pistol</t>
   </si>
   <si>
+    <t>heal</t>
+  </si>
+  <si>
     <t>Sentinel</t>
   </si>
   <si>
     <t>SMG, Shotgun, Pistol</t>
   </si>
   <si>
+    <t>gain armour</t>
+  </si>
+  <si>
     <t>LMG, Rifle</t>
   </si>
   <si>
+    <t>summon</t>
+  </si>
+  <si>
     <t>Mountain</t>
   </si>
   <si>
@@ -2120,7 +2135,13 @@
     <t>Martyr</t>
   </si>
   <si>
+    <t>explode</t>
+  </si>
+  <si>
     <t>Witch</t>
+  </si>
+  <si>
+    <t>grenade</t>
   </si>
   <si>
     <t>Grazer</t>
@@ -2457,11 +2478,11 @@
   <numFmts count="7">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="0.0"/>
-    <numFmt numFmtId="177" formatCode="0.0_ "/>
-    <numFmt numFmtId="178" formatCode="0.00_ "/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0.0_ "/>
+    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="178" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -2531,6 +2552,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -2539,15 +2568,36 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2561,9 +2611,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2577,9 +2659,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2594,82 +2690,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2798,13 +2819,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2816,55 +2927,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2882,49 +2945,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2936,13 +2981,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2954,31 +2999,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3523,15 +3544,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -3556,41 +3568,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3610,6 +3592,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -3618,12 +3624,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3641,130 +3662,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="48" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="47" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="52" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="49" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="51" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="41" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="51" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="44" borderId="53" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="44" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="52" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="53" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3832,7 +3853,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3895,7 +3916,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4093,7 +4114,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="12" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
@@ -16402,10 +16423,10 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -16419,6 +16440,7 @@
     <col min="8" max="8" width="8.28571428571429" customWidth="1"/>
     <col min="9" max="9" width="11.4285714285714" customWidth="1"/>
     <col min="10" max="10" width="8.28571428571429" customWidth="1"/>
+    <col min="12" max="12" width="11.8571428571429" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -16469,7 +16491,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>686</v>
       </c>
@@ -16505,10 +16527,13 @@
         <f t="shared" ref="J3:J10" si="1">C3/110</f>
         <v>6.36363636363636</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="L3" s="39" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B4">
         <v>100</v>
@@ -16539,10 +16564,13 @@
         <f t="shared" si="1"/>
         <v>5.45454545454545</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="L4" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="B5">
         <v>200</v>
@@ -16558,7 +16586,7 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="G5" s="42">
         <f t="shared" si="3"/>
@@ -16576,10 +16604,13 @@
         <f t="shared" si="1"/>
         <v>6.36363636363636</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="L5" s="39" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="B6">
         <v>200</v>
@@ -16595,7 +16626,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="G6" s="42">
         <f t="shared" si="3"/>
@@ -16613,8 +16644,11 @@
         <f t="shared" si="1"/>
         <v>6.36363636363636</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="L6" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>399</v>
       </c>
@@ -16632,7 +16666,7 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>692</v>
+        <v>696</v>
       </c>
       <c r="G7" s="42">
         <f t="shared" si="3"/>
@@ -16650,10 +16684,13 @@
         <f t="shared" si="1"/>
         <v>8.18181818181818</v>
       </c>
+      <c r="L7" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
-        <v>693</v>
+        <v>698</v>
       </c>
       <c r="B8">
         <v>600</v>
@@ -16669,7 +16706,7 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>694</v>
+        <v>699</v>
       </c>
       <c r="G8" s="42">
         <f t="shared" si="3"/>
@@ -16688,9 +16725,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
-        <v>695</v>
+        <v>700</v>
       </c>
       <c r="B9">
         <v>50</v>
@@ -16721,10 +16758,13 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="L9" s="39" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
-        <v>696</v>
+        <v>702</v>
       </c>
       <c r="B10">
         <v>150</v>
@@ -16740,7 +16780,7 @@
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="G10" s="42">
         <f t="shared" si="3"/>
@@ -16757,6 +16797,9 @@
       <c r="J10" s="42">
         <f t="shared" si="1"/>
         <v>5.90909090909091</v>
+      </c>
+      <c r="L10" s="39" t="s">
+        <v>703</v>
       </c>
     </row>
     <row r="11" spans="7:10">
@@ -16767,7 +16810,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
-        <v>697</v>
+        <v>704</v>
       </c>
       <c r="B12">
         <v>150</v>
@@ -16798,7 +16841,7 @@
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>698</v>
+        <v>705</v>
       </c>
       <c r="B13">
         <v>50</v>
@@ -16891,7 +16934,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
-        <v>699</v>
+        <v>706</v>
       </c>
       <c r="B16">
         <v>200</v>
@@ -16928,7 +16971,7 @@
     </row>
     <row r="18" spans="1:10">
       <c r="A18" t="s">
-        <v>700</v>
+        <v>707</v>
       </c>
       <c r="B18">
         <v>200</v>
@@ -16956,7 +16999,7 @@
     </row>
     <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>701</v>
+        <v>708</v>
       </c>
       <c r="B19">
         <v>50</v>
@@ -16984,7 +17027,7 @@
     </row>
     <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>702</v>
+        <v>709</v>
       </c>
       <c r="B20">
         <v>400</v>
@@ -17012,7 +17055,7 @@
     </row>
     <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>703</v>
+        <v>710</v>
       </c>
       <c r="B21">
         <v>100</v>
@@ -17040,7 +17083,7 @@
     </row>
     <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>704</v>
+        <v>711</v>
       </c>
       <c r="B22">
         <v>300</v>
@@ -17068,7 +17111,7 @@
     </row>
     <row r="23" spans="1:10">
       <c r="A23" t="s">
-        <v>705</v>
+        <v>712</v>
       </c>
       <c r="B23">
         <v>100</v>
@@ -17096,7 +17139,7 @@
     </row>
     <row r="24" spans="1:10">
       <c r="A24" t="s">
-        <v>706</v>
+        <v>713</v>
       </c>
       <c r="B24">
         <v>1000</v>
@@ -17154,241 +17197,241 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="30" t="s">
-        <v>707</v>
+        <v>714</v>
       </c>
       <c r="B1" s="31" t="s">
-        <v>708</v>
+        <v>715</v>
       </c>
       <c r="C1" s="31"/>
       <c r="D1" s="31" t="s">
-        <v>709</v>
+        <v>716</v>
       </c>
       <c r="E1" s="31"/>
       <c r="F1" s="31" t="s">
-        <v>710</v>
+        <v>717</v>
       </c>
       <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="30"/>
       <c r="B2" s="30" t="s">
-        <v>711</v>
+        <v>718</v>
       </c>
       <c r="C2" s="30" t="s">
-        <v>712</v>
+        <v>719</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>711</v>
+        <v>718</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>712</v>
+        <v>719</v>
       </c>
       <c r="F2" s="30" t="s">
-        <v>711</v>
+        <v>718</v>
       </c>
       <c r="G2" s="30" t="s">
-        <v>712</v>
+        <v>719</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="32" t="s">
-        <v>713</v>
+        <v>720</v>
       </c>
       <c r="B3" s="33" t="s">
-        <v>714</v>
+        <v>721</v>
       </c>
       <c r="C3" s="34"/>
       <c r="D3" s="33" t="s">
-        <v>715</v>
+        <v>722</v>
       </c>
       <c r="E3" s="34" t="s">
-        <v>716</v>
+        <v>723</v>
       </c>
       <c r="F3" s="33" t="s">
-        <v>717</v>
+        <v>724</v>
       </c>
       <c r="G3" s="34" t="s">
-        <v>718</v>
+        <v>725</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="32" t="s">
-        <v>719</v>
+        <v>726</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>720</v>
+        <v>727</v>
       </c>
       <c r="C4" s="34"/>
       <c r="D4" s="33" t="s">
-        <v>721</v>
+        <v>728</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>722</v>
+        <v>729</v>
       </c>
       <c r="F4" s="33" t="s">
-        <v>723</v>
+        <v>730</v>
       </c>
       <c r="G4" s="34" t="s">
-        <v>724</v>
+        <v>731</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="32" t="s">
-        <v>725</v>
+        <v>732</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>726</v>
+        <v>733</v>
       </c>
       <c r="C5" s="34"/>
       <c r="D5" s="33" t="s">
-        <v>727</v>
+        <v>734</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>728</v>
+        <v>735</v>
       </c>
       <c r="F5" s="33" t="s">
-        <v>729</v>
+        <v>736</v>
       </c>
       <c r="G5" s="34" t="s">
-        <v>730</v>
+        <v>737</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="32" t="s">
-        <v>731</v>
+        <v>738</v>
       </c>
       <c r="B6" s="33" t="s">
-        <v>732</v>
+        <v>739</v>
       </c>
       <c r="C6" s="34"/>
       <c r="D6" s="33" t="s">
-        <v>733</v>
+        <v>740</v>
       </c>
       <c r="E6" s="34"/>
       <c r="F6" s="33" t="s">
-        <v>734</v>
+        <v>741</v>
       </c>
       <c r="G6" s="34" t="s">
-        <v>735</v>
+        <v>742</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="32" t="s">
-        <v>736</v>
+        <v>743</v>
       </c>
       <c r="B7" s="33" t="s">
-        <v>737</v>
+        <v>744</v>
       </c>
       <c r="C7" s="34"/>
       <c r="D7" s="33" t="s">
-        <v>738</v>
+        <v>745</v>
       </c>
       <c r="E7" s="34"/>
       <c r="F7" s="33" t="s">
-        <v>739</v>
+        <v>746</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>740</v>
+        <v>747</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="32" t="s">
-        <v>741</v>
+        <v>748</v>
       </c>
       <c r="B8" s="33" t="s">
-        <v>742</v>
+        <v>749</v>
       </c>
       <c r="C8" s="34"/>
       <c r="D8" s="33"/>
       <c r="E8" s="34"/>
       <c r="F8" s="33" t="s">
-        <v>743</v>
+        <v>750</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>717</v>
+        <v>724</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="32" t="s">
-        <v>744</v>
+        <v>751</v>
       </c>
       <c r="B9" s="33" t="s">
-        <v>745</v>
+        <v>752</v>
       </c>
       <c r="C9" s="34"/>
       <c r="D9" s="33"/>
       <c r="E9" s="34"/>
       <c r="F9" s="33" t="s">
-        <v>746</v>
+        <v>753</v>
       </c>
       <c r="G9" s="34"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="32" t="s">
-        <v>747</v>
+        <v>754</v>
       </c>
       <c r="B10" s="33" t="s">
-        <v>748</v>
+        <v>755</v>
       </c>
       <c r="C10" s="34"/>
       <c r="D10" s="33"/>
       <c r="E10" s="34"/>
       <c r="F10" s="33" t="s">
-        <v>749</v>
+        <v>756</v>
       </c>
       <c r="G10" s="34"/>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="32" t="s">
-        <v>750</v>
+        <v>757</v>
       </c>
       <c r="B11" s="33" t="s">
-        <v>751</v>
+        <v>758</v>
       </c>
       <c r="C11" s="34"/>
       <c r="D11" s="33"/>
       <c r="E11" s="34"/>
       <c r="F11" s="33" t="s">
-        <v>752</v>
+        <v>759</v>
       </c>
       <c r="G11" s="34"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="32" t="s">
-        <v>753</v>
+        <v>760</v>
       </c>
       <c r="B12" s="33"/>
       <c r="C12" s="34"/>
       <c r="D12" s="33"/>
       <c r="E12" s="34"/>
       <c r="F12" s="33" t="s">
-        <v>754</v>
+        <v>761</v>
       </c>
       <c r="G12" s="34"/>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" s="32" t="s">
-        <v>755</v>
+        <v>762</v>
       </c>
       <c r="B13" s="33"/>
       <c r="C13" s="34"/>
       <c r="D13" s="33"/>
       <c r="E13" s="34"/>
       <c r="F13" s="33" t="s">
-        <v>756</v>
+        <v>763</v>
       </c>
       <c r="G13" s="34"/>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="32" t="s">
-        <v>757</v>
+        <v>764</v>
       </c>
       <c r="B14" s="33"/>
       <c r="C14" s="34"/>
       <c r="D14" s="33"/>
       <c r="E14" s="34"/>
       <c r="F14" s="33" t="s">
-        <v>740</v>
+        <v>747</v>
       </c>
       <c r="G14" s="34"/>
     </row>
@@ -17399,7 +17442,7 @@
       <c r="D15" s="33"/>
       <c r="E15" s="34"/>
       <c r="F15" s="33" t="s">
-        <v>758</v>
+        <v>765</v>
       </c>
       <c r="G15" s="34"/>
     </row>
@@ -17410,7 +17453,7 @@
       <c r="D16" s="33"/>
       <c r="E16" s="34"/>
       <c r="F16" s="33" t="s">
-        <v>759</v>
+        <v>766</v>
       </c>
       <c r="G16" s="34"/>
     </row>
@@ -17421,7 +17464,7 @@
       <c r="D17" s="33"/>
       <c r="E17" s="34"/>
       <c r="F17" s="33" t="s">
-        <v>735</v>
+        <v>742</v>
       </c>
       <c r="G17" s="34"/>
     </row>
@@ -17544,16 +17587,16 @@
         <v>10</v>
       </c>
       <c r="J1" s="29" t="s">
-        <v>760</v>
+        <v>767</v>
       </c>
       <c r="K1" s="29" t="s">
         <v>578</v>
       </c>
       <c r="L1" s="29" t="s">
-        <v>761</v>
+        <v>768</v>
       </c>
       <c r="M1" s="29" t="s">
-        <v>762</v>
+        <v>769</v>
       </c>
       <c r="N1" s="23" t="s">
         <v>173</v>
@@ -17570,7 +17613,7 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="25" t="s">
-        <v>763</v>
+        <v>770</v>
       </c>
       <c r="B2" s="26">
         <v>1.2</v>
@@ -17595,7 +17638,7 @@
     </row>
     <row r="3" spans="1:17">
       <c r="A3" s="25" t="s">
-        <v>764</v>
+        <v>771</v>
       </c>
       <c r="B3" s="26"/>
       <c r="C3" s="26"/>
@@ -17620,7 +17663,7 @@
     </row>
     <row r="4" spans="1:17">
       <c r="A4" s="25" t="s">
-        <v>765</v>
+        <v>772</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="26">
@@ -17670,7 +17713,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6" s="25" t="s">
-        <v>766</v>
+        <v>773</v>
       </c>
       <c r="B6" s="26"/>
       <c r="C6" s="26"/>
@@ -17695,7 +17738,7 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7" s="25" t="s">
-        <v>767</v>
+        <v>774</v>
       </c>
       <c r="B7" s="26"/>
       <c r="C7" s="26"/>
@@ -17745,7 +17788,7 @@
     </row>
     <row r="9" spans="1:17">
       <c r="A9" s="25" t="s">
-        <v>768</v>
+        <v>775</v>
       </c>
       <c r="B9" s="26"/>
       <c r="C9" s="26">
@@ -17770,7 +17813,7 @@
     </row>
     <row r="10" spans="1:17">
       <c r="A10" s="27" t="s">
-        <v>769</v>
+        <v>776</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -17795,7 +17838,7 @@
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="28" t="s">
-        <v>770</v>
+        <v>777</v>
       </c>
       <c r="B11" s="26">
         <v>1.5</v>
@@ -17845,7 +17888,7 @@
     </row>
     <row r="13" spans="1:17">
       <c r="A13" s="25" t="s">
-        <v>771</v>
+        <v>778</v>
       </c>
       <c r="B13" s="26">
         <v>2</v>
@@ -17870,7 +17913,7 @@
     </row>
     <row r="14" spans="1:17">
       <c r="A14" s="25" t="s">
-        <v>772</v>
+        <v>779</v>
       </c>
       <c r="B14" s="26">
         <v>0.1</v>
@@ -17895,7 +17938,7 @@
     </row>
     <row r="15" spans="1:17">
       <c r="A15" s="27" t="s">
-        <v>773</v>
+        <v>780</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="26"/>
@@ -17920,7 +17963,7 @@
     </row>
     <row r="16" spans="1:17">
       <c r="A16" s="27" t="s">
-        <v>774</v>
+        <v>781</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="26"/>
@@ -17943,7 +17986,7 @@
     </row>
     <row r="17" spans="1:17">
       <c r="A17" s="27" t="s">
-        <v>775</v>
+        <v>782</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="26"/>
@@ -17968,7 +18011,7 @@
     </row>
     <row r="18" spans="1:17">
       <c r="A18" s="27" t="s">
-        <v>776</v>
+        <v>783</v>
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="26"/>
@@ -17991,7 +18034,7 @@
     </row>
     <row r="19" spans="1:17">
       <c r="A19" s="27" t="s">
-        <v>777</v>
+        <v>784</v>
       </c>
       <c r="B19" s="26"/>
       <c r="C19" s="26"/>
@@ -18016,7 +18059,7 @@
     </row>
     <row r="20" spans="1:17">
       <c r="A20" s="27" t="s">
-        <v>778</v>
+        <v>785</v>
       </c>
       <c r="B20" s="26"/>
       <c r="C20" s="26"/>
@@ -18039,7 +18082,7 @@
     </row>
     <row r="21" spans="1:17">
       <c r="A21" s="27" t="s">
-        <v>779</v>
+        <v>786</v>
       </c>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
@@ -18064,7 +18107,7 @@
     </row>
     <row r="22" spans="1:17">
       <c r="A22" s="27" t="s">
-        <v>780</v>
+        <v>787</v>
       </c>
       <c r="B22" s="26"/>
       <c r="C22" s="26"/>
@@ -18087,7 +18130,7 @@
     </row>
     <row r="23" spans="1:17">
       <c r="A23" s="27" t="s">
-        <v>781</v>
+        <v>788</v>
       </c>
       <c r="B23" s="26"/>
       <c r="C23" s="26"/>
@@ -18110,7 +18153,7 @@
     </row>
     <row r="24" spans="1:17">
       <c r="A24" s="27" t="s">
-        <v>782</v>
+        <v>789</v>
       </c>
       <c r="B24" s="26"/>
       <c r="C24" s="26"/>
@@ -18133,7 +18176,7 @@
     </row>
     <row r="25" spans="1:17">
       <c r="A25" s="27" t="s">
-        <v>783</v>
+        <v>790</v>
       </c>
       <c r="B25" s="26"/>
       <c r="C25" s="26"/>
@@ -18156,7 +18199,7 @@
     </row>
     <row r="26" spans="1:17">
       <c r="A26" s="27" t="s">
-        <v>784</v>
+        <v>791</v>
       </c>
       <c r="B26" s="26"/>
       <c r="C26" s="26"/>
@@ -18394,23 +18437,23 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>785</v>
+        <v>792</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>786</v>
+        <v>793</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
       <c r="E1" s="22" t="s">
-        <v>787</v>
+        <v>794</v>
       </c>
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
       <c r="I1" t="s">
-        <v>788</v>
+        <v>795</v>
       </c>
       <c r="L1" t="s">
-        <v>789</v>
+        <v>796</v>
       </c>
     </row>
     <row r="2" spans="2:12">
@@ -18418,7 +18461,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>790</v>
+        <v>797</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -18427,7 +18470,7 @@
         <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>790</v>
+        <v>797</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
@@ -18567,7 +18610,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>791</v>
+        <v>798</v>
       </c>
       <c r="B8">
         <f>B3*0.5+B3</f>
@@ -18648,22 +18691,22 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>792</v>
+        <v>799</v>
       </c>
       <c r="B14" t="s">
-        <v>793</v>
+        <v>800</v>
       </c>
       <c r="C14" t="s">
-        <v>789</v>
+        <v>796</v>
       </c>
       <c r="D14" t="s">
-        <v>794</v>
+        <v>801</v>
       </c>
       <c r="E14" t="s">
-        <v>795</v>
+        <v>802</v>
       </c>
       <c r="F14" t="s">
-        <v>796</v>
+        <v>803</v>
       </c>
       <c r="L14">
         <v>9</v>
@@ -18833,13 +18876,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>797</v>
+        <v>804</v>
       </c>
       <c r="B1" t="s">
-        <v>798</v>
+        <v>805</v>
       </c>
       <c r="C1" t="s">
-        <v>799</v>
+        <v>806</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -19180,7 +19223,7 @@
     </row>
     <row r="30" spans="4:5">
       <c r="D30" t="s">
-        <v>800</v>
+        <v>807</v>
       </c>
       <c r="E30">
         <v>0.75</v>
@@ -19188,7 +19231,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
-        <v>801</v>
+        <v>808</v>
       </c>
       <c r="B32" s="2">
         <v>10</v>
@@ -19213,13 +19256,13 @@
         <v>68</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>802</v>
+        <v>809</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>803</v>
+        <v>810</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>804</v>
+        <v>811</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>3</v>
@@ -19246,7 +19289,7 @@
         <v>13</v>
       </c>
       <c r="O33" s="5" t="s">
-        <v>805</v>
+        <v>812</v>
       </c>
       <c r="P33" s="7" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
<Feature> Conditions, Aim, Brawler, Skills
Implemented most character and weapon skills.
Reimplemented conditions.
Added brawler enemy type with dash attack.
Added laser-sight style aimer for player.
Made bullets easier to see, enemy bullets are red.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13200" firstSheet="6" activeTab="9"/>
+    <workbookView windowWidth="28695" windowHeight="13200" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -1985,13 +1985,13 @@
     <t>Staunch</t>
   </si>
   <si>
-    <t>Recover 50 health.</t>
+    <t>Remove all conditions</t>
   </si>
   <si>
     <t>Rejuvinate</t>
   </si>
   <si>
-    <t>Transfer conditions to target.</t>
+    <t>Restore 50 health</t>
   </si>
   <si>
     <t>Immolate</t>
@@ -2057,7 +2057,7 @@
     <t>Restock</t>
   </si>
   <si>
-    <t>Recover additional magazine</t>
+    <t>..............</t>
   </si>
   <si>
     <t>Fortify</t>
@@ -2484,10 +2484,10 @@
   <numFmts count="7">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="0.0_ "/>
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0.0_ "/>
     <numFmt numFmtId="178" formatCode="0.0"/>
   </numFmts>
   <fonts count="27">
@@ -2564,8 +2564,16 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2581,14 +2589,22 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2604,14 +2620,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2625,25 +2634,38 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2656,38 +2678,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2816,25 +2816,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2846,145 +2918,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2997,6 +2937,66 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3539,36 +3539,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -3589,15 +3563,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -3609,6 +3574,50 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3627,21 +3636,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3659,130 +3659,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="47" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="51" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="48" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="50" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="38" borderId="53" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="52" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="51" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="50" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="45" borderId="46" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="52" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="46" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="53" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3829,13 +3829,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3850,7 +3850,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -14681,7 +14681,7 @@
   <sheetPr/>
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -16269,8 +16269,8 @@
   <sheetPr/>
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -32647,7 +32647,6 @@
       <c r="F12" s="12" t="s">
         <v>432</v>
       </c>
-      <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
         <v>433</v>
       </c>
@@ -32671,7 +32670,6 @@
       <c r="F13" s="12" t="s">
         <v>438</v>
       </c>
-      <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
         <v>439</v>
       </c>
@@ -32689,11 +32687,9 @@
       <c r="D14" s="12" t="s">
         <v>443</v>
       </c>
-      <c r="E14" s="2"/>
       <c r="F14" s="12" t="s">
         <v>444</v>
       </c>
-      <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
         <v>445</v>
       </c>
@@ -32711,11 +32707,9 @@
       <c r="D15" s="12" t="s">
         <v>449</v>
       </c>
-      <c r="E15" s="2"/>
       <c r="F15" s="12" t="s">
         <v>450</v>
       </c>
-      <c r="G15" s="2"/>
       <c r="H15" s="2" t="s">
         <v>451</v>
       </c>
@@ -32727,13 +32721,10 @@
       <c r="B16" s="12" t="s">
         <v>453</v>
       </c>
-      <c r="C16" s="2"/>
       <c r="D16" s="12" t="s">
         <v>454</v>
       </c>
-      <c r="E16" s="2"/>
       <c r="F16" s="12"/>
-      <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
         <v>455</v>
       </c>
@@ -32745,13 +32736,10 @@
       <c r="B17" s="12" t="s">
         <v>457</v>
       </c>
-      <c r="C17" s="2"/>
       <c r="D17" s="12" t="s">
         <v>458</v>
       </c>
-      <c r="E17" s="2"/>
       <c r="F17" s="12"/>
-      <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
         <v>459</v>
       </c>
@@ -32763,13 +32751,10 @@
       <c r="B18" s="12" t="s">
         <v>461</v>
       </c>
-      <c r="C18" s="2"/>
       <c r="D18" s="12" t="s">
         <v>462</v>
       </c>
-      <c r="E18" s="2"/>
       <c r="F18" s="12"/>
-      <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
         <v>463</v>
       </c>
@@ -32781,11 +32766,9 @@
       <c r="B19" s="12" t="s">
         <v>387</v>
       </c>
-      <c r="C19" s="2"/>
       <c r="D19" s="12" t="s">
         <v>465</v>
       </c>
-      <c r="E19" s="2"/>
       <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6">
@@ -32795,11 +32778,9 @@
       <c r="B20" s="12" t="s">
         <v>394</v>
       </c>
-      <c r="C20" s="2"/>
       <c r="D20" s="12" t="s">
         <v>467</v>
       </c>
-      <c r="E20" s="2"/>
       <c r="F20" s="12"/>
     </row>
     <row r="21" spans="1:6">
@@ -32809,11 +32790,9 @@
       <c r="B21" s="12" t="s">
         <v>469</v>
       </c>
-      <c r="C21" s="2"/>
       <c r="D21" s="12" t="s">
         <v>384</v>
       </c>
-      <c r="E21" s="2"/>
       <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:6">
@@ -32823,11 +32802,9 @@
       <c r="B22" s="12" t="s">
         <v>470</v>
       </c>
-      <c r="C22" s="2"/>
       <c r="D22" s="12" t="s">
         <v>471</v>
       </c>
-      <c r="E22" s="2"/>
       <c r="F22" s="12"/>
     </row>
     <row r="23" spans="1:6">
@@ -32837,11 +32814,9 @@
       <c r="B23" s="12" t="s">
         <v>473</v>
       </c>
-      <c r="C23" s="2"/>
       <c r="D23" s="12" t="s">
         <v>474</v>
       </c>
-      <c r="E23" s="2"/>
       <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:6">
@@ -32851,11 +32826,9 @@
       <c r="B24" s="12" t="s">
         <v>476</v>
       </c>
-      <c r="C24" s="2"/>
       <c r="D24" s="12" t="s">
         <v>477</v>
       </c>
-      <c r="E24" s="2"/>
       <c r="F24" s="12"/>
     </row>
     <row r="25" spans="1:6">
@@ -32865,11 +32838,9 @@
       <c r="B25" s="12" t="s">
         <v>479</v>
       </c>
-      <c r="C25" s="2"/>
       <c r="D25" s="12" t="s">
         <v>480</v>
       </c>
-      <c r="E25" s="2"/>
       <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:6">
@@ -32879,11 +32850,9 @@
       <c r="B26" s="12" t="s">
         <v>482</v>
       </c>
-      <c r="C26" s="2"/>
       <c r="D26" s="12" t="s">
         <v>483</v>
       </c>
-      <c r="E26" s="2"/>
       <c r="F26" s="12"/>
     </row>
     <row r="27" spans="1:6">
@@ -32893,11 +32862,9 @@
       <c r="B27" s="12" t="s">
         <v>485</v>
       </c>
-      <c r="C27" s="2"/>
       <c r="D27" s="12" t="s">
         <v>486</v>
       </c>
-      <c r="E27" s="2"/>
       <c r="F27" s="12"/>
     </row>
     <row r="28" spans="1:6">
@@ -32907,9 +32874,7 @@
       <c r="B28" s="12" t="s">
         <v>488</v>
       </c>
-      <c r="C28" s="2"/>
       <c r="D28" s="12"/>
-      <c r="E28" s="2"/>
       <c r="F28" s="12"/>
     </row>
     <row r="29" spans="1:6">
@@ -32919,9 +32884,7 @@
       <c r="B29" s="12" t="s">
         <v>385</v>
       </c>
-      <c r="C29" s="2"/>
       <c r="D29" s="12"/>
-      <c r="E29" s="2"/>
       <c r="F29" s="12"/>
     </row>
     <row r="30" spans="1:6">
@@ -32931,9 +32894,7 @@
       <c r="B30" s="12" t="s">
         <v>446</v>
       </c>
-      <c r="C30" s="2"/>
       <c r="D30" s="12"/>
-      <c r="E30" s="2"/>
       <c r="F30" s="12"/>
     </row>
     <row r="31" spans="1:6">
@@ -32943,9 +32904,7 @@
       <c r="B31" s="12" t="s">
         <v>492</v>
       </c>
-      <c r="C31" s="2"/>
       <c r="D31" s="12"/>
-      <c r="E31" s="2"/>
       <c r="F31" s="12"/>
     </row>
     <row r="32" spans="1:6">
@@ -32955,9 +32914,7 @@
       <c r="B32" s="12" t="s">
         <v>494</v>
       </c>
-      <c r="C32" s="2"/>
       <c r="D32" s="12"/>
-      <c r="E32" s="2"/>
       <c r="F32" s="12"/>
     </row>
     <row r="33" spans="1:6">
@@ -32967,9 +32924,7 @@
       <c r="B33" s="12" t="s">
         <v>456</v>
       </c>
-      <c r="C33" s="2"/>
       <c r="D33" s="12"/>
-      <c r="E33" s="2"/>
       <c r="F33" s="12"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
<Feature> Maelstrom, Enemy Icons
Added Maelstrom enemy type.
Maelstrom splits into 1-health clones when it receives enough damage.
Maelstrom attacks players with high damage shot.
Created icons for Maelstrom, Ghoul, and Ghoul Mother.
Fixed issue where barriers could overlap.
Changed exit combat condition to all enemies dead, not just enemies on
screen.
Changed player input- much easier to use now.
Removed sprinting.
Added second, larger, collider to enemies to increase the radius at
which their UI will display.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -2177,10 +2177,10 @@
     <t>GhoulMother</t>
   </si>
   <si>
+    <t>Maelstrom</t>
+  </si>
+  <si>
     <t>Ghast</t>
-  </si>
-  <si>
-    <t>Maelstrom</t>
   </si>
   <si>
     <t>Shocker</t>
@@ -2482,13 +2482,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0.0_ "/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="0.0"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -2550,7 +2550,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2565,10 +2587,47 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2582,23 +2641,31 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2612,29 +2679,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -2643,51 +2687,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2816,7 +2816,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2828,13 +2840,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2846,13 +2918,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2864,25 +2954,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2894,91 +2966,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2991,6 +2979,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3541,9 +3541,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3568,17 +3570,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3613,15 +3604,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3636,12 +3618,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3659,130 +3659,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="48" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="48" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="51" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="50" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="52" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="39" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="26" borderId="53" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="52" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="49" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="38" borderId="51" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="53" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -16728,7 +16728,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -16814,19 +16814,19 @@
         <v>28</v>
       </c>
       <c r="G3" s="35">
-        <f>B3/25</f>
+        <f t="shared" ref="G3:G22" si="0">B3/25</f>
         <v>8</v>
       </c>
       <c r="H3" s="35">
-        <f t="shared" ref="H3:H10" si="0">C3/25</f>
+        <f t="shared" ref="H3:H22" si="1">C3/25</f>
         <v>28</v>
       </c>
       <c r="I3" s="35">
-        <f>B3/110</f>
+        <f t="shared" ref="I3:I22" si="2">B3/110</f>
         <v>1.81818181818182</v>
       </c>
       <c r="J3" s="35">
-        <f t="shared" ref="J3:J10" si="1">C3/110</f>
+        <f t="shared" ref="J3:J22" si="3">C3/110</f>
         <v>6.36363636363636</v>
       </c>
       <c r="L3" s="32" t="s">
@@ -16841,7 +16841,7 @@
         <v>100</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C10" si="2">B4+500</f>
+        <f t="shared" ref="C4:C22" si="4">B4+500</f>
         <v>600</v>
       </c>
       <c r="D4">
@@ -16851,19 +16851,19 @@
         <v>2</v>
       </c>
       <c r="G4" s="35">
-        <f>B4/25</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H4" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="I4" s="35">
-        <f>B4/110</f>
+        <f t="shared" si="2"/>
         <v>0.909090909090909</v>
       </c>
       <c r="J4" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.45454545454545</v>
       </c>
       <c r="L4" t="s">
@@ -16878,7 +16878,7 @@
         <v>200</v>
       </c>
       <c r="C5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>700</v>
       </c>
       <c r="D5">
@@ -16891,19 +16891,19 @@
         <v>699</v>
       </c>
       <c r="G5" s="35">
-        <f>B5/25</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H5" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="I5" s="35">
-        <f>B5/110</f>
+        <f t="shared" si="2"/>
         <v>1.81818181818182</v>
       </c>
       <c r="J5" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.36363636363636</v>
       </c>
       <c r="L5" s="32" t="s">
@@ -16918,7 +16918,7 @@
         <v>200</v>
       </c>
       <c r="C6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>700</v>
       </c>
       <c r="D6">
@@ -16931,19 +16931,19 @@
         <v>702</v>
       </c>
       <c r="G6" s="35">
-        <f>B6/25</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H6" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="I6" s="35">
-        <f>B6/110</f>
+        <f t="shared" si="2"/>
         <v>1.81818181818182</v>
       </c>
       <c r="J6" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.36363636363636</v>
       </c>
       <c r="L6" t="s">
@@ -16958,7 +16958,7 @@
         <v>400</v>
       </c>
       <c r="C7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
       <c r="D7">
@@ -16971,19 +16971,19 @@
         <v>705</v>
       </c>
       <c r="G7" s="35">
-        <f>B7/25</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="H7" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="I7" s="35">
-        <f>B7/110</f>
+        <f t="shared" si="2"/>
         <v>3.63636363636364</v>
       </c>
       <c r="J7" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>8.18181818181818</v>
       </c>
       <c r="L7" t="s">
@@ -16998,7 +16998,7 @@
         <v>600</v>
       </c>
       <c r="C8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>1100</v>
       </c>
       <c r="D8">
@@ -17011,19 +17011,19 @@
         <v>708</v>
       </c>
       <c r="G8" s="35">
-        <f>B8/25</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="H8" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
       <c r="I8" s="35">
-        <f>B8/110</f>
+        <f t="shared" si="2"/>
         <v>5.45454545454545</v>
       </c>
       <c r="J8" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
     </row>
@@ -17035,7 +17035,7 @@
         <v>50</v>
       </c>
       <c r="C9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>550</v>
       </c>
       <c r="D9">
@@ -17045,19 +17045,19 @@
         <v>1</v>
       </c>
       <c r="G9" s="35">
-        <f>B9/25</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H9" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="I9" s="35">
-        <f>B9/110</f>
+        <f t="shared" si="2"/>
         <v>0.454545454545455</v>
       </c>
       <c r="J9" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="L9" s="32" t="s">
@@ -17072,7 +17072,7 @@
         <v>150</v>
       </c>
       <c r="C10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>650</v>
       </c>
       <c r="D10">
@@ -17085,19 +17085,19 @@
         <v>699</v>
       </c>
       <c r="G10" s="35">
-        <f>B10/25</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H10" s="35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="I10" s="35">
-        <f>B10/110</f>
+        <f t="shared" si="2"/>
         <v>1.36363636363636</v>
       </c>
       <c r="J10" s="35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.90909090909091</v>
       </c>
       <c r="L10" s="32" t="s">
@@ -17112,7 +17112,7 @@
         <v>50</v>
       </c>
       <c r="C11" s="36">
-        <f>B11+500</f>
+        <f t="shared" si="4"/>
         <v>550</v>
       </c>
       <c r="D11" s="36">
@@ -17123,19 +17123,19 @@
       </c>
       <c r="F11" s="36"/>
       <c r="G11" s="37">
-        <f>B11/25</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H11" s="37">
-        <f>C11/25</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="I11" s="37">
-        <f>B11/110</f>
+        <f t="shared" si="2"/>
         <v>0.454545454545455</v>
       </c>
       <c r="J11" s="37">
-        <f>C11/110</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -17147,7 +17147,7 @@
         <v>400</v>
       </c>
       <c r="C12" s="36">
-        <f>B12+500</f>
+        <f t="shared" si="4"/>
         <v>900</v>
       </c>
       <c r="D12" s="36">
@@ -17158,19 +17158,19 @@
       </c>
       <c r="F12" s="36"/>
       <c r="G12" s="37">
-        <f>B12/25</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="H12" s="37">
-        <f>C12/25</f>
+        <f t="shared" si="1"/>
         <v>36</v>
       </c>
       <c r="I12" s="37">
-        <f>B12/110</f>
+        <f t="shared" si="2"/>
         <v>3.63636363636364</v>
       </c>
       <c r="J12" s="37">
-        <f>C12/110</f>
+        <f t="shared" si="3"/>
         <v>8.18181818181818</v>
       </c>
     </row>
@@ -17179,30 +17179,34 @@
         <v>715</v>
       </c>
       <c r="B13" s="36">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="C13" s="36">
         <f>B13+500</f>
-        <v>600</v>
-      </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
+        <v>800</v>
+      </c>
+      <c r="D13" s="36">
+        <v>5</v>
+      </c>
+      <c r="E13" s="36">
+        <v>2</v>
+      </c>
       <c r="F13" s="36"/>
       <c r="G13" s="37">
         <f>B13/25</f>
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="H13" s="37">
         <f>C13/25</f>
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="I13" s="37">
         <f>B13/110</f>
-        <v>0.909090909090909</v>
+        <v>2.72727272727273</v>
       </c>
       <c r="J13" s="37">
         <f>C13/110</f>
-        <v>5.45454545454545</v>
+        <v>7.27272727272727</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -17210,30 +17214,30 @@
         <v>716</v>
       </c>
       <c r="B14" s="36">
-        <v>300</v>
+        <v>100</v>
       </c>
       <c r="C14" s="36">
         <f>B14+500</f>
-        <v>800</v>
+        <v>600</v>
       </c>
       <c r="D14" s="36"/>
       <c r="E14" s="36"/>
       <c r="F14" s="36"/>
       <c r="G14" s="37">
         <f>B14/25</f>
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H14" s="37">
         <f>C14/25</f>
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="I14" s="37">
         <f>B14/110</f>
-        <v>2.72727272727273</v>
+        <v>0.909090909090909</v>
       </c>
       <c r="J14" s="37">
         <f>C14/110</f>
-        <v>7.27272727272727</v>
+        <v>5.45454545454545</v>
       </c>
     </row>
     <row r="15" spans="1:10">
@@ -17244,26 +17248,26 @@
         <v>100</v>
       </c>
       <c r="C15" s="36">
-        <f>B15+500</f>
+        <f t="shared" si="4"/>
         <v>600</v>
       </c>
       <c r="D15" s="36"/>
       <c r="E15" s="36"/>
       <c r="F15" s="36"/>
       <c r="G15" s="37">
-        <f>B15/25</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H15" s="37">
-        <f>C15/25</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="I15" s="37">
-        <f>B15/110</f>
+        <f t="shared" si="2"/>
         <v>0.909090909090909</v>
       </c>
       <c r="J15" s="37">
-        <f>C15/110</f>
+        <f t="shared" si="3"/>
         <v>5.45454545454545</v>
       </c>
     </row>
@@ -17275,26 +17279,26 @@
         <v>1000</v>
       </c>
       <c r="C16" s="36">
-        <f>B16+500</f>
+        <f t="shared" si="4"/>
         <v>1500</v>
       </c>
       <c r="D16" s="36"/>
       <c r="E16" s="36"/>
       <c r="F16" s="36"/>
       <c r="G16" s="37">
-        <f>B16/25</f>
+        <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="H16" s="37">
-        <f>C16/25</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="I16" s="37">
-        <f>B16/110</f>
+        <f t="shared" si="2"/>
         <v>9.09090909090909</v>
       </c>
       <c r="J16" s="37">
-        <f>C16/110</f>
+        <f t="shared" si="3"/>
         <v>13.6363636363636</v>
       </c>
     </row>
@@ -17306,26 +17310,26 @@
         <v>200</v>
       </c>
       <c r="C17" s="36">
-        <f>B17+500</f>
+        <f t="shared" si="4"/>
         <v>700</v>
       </c>
       <c r="D17" s="36"/>
       <c r="E17" s="36"/>
       <c r="F17" s="36"/>
       <c r="G17" s="37">
-        <f>B17/25</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H17" s="37">
-        <f>C17/25</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="I17" s="37">
-        <f>B17/110</f>
+        <f t="shared" si="2"/>
         <v>1.81818181818182</v>
       </c>
       <c r="J17" s="37">
-        <f>C17/110</f>
+        <f t="shared" si="3"/>
         <v>6.36363636363636</v>
       </c>
     </row>
@@ -17337,26 +17341,26 @@
         <v>150</v>
       </c>
       <c r="C18">
-        <f>B18+500</f>
+        <f t="shared" si="4"/>
         <v>650</v>
       </c>
       <c r="D18">
         <v>3</v>
       </c>
       <c r="G18" s="35">
-        <f>B18/25</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="H18" s="35">
-        <f>C18/25</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="I18" s="35">
-        <f>B18/110</f>
+        <f t="shared" si="2"/>
         <v>1.36363636363636</v>
       </c>
       <c r="J18" s="35">
-        <f>C18/110</f>
+        <f t="shared" si="3"/>
         <v>5.90909090909091</v>
       </c>
     </row>
@@ -17368,26 +17372,26 @@
         <v>50</v>
       </c>
       <c r="C19">
-        <f>B19+500</f>
+        <f t="shared" si="4"/>
         <v>550</v>
       </c>
       <c r="D19">
         <v>7</v>
       </c>
       <c r="G19" s="35">
-        <f>B19/25</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H19" s="35">
-        <f>C19/25</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="I19" s="35">
-        <f>B19/110</f>
+        <f t="shared" si="2"/>
         <v>0.454545454545455</v>
       </c>
       <c r="J19" s="35">
-        <f>C19/110</f>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
     </row>
@@ -17399,26 +17403,26 @@
         <v>200</v>
       </c>
       <c r="C20">
-        <f>B20+500</f>
+        <f t="shared" si="4"/>
         <v>700</v>
       </c>
       <c r="D20">
         <v>5</v>
       </c>
       <c r="G20" s="35">
-        <f>B20/25</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H20" s="35">
-        <f>C20/25</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="I20" s="35">
-        <f>B20/110</f>
+        <f t="shared" si="2"/>
         <v>1.81818181818182</v>
       </c>
       <c r="J20" s="35">
-        <f>C20/110</f>
+        <f t="shared" si="3"/>
         <v>6.36363636363636</v>
       </c>
     </row>
@@ -17430,26 +17434,26 @@
         <v>100</v>
       </c>
       <c r="C21">
-        <f>B21+500</f>
+        <f t="shared" si="4"/>
         <v>600</v>
       </c>
       <c r="D21">
         <v>5</v>
       </c>
       <c r="G21" s="35">
-        <f>B21/25</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H21" s="35">
-        <f>C21/25</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="I21" s="35">
-        <f>B21/110</f>
+        <f t="shared" si="2"/>
         <v>0.909090909090909</v>
       </c>
       <c r="J21" s="35">
-        <f>C21/110</f>
+        <f t="shared" si="3"/>
         <v>5.45454545454545</v>
       </c>
     </row>
@@ -17461,26 +17465,26 @@
         <v>200</v>
       </c>
       <c r="C22">
-        <f>B22+500</f>
+        <f t="shared" si="4"/>
         <v>700</v>
       </c>
       <c r="D22">
         <v>3</v>
       </c>
       <c r="G22" s="35">
-        <f>B22/25</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="H22" s="35">
-        <f>C22/25</f>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="I22" s="35">
-        <f>B22/110</f>
+        <f t="shared" si="2"/>
         <v>1.81818181818182</v>
       </c>
       <c r="J22" s="35">
-        <f>C22/110</f>
+        <f t="shared" si="3"/>
         <v>6.36363636363636</v>
       </c>
     </row>

</xml_diff>

<commit_message>
<Feature, Story> Prologue, Ch1, Dialogue
Started Ghast enemy.
Enemy prefabs rather than add script on creation.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -2482,12 +2482,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0.0_ "/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="0.0"/>
   </numFmts>
   <fonts count="27">
@@ -2549,73 +2549,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -2631,35 +2564,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2672,10 +2589,85 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2687,7 +2679,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2816,31 +2816,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2858,7 +2840,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2870,7 +2912,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2882,37 +2936,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2924,67 +2960,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2997,6 +2973,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3539,6 +3539,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -3546,6 +3561,21 @@
       </top>
       <bottom style="double">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3574,6 +3604,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -3585,45 +3624,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3641,7 +3641,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3659,130 +3659,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="48" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="49" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="50" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="46" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="49" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="51" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="38" borderId="52" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="52" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="48" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="23" borderId="52" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="53" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="38" borderId="51" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="49" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="53" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="46" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -16728,7 +16728,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -17182,7 +17182,7 @@
         <v>300</v>
       </c>
       <c r="C13" s="36">
-        <f>B13+500</f>
+        <f t="shared" si="4"/>
         <v>800</v>
       </c>
       <c r="D13" s="36">
@@ -17193,19 +17193,19 @@
       </c>
       <c r="F13" s="36"/>
       <c r="G13" s="37">
-        <f>B13/25</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="H13" s="37">
-        <f>C13/25</f>
+        <f t="shared" si="1"/>
         <v>32</v>
       </c>
       <c r="I13" s="37">
-        <f>B13/110</f>
+        <f t="shared" si="2"/>
         <v>2.72727272727273</v>
       </c>
       <c r="J13" s="37">
-        <f>C13/110</f>
+        <f t="shared" si="3"/>
         <v>7.27272727272727</v>
       </c>
     </row>
@@ -17217,26 +17217,26 @@
         <v>100</v>
       </c>
       <c r="C14" s="36">
-        <f>B14+500</f>
+        <f t="shared" si="4"/>
         <v>600</v>
       </c>
       <c r="D14" s="36"/>
       <c r="E14" s="36"/>
       <c r="F14" s="36"/>
       <c r="G14" s="37">
-        <f>B14/25</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="H14" s="37">
-        <f>C14/25</f>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="I14" s="37">
-        <f>B14/110</f>
+        <f t="shared" si="2"/>
         <v>0.909090909090909</v>
       </c>
       <c r="J14" s="37">
-        <f>C14/110</f>
+        <f t="shared" si="3"/>
         <v>5.45454545454545</v>
       </c>
     </row>

</xml_diff>

<commit_message>
<Feature> Ghast, Nightmare, Ghoul Behaviour
Added Ghast projectiles.
Created Nightmare enemy.
Added ghoul drain life attack to Nightmare.
Added crossbeam attack to Nightmare.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13200" firstSheet="2" activeTab="12"/>
+    <workbookView windowWidth="28695" windowHeight="13200" firstSheet="6" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -22,15 +22,16 @@
     <sheet name="Enemy Types" sheetId="16" r:id="rId13"/>
     <sheet name="Region DescriptionGenerator" sheetId="17" r:id="rId14"/>
     <sheet name="Inscriptions" sheetId="22" r:id="rId15"/>
-    <sheet name="Sheet1" sheetId="18" r:id="rId16"/>
-    <sheet name="Sheet2" sheetId="21" r:id="rId17"/>
+    <sheet name="Crafting" sheetId="24" r:id="rId16"/>
+    <sheet name="Sheet1" sheetId="18" r:id="rId17"/>
+    <sheet name="Sheet2" sheetId="21" r:id="rId18"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827">
   <si>
     <t>Type</t>
   </si>
@@ -2412,6 +2413,42 @@
   </si>
   <si>
     <t>Focus</t>
+  </si>
+  <si>
+    <t>Recipes</t>
+  </si>
+  <si>
+    <t>Animal Skin</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>Leather</t>
+  </si>
+  <si>
+    <t>Scrap</t>
+  </si>
+  <si>
+    <t>Reinforced Leather</t>
+  </si>
+  <si>
+    <t>Essence</t>
+  </si>
+  <si>
+    <t>Charcoal</t>
+  </si>
+  <si>
+    <t>Metal</t>
+  </si>
+  <si>
+    <t>Imbued Plate</t>
+  </si>
+  <si>
+    <t>Meat</t>
+  </si>
+  <si>
+    <t>Fuel</t>
   </si>
   <si>
     <t>No Chars</t>
@@ -2482,12 +2519,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0.0_ "/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="0.0"/>
   </numFmts>
   <fonts count="27">
@@ -2549,6 +2586,97 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -2558,7 +2686,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2574,53 +2709,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2634,60 +2723,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2816,7 +2853,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2834,7 +2889,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2846,115 +3003,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2966,25 +3015,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2997,6 +3028,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3540,6 +3577,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -3550,6 +3602,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3580,15 +3641,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3607,23 +3659,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3631,8 +3668,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3641,7 +3678,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3659,130 +3696,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="51" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="49" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="46" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="47" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="48" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="53" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="46" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="50" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="46" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="52" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="49" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="49" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="51" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="38" borderId="52" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="48" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="52" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="53" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="47" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -16727,7 +16764,7 @@
   <sheetPr/>
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
@@ -18651,6 +18688,211 @@
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:I11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.2857142857143" customWidth="1"/>
+    <col min="5" max="5" width="12.2857142857143" customWidth="1"/>
+    <col min="6" max="6" width="19.4285714285714" customWidth="1"/>
+    <col min="7" max="7" width="10.5714285714286" customWidth="1"/>
+    <col min="8" max="8" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D1" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2" t="s">
+        <v>796</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>795</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>797</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>796</v>
+      </c>
+      <c r="D3" t="s">
+        <v>797</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3" t="s">
+        <v>798</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>799</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>800</v>
+      </c>
+      <c r="D4" t="s">
+        <v>798</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>801</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
+        <v>802</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>798</v>
+      </c>
+      <c r="D5" t="s">
+        <v>802</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>800</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>803</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>802</v>
+      </c>
+      <c r="D6" t="s">
+        <v>381</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>804</v>
+      </c>
+      <c r="D7" t="s">
+        <v>804</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>121</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>381</v>
+      </c>
+      <c r="D8" t="s">
+        <v>805</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>797</v>
+      </c>
+      <c r="D9" t="s">
+        <v>805</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>615</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9" t="s">
+        <v>801</v>
+      </c>
+      <c r="I9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>805</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18669,23 +18911,23 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>794</v>
+        <v>806</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>795</v>
+        <v>807</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
       <c r="E1" s="22" t="s">
-        <v>796</v>
+        <v>808</v>
       </c>
       <c r="F1" s="22"/>
       <c r="G1" s="22"/>
       <c r="I1" t="s">
-        <v>797</v>
+        <v>809</v>
       </c>
       <c r="L1" t="s">
-        <v>798</v>
+        <v>810</v>
       </c>
     </row>
     <row r="2" spans="2:12">
@@ -18693,7 +18935,7 @@
         <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>799</v>
+        <v>811</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
@@ -18702,7 +18944,7 @@
         <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>799</v>
+        <v>811</v>
       </c>
       <c r="G2" t="s">
         <v>18</v>
@@ -18842,7 +19084,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" t="s">
-        <v>800</v>
+        <v>812</v>
       </c>
       <c r="B8">
         <f>B3*0.5+B3</f>
@@ -18923,22 +19165,22 @@
     </row>
     <row r="14" spans="1:12">
       <c r="A14" t="s">
-        <v>801</v>
+        <v>813</v>
       </c>
       <c r="B14" t="s">
-        <v>802</v>
+        <v>814</v>
       </c>
       <c r="C14" t="s">
-        <v>798</v>
+        <v>810</v>
       </c>
       <c r="D14" t="s">
-        <v>803</v>
+        <v>815</v>
       </c>
       <c r="E14" t="s">
-        <v>804</v>
+        <v>816</v>
       </c>
       <c r="F14" t="s">
-        <v>805</v>
+        <v>817</v>
       </c>
       <c r="L14">
         <v>9</v>
@@ -19087,12 +19329,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -19108,13 +19350,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>806</v>
+        <v>818</v>
       </c>
       <c r="B1" t="s">
-        <v>807</v>
+        <v>819</v>
       </c>
       <c r="C1" t="s">
-        <v>808</v>
+        <v>820</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -19455,7 +19697,7 @@
     </row>
     <row r="30" spans="4:5">
       <c r="D30" t="s">
-        <v>809</v>
+        <v>821</v>
       </c>
       <c r="E30">
         <v>0.75</v>
@@ -19463,7 +19705,7 @@
     </row>
     <row r="32" spans="1:8">
       <c r="A32" s="2" t="s">
-        <v>810</v>
+        <v>822</v>
       </c>
       <c r="B32" s="2">
         <v>10</v>
@@ -19488,13 +19730,13 @@
         <v>68</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>811</v>
+        <v>823</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>812</v>
+        <v>824</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>813</v>
+        <v>825</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>3</v>
@@ -19521,7 +19763,7 @@
         <v>13</v>
       </c>
       <c r="O33" s="5" t="s">
-        <v>814</v>
+        <v>826</v>
       </c>
       <c r="P33" s="7" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
<Feature> Shake, Sound, Menus
Added light camera shake.
Fixed bug where enemy fire rate matched frame rate.
Insect fades when plant found.
Fixed bug where map could try to find a route to a null region.
Added explosion audio.
Added map pulse audio.
Moved construction and consumable menus to inventory menu.
Fixed issue where pathinggrid would not resize with gridwidth.
Fixed issue where map rings would have no material.
Rebalanced weapon fire rates.
Added high pass filter to weapons to make them sound cruddy at low
durabilities.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="3" activeTab="5"/>
+    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -2935,11 +2935,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
-    <numFmt numFmtId="177" formatCode="0_ "/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="0_ "/>
     <numFmt numFmtId="178" formatCode="0.0"/>
     <numFmt numFmtId="179" formatCode="0.0_ "/>
   </numFmts>
@@ -3002,8 +3002,113 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -3018,114 +3123,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3139,10 +3139,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3268,13 +3268,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3292,7 +3376,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3304,31 +3388,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3346,37 +3424,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3388,67 +3442,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3855,16 +3855,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3873,17 +3873,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -3905,25 +3894,42 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3937,17 +3943,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3956,7 +3956,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3974,130 +3974,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="35" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="49" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="38" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -21614,8 +21614,8 @@
   <sheetPr/>
   <dimension ref="A1:Y18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -22070,7 +22070,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="119">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F9" s="119">
         <v>2.5</v>
@@ -22090,11 +22090,11 @@
       </c>
       <c r="K9" s="143">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="L9" s="143">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="M9" s="143">
         <f t="shared" si="3"/>
@@ -22102,7 +22102,7 @@
       </c>
       <c r="N9" s="144">
         <f t="shared" si="4"/>
-        <v>51.4285714285714</v>
+        <v>45</v>
       </c>
       <c r="P9">
         <f t="shared" si="5"/>
@@ -22179,7 +22179,7 @@
         <v>8</v>
       </c>
       <c r="E11" s="125">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" s="125">
         <v>2.5</v>
@@ -22199,11 +22199,11 @@
       </c>
       <c r="K11" s="145">
         <f t="shared" si="1"/>
-        <v>0.666666666666667</v>
+        <v>1</v>
       </c>
       <c r="L11" s="145">
         <f t="shared" si="2"/>
-        <v>3.16666666666667</v>
+        <v>3.5</v>
       </c>
       <c r="M11" s="145">
         <f t="shared" si="3"/>
@@ -22211,7 +22211,7 @@
       </c>
       <c r="N11" s="146">
         <f t="shared" si="4"/>
-        <v>50.5263157894737</v>
+        <v>45.7142857142857</v>
       </c>
       <c r="P11">
         <f t="shared" si="5"/>
@@ -22236,7 +22236,7 @@
         <v>5</v>
       </c>
       <c r="E12" s="119">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F12" s="119">
         <v>1</v>
@@ -22256,11 +22256,11 @@
       </c>
       <c r="K12" s="143">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="L12" s="143">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="M12" s="143">
         <f t="shared" si="3"/>
@@ -22268,7 +22268,7 @@
       </c>
       <c r="N12" s="144">
         <f t="shared" si="4"/>
-        <v>50</v>
+        <v>42.8571428571429</v>
       </c>
       <c r="P12">
         <f t="shared" si="5"/>
@@ -22290,7 +22290,7 @@
         <v>8</v>
       </c>
       <c r="E13" s="119">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F13" s="119">
         <v>1.25</v>
@@ -22310,11 +22310,11 @@
       </c>
       <c r="K13" s="143">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="L13" s="143">
         <f t="shared" si="2"/>
-        <v>3.25</v>
+        <v>3.75</v>
       </c>
       <c r="M13" s="143">
         <f t="shared" si="3"/>
@@ -22322,7 +22322,7 @@
       </c>
       <c r="N13" s="144">
         <f t="shared" si="4"/>
-        <v>49.2307692307692</v>
+        <v>42.6666666666667</v>
       </c>
       <c r="P13">
         <f t="shared" si="5"/>
@@ -22344,7 +22344,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="125">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F14" s="125">
         <v>1</v>
@@ -22364,11 +22364,11 @@
       </c>
       <c r="K14" s="145">
         <f t="shared" si="1"/>
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="L14" s="145">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="M14" s="145">
         <f t="shared" si="3"/>
@@ -22376,7 +22376,7 @@
       </c>
       <c r="N14" s="146">
         <f t="shared" si="4"/>
-        <v>51.4285714285714</v>
+        <v>45</v>
       </c>
       <c r="P14">
         <f t="shared" si="5"/>
@@ -22397,10 +22397,10 @@
         <v>58</v>
       </c>
       <c r="D15" s="118">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E15" s="119">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="F15" s="119">
         <v>5</v>
@@ -22416,28 +22416,28 @@
       </c>
       <c r="J15" s="143">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="K15" s="143">
         <f t="shared" si="1"/>
-        <v>3.5</v>
+        <v>14</v>
       </c>
       <c r="L15" s="143">
         <f t="shared" si="2"/>
-        <v>8.5</v>
+        <v>19</v>
       </c>
       <c r="M15" s="143">
         <f t="shared" si="3"/>
-        <v>420</v>
+        <v>700</v>
       </c>
       <c r="N15" s="144">
         <f t="shared" si="4"/>
-        <v>49.4117647058824</v>
+        <v>36.8421052631579</v>
       </c>
       <c r="O15" s="82"/>
       <c r="P15">
         <f t="shared" si="5"/>
-        <v>0.006</v>
+        <v>0.01</v>
       </c>
       <c r="Q15"/>
       <c r="R15" t="s">
@@ -25062,7 +25062,7 @@
   <sheetPr/>
   <dimension ref="A1:W40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
<Feature, Art> Boss 4, Tombs
Started Ova boss (sperm and egg).
Added nightmare art.
Updated ghoulmother art.
Added player art.
Fixed issue where instantly returning to home wouldn't return to rest
state.
Fixed bug where shotgun skill 4 had no seek target if there are no
enemies.
Boss sections now register as enemies.
Removed slice attack.
Completing temples now increments the temple counter.
When all temples explored player is taken to tomb to fight boss.
When boss fight is won, player is taken to new environment.
Fixed bug where echoes would try to generate when there are no valid
positions.
Updated temple behaviour to have more varied enemies.
Improved shot accuracy calculation, now has a tendancy to shoot
centrally rather than evenly spread.
Fixed bug where disabling an enhanced button wouldn't cause it to
deselect.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="2" activeTab="11"/>
+    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="3" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="990">
   <si>
     <t>Type</t>
   </si>
@@ -2907,9 +2907,6 @@
   </si>
   <si>
     <t>Sickness noise</t>
-  </si>
-  <si>
-    <t>Wolves</t>
   </si>
   <si>
     <t>Bullet impact</t>
@@ -14433,8 +14430,8 @@
   <sheetPr/>
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -16752,8 +16749,8 @@
   <sheetPr/>
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -16912,25 +16909,22 @@
         <v>957</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:1">
       <c r="A14" t="s">
         <v>958</v>
       </c>
-      <c r="B14" t="s">
-        <v>959</v>
-      </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
+        <v>959</v>
+      </c>
+      <c r="B15" t="s">
         <v>960</v>
-      </c>
-      <c r="B15" t="s">
-        <v>961</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B16" t="s">
         <v>132</v>
@@ -16938,73 +16932,73 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
+        <v>962</v>
+      </c>
+      <c r="B17" t="s">
         <v>963</v>
-      </c>
-      <c r="B17" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
+        <v>964</v>
+      </c>
+      <c r="B18" t="s">
         <v>965</v>
-      </c>
-      <c r="B18" t="s">
-        <v>966</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="B19" t="s">
         <v>967</v>
-      </c>
-      <c r="B19" t="s">
-        <v>968</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="B20" t="s">
         <v>969</v>
-      </c>
-      <c r="B20" t="s">
-        <v>970</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="B21" t="s">
         <v>971</v>
-      </c>
-      <c r="B21" t="s">
-        <v>972</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="B22" t="s">
         <v>973</v>
-      </c>
-      <c r="B22" t="s">
-        <v>974</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
+        <v>974</v>
+      </c>
+      <c r="B23" t="s">
         <v>975</v>
-      </c>
-      <c r="B23" t="s">
-        <v>976</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
   </sheetData>
@@ -17323,57 +17317,57 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="6" spans="1:1">
       <c r="A6" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="1" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="9" spans="1:1">
       <c r="A9" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="11" spans="1:1">
       <c r="A11" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="12" spans="1:1">
       <c r="A12" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="13" spans="1:1">

</xml_diff>

<commit_message>
<Feature, Lore> Weapon Menu, Lore
Added 3 new lore entries.
Finished weapon updated weapon menu.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -3017,8 +3017,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="0_ "/>
@@ -3084,9 +3084,31 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3106,6 +3128,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -3114,11 +3143,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3129,8 +3173,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3146,60 +3207,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3213,16 +3221,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3350,13 +3350,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3368,55 +3374,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3428,13 +3386,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3452,25 +3410,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3488,19 +3446,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3512,25 +3464,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3936,26 +3936,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3971,17 +3951,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3996,16 +3970,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4027,6 +4001,32 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
@@ -4038,7 +4038,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4056,31 +4056,31 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="38" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="38" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4089,97 +4089,97 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="46" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="45" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="45" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -23685,7 +23685,7 @@
   <dimension ref="A1:U34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -24036,7 +24036,7 @@
         <v>0.2</v>
       </c>
       <c r="E8" s="95">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="95">
         <v>3</v>
@@ -24085,10 +24085,10 @@
         <v>1</v>
       </c>
       <c r="E9" s="95">
+        <v>-1</v>
+      </c>
+      <c r="F9" s="95">
         <v>0</v>
-      </c>
-      <c r="F9" s="95">
-        <v>0.3</v>
       </c>
       <c r="G9" s="95">
         <v>0</v>
@@ -24132,7 +24132,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="95">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="G10" s="95">
         <v>0</v>
@@ -24180,7 +24180,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="95">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="95">
         <v>0</v>
@@ -24228,7 +24228,7 @@
         <v>0.8</v>
       </c>
       <c r="E12" s="95">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="95">
         <v>0</v>
@@ -24274,7 +24274,7 @@
         <v>0.2</v>
       </c>
       <c r="E13" s="95">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F13" s="95">
         <v>1</v>
@@ -24379,7 +24379,7 @@
         <v>1</v>
       </c>
       <c r="E15" s="95">
-        <v>-0.2</v>
+        <v>-2</v>
       </c>
       <c r="F15" s="95">
         <v>0</v>
@@ -24421,7 +24421,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="95">
-        <v>-0.2</v>
+        <v>0</v>
       </c>
       <c r="G16" s="95">
         <v>3</v>
@@ -24468,7 +24468,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="95">
-        <v>-0.3</v>
+        <v>0</v>
       </c>
       <c r="G17" s="95">
         <v>0</v>

</xml_diff>

<commit_message>
<Feature, Art> Skill art
Added skill art for Sniper, Medic, Martyr, Warlord, Witch, Beam, and
Split.
Fixed mapnode shadow not showing.
Fixed instant reload brand not working.
Added resource bonus from brand.
Added hunger and thirst bonuses from brand.
Fixed push not aligning to target correctly.
Fixed split generating too many children.
Fixed splitting bosses not counting towards Temple.
Added skill animation.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="2" activeTab="7"/>
+    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="4" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -3019,12 +3019,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
+    <numFmt numFmtId="176" formatCode="0_ "/>
+    <numFmt numFmtId="177" formatCode="0.00_ "/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
-    <numFmt numFmtId="177" formatCode="0_ "/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="0.0"/>
     <numFmt numFmtId="179" formatCode="0.0_ "/>
   </numFmts>
@@ -3088,6 +3088,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -3111,43 +3126,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3170,7 +3188,36 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3179,53 +3226,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3353,7 +3353,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3365,25 +3491,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3395,85 +3503,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3486,54 +3534,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3939,6 +3939,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3963,11 +3974,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4004,35 +4030,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4041,7 +4041,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4059,130 +4059,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="38" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="40" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="45" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="27" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4217,13 +4217,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -4388,7 +4388,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -17319,13 +17319,13 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="26.7142857142857" customWidth="1"/>
   </cols>
@@ -17388,6 +17388,47 @@
     <row r="13" spans="1:1">
       <c r="A13" t="s">
         <v>210</v>
+      </c>
+    </row>
+    <row r="16" spans="6:7">
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="6:8">
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>50</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="6:8">
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>12</v>
+      </c>
+      <c r="H18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8">
+      <c r="F19">
+        <v>3</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -28154,7 +28195,7 @@
   <sheetPr/>
   <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -28926,7 +28967,7 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -29152,13 +29193,13 @@
       <c r="C11" s="48" t="s">
         <v>710</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="49" t="s">
         <v>711</v>
       </c>
       <c r="E11" s="48" t="s">
         <v>712</v>
       </c>
-      <c r="F11" s="48" t="s">
+      <c r="F11" s="49" t="s">
         <v>707</v>
       </c>
     </row>
@@ -29172,13 +29213,13 @@
       <c r="C12" s="50" t="s">
         <v>715</v>
       </c>
-      <c r="D12" s="50" t="s">
+      <c r="D12" s="51" t="s">
         <v>716</v>
       </c>
       <c r="E12" s="50" t="s">
         <v>717</v>
       </c>
-      <c r="F12" s="50" t="s">
+      <c r="F12" s="51" t="s">
         <v>718</v>
       </c>
     </row>
@@ -29192,13 +29233,13 @@
       <c r="C13" s="48" t="s">
         <v>721</v>
       </c>
-      <c r="D13" s="48" t="s">
+      <c r="D13" s="49" t="s">
         <v>722</v>
       </c>
       <c r="E13" s="48" t="s">
         <v>723</v>
       </c>
-      <c r="F13" s="48" t="s">
+      <c r="F13" s="49" t="s">
         <v>724</v>
       </c>
     </row>
@@ -29212,7 +29253,7 @@
       <c r="C14" s="50" t="s">
         <v>727</v>
       </c>
-      <c r="D14" s="50" t="s">
+      <c r="D14" s="51" t="s">
         <v>728</v>
       </c>
       <c r="E14" s="50" t="s">

</xml_diff>

<commit_message>
<Lore, Art> Enemy Icons
Redesigned and added enemy icons for human enemies.
Implemented all brand mechanics.
Added willpower requirement for exploring and crafting.
Added another page of lore.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="4" activeTab="16"/>
+    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -3019,10 +3019,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
-    <numFmt numFmtId="176" formatCode="0_ "/>
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0_ "/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="0.0"/>
@@ -3088,7 +3088,21 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3097,21 +3111,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3126,7 +3125,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3165,14 +3186,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -3187,35 +3208,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -3224,8 +3217,15 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3353,7 +3353,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3365,13 +3365,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3383,79 +3443,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3479,13 +3467,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3497,43 +3527,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3950,6 +3950,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -3968,8 +3992,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3997,51 +4036,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4059,130 +4059,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="40" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="36" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="40" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="45" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4217,13 +4217,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -4388,7 +4388,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -17321,7 +17321,7 @@
   <sheetPr/>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -28966,8 +28966,8 @@
   <sheetPr/>
   <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -29153,13 +29153,13 @@
       <c r="C9" s="48" t="s">
         <v>698</v>
       </c>
-      <c r="D9" s="48" t="s">
+      <c r="D9" s="49" t="s">
         <v>699</v>
       </c>
       <c r="E9" s="48" t="s">
         <v>700</v>
       </c>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="49" t="s">
         <v>701</v>
       </c>
     </row>

</xml_diff>

<commit_message>
<Feature, Bugfix, Story> Fountain Spawn, Action Bar
Action progress now denoted by bar.
Progress updated correctly.
Fountain spawns enemies using spawning projectile.
Fixed bug where light obstructors weren't being detected.
Fixed bug where object pool tried to destroy obejcts that didn't exist.
Fixed bug where shadow rendertexture size didn't fit screen.
2nd pass on story.
Added more lore entries.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="3" activeTab="14"/>
+    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="5" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -16779,7 +16779,7 @@
   <sheetPr/>
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -17376,8 +17376,8 @@
   <sheetPr/>
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>

</xml_diff>

<commit_message>
<Feature, Bugfix> Events, Fire, Audio
Combat rain and wind sounds.
Button click in combat.
Crackling fire controller.
Fire intensity controller.
Combat event text controller.
Radiance visuals.
Fixed bug where couldn't claim region even if more than 1 radiance
available.
Added radiance visuals to map node.
Added enemy health scaling.
Fixed bug with damage calculation on shot.
Fixed region name fade in.
Added fire bursts to fire.
Campfire regenerates endurance and perception.
Brand requirement now shown.
More footprint audio added.
Footprint audio randomiser better.
Equipping weapons and armour works in combat.
Reduced double fire delay time.
Simplified scene change code.
Fixed bug where equipping gear in combat would send it to home
inventory.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="5" activeTab="15"/>
+    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="5" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -11956,8 +11956,8 @@
   <sheetPr/>
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -12042,11 +12042,11 @@
         <v>641</v>
       </c>
       <c r="B3">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="C3">
         <f>B3+500</f>
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -12068,19 +12068,19 @@
       </c>
       <c r="J3" s="35">
         <f t="shared" ref="J3:J24" si="0">B3/25</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="K3" s="35">
         <f t="shared" ref="K3:K24" si="1">C3/25</f>
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="L3" s="35">
         <f t="shared" ref="L3:L24" si="2">B3/110</f>
-        <v>3.63636363636364</v>
+        <v>1.81818181818182</v>
       </c>
       <c r="M3" s="35">
         <f t="shared" ref="M3:M24" si="3">C3/110</f>
-        <v>8.18181818181818</v>
+        <v>6.36363636363636</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>800</v>
@@ -12091,11 +12091,11 @@
         <v>801</v>
       </c>
       <c r="B4">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C24" si="4">B4+500</f>
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -12117,19 +12117,19 @@
       </c>
       <c r="J4" s="35">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K4" s="35">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L4" s="35">
         <f t="shared" si="2"/>
-        <v>1.81818181818182</v>
+        <v>0.909090909090909</v>
       </c>
       <c r="M4" s="35">
         <f t="shared" si="3"/>
-        <v>6.36363636363636</v>
+        <v>5.45454545454545</v>
       </c>
       <c r="O4" t="s">
         <v>802</v>
@@ -12140,11 +12140,11 @@
         <v>803</v>
       </c>
       <c r="B5">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="C5">
         <f t="shared" si="4"/>
-        <v>1100</v>
+        <v>800</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -12166,19 +12166,19 @@
       </c>
       <c r="J5" s="35">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="K5" s="35">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="L5" s="35">
         <f t="shared" si="2"/>
-        <v>5.45454545454545</v>
+        <v>2.72727272727273</v>
       </c>
       <c r="M5" s="35">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>7.27272727272727</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>805</v>
@@ -12189,11 +12189,11 @@
         <v>806</v>
       </c>
       <c r="B6">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="C6">
         <f t="shared" si="4"/>
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -12215,19 +12215,19 @@
       </c>
       <c r="J6" s="35">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="K6" s="35">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="L6" s="35">
         <f t="shared" si="2"/>
-        <v>3.63636363636364</v>
+        <v>1.81818181818182</v>
       </c>
       <c r="M6" s="35">
         <f t="shared" si="3"/>
-        <v>8.18181818181818</v>
+        <v>6.36363636363636</v>
       </c>
       <c r="O6" t="s">
         <v>808</v>
@@ -12238,11 +12238,11 @@
         <v>809</v>
       </c>
       <c r="B7">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="C7">
         <f t="shared" si="4"/>
-        <v>1300</v>
+        <v>900</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -12264,19 +12264,19 @@
       </c>
       <c r="J7" s="35">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="K7" s="35">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="L7" s="35">
         <f t="shared" si="2"/>
-        <v>7.27272727272727</v>
+        <v>3.63636363636364</v>
       </c>
       <c r="M7" s="35">
         <f t="shared" si="3"/>
-        <v>11.8181818181818</v>
+        <v>8.18181818181818</v>
       </c>
       <c r="O7" t="s">
         <v>811</v>
@@ -12287,11 +12287,11 @@
         <v>812</v>
       </c>
       <c r="B8">
-        <v>1200</v>
+        <v>600</v>
       </c>
       <c r="C8">
         <f t="shared" si="4"/>
-        <v>1700</v>
+        <v>1100</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -12313,19 +12313,19 @@
       </c>
       <c r="J8" s="35">
         <f t="shared" si="0"/>
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="K8" s="35">
         <f t="shared" si="1"/>
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="L8" s="35">
         <f t="shared" si="2"/>
-        <v>10.9090909090909</v>
+        <v>5.45454545454545</v>
       </c>
       <c r="M8" s="35">
         <f t="shared" si="3"/>
-        <v>15.4545454545455</v>
+        <v>10</v>
       </c>
       <c r="O8" t="s">
         <v>813</v>
@@ -12336,11 +12336,11 @@
         <v>814</v>
       </c>
       <c r="B9">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <f t="shared" si="4"/>
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -12362,19 +12362,19 @@
       </c>
       <c r="J9" s="35">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K9" s="35">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L9" s="35">
         <f t="shared" si="2"/>
-        <v>0.909090909090909</v>
+        <v>0.454545454545455</v>
       </c>
       <c r="M9" s="35">
         <f t="shared" si="3"/>
-        <v>5.45454545454545</v>
+        <v>5</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>815</v>
@@ -12391,11 +12391,11 @@
         <v>818</v>
       </c>
       <c r="B10">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="C10">
         <f t="shared" si="4"/>
-        <v>1100</v>
+        <v>800</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -12417,19 +12417,19 @@
       </c>
       <c r="J10" s="35">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="K10" s="35">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="L10" s="35">
         <f t="shared" si="2"/>
-        <v>5.45454545454545</v>
+        <v>2.72727272727273</v>
       </c>
       <c r="M10" s="35">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>7.27272727272727</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>819</v>
@@ -12455,11 +12455,11 @@
         <v>820</v>
       </c>
       <c r="B11" s="34">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C11" s="34">
         <f t="shared" si="4"/>
-        <v>550</v>
+        <v>525</v>
       </c>
       <c r="D11" s="34">
         <v>6</v>
@@ -12481,19 +12481,19 @@
       </c>
       <c r="J11" s="36">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K11" s="36">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L11" s="36">
         <f t="shared" si="2"/>
-        <v>0.454545454545455</v>
+        <v>0.227272727272727</v>
       </c>
       <c r="M11" s="36">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>4.77272727272727</v>
       </c>
       <c r="O11" t="s">
         <v>823</v>
@@ -12519,11 +12519,11 @@
         <v>824</v>
       </c>
       <c r="B12" s="34">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="C12" s="34">
         <f t="shared" si="4"/>
-        <v>1100</v>
+        <v>800</v>
       </c>
       <c r="D12" s="34">
         <v>3</v>
@@ -12545,19 +12545,19 @@
       </c>
       <c r="J12" s="36">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="K12" s="36">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="L12" s="36">
         <f t="shared" si="2"/>
-        <v>5.45454545454545</v>
+        <v>2.72727272727273</v>
       </c>
       <c r="M12" s="36">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>7.27272727272727</v>
       </c>
       <c r="O12" t="s">
         <v>826</v>
@@ -12583,11 +12583,11 @@
         <v>827</v>
       </c>
       <c r="B13" s="34">
-        <v>600</v>
+        <v>300</v>
       </c>
       <c r="C13" s="34">
         <f t="shared" si="4"/>
-        <v>1100</v>
+        <v>800</v>
       </c>
       <c r="D13" s="34">
         <v>5</v>
@@ -12609,19 +12609,19 @@
       </c>
       <c r="J13" s="36">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="K13" s="36">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="L13" s="36">
         <f t="shared" si="2"/>
-        <v>5.45454545454545</v>
+        <v>2.72727272727273</v>
       </c>
       <c r="M13" s="36">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>7.27272727272727</v>
       </c>
       <c r="O13" t="s">
         <v>828</v>
@@ -12647,11 +12647,11 @@
         <v>829</v>
       </c>
       <c r="B14" s="34">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="C14" s="34">
         <f t="shared" si="4"/>
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="D14" s="34">
         <v>5</v>
@@ -12673,19 +12673,19 @@
       </c>
       <c r="J14" s="36">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="K14" s="36">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="L14" s="36">
         <f t="shared" si="2"/>
-        <v>3.63636363636364</v>
+        <v>1.81818181818182</v>
       </c>
       <c r="M14" s="36">
         <f t="shared" si="3"/>
-        <v>8.18181818181818</v>
+        <v>6.36363636363636</v>
       </c>
       <c r="O14" t="s">
         <v>831</v>
@@ -12711,11 +12711,11 @@
         <v>832</v>
       </c>
       <c r="B15" s="34">
-        <v>250</v>
+        <v>125</v>
       </c>
       <c r="C15" s="34">
         <f t="shared" si="4"/>
-        <v>750</v>
+        <v>625</v>
       </c>
       <c r="D15" s="34">
         <v>5</v>
@@ -12737,19 +12737,19 @@
       </c>
       <c r="J15" s="36">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="K15" s="36">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="L15" s="36">
         <f t="shared" si="2"/>
-        <v>2.27272727272727</v>
+        <v>1.13636363636364</v>
       </c>
       <c r="M15" s="36">
         <f t="shared" si="3"/>
-        <v>6.81818181818182</v>
+        <v>5.68181818181818</v>
       </c>
       <c r="O15" t="s">
         <v>834</v>
@@ -12775,11 +12775,11 @@
         <v>822</v>
       </c>
       <c r="B16" s="34">
-        <v>800</v>
+        <v>400</v>
       </c>
       <c r="C16" s="34">
         <f t="shared" si="4"/>
-        <v>1300</v>
+        <v>900</v>
       </c>
       <c r="D16" s="34">
         <v>5</v>
@@ -12801,19 +12801,19 @@
       </c>
       <c r="J16" s="36">
         <f t="shared" si="0"/>
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="K16" s="36">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="L16" s="36">
         <f t="shared" si="2"/>
-        <v>7.27272727272727</v>
+        <v>3.63636363636364</v>
       </c>
       <c r="M16" s="36">
         <f t="shared" si="3"/>
-        <v>11.8181818181818</v>
+        <v>8.18181818181818</v>
       </c>
       <c r="O16" t="s">
         <v>836</v>
@@ -12839,11 +12839,11 @@
         <v>837</v>
       </c>
       <c r="B17" s="34">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C17" s="34">
         <f t="shared" si="4"/>
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="D17" s="34">
         <v>5</v>
@@ -12865,19 +12865,19 @@
       </c>
       <c r="J17" s="36">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K17" s="36">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L17" s="36">
         <f t="shared" si="2"/>
-        <v>1.81818181818182</v>
+        <v>0.909090909090909</v>
       </c>
       <c r="M17" s="36">
         <f t="shared" si="3"/>
-        <v>6.36363636363636</v>
+        <v>5.45454545454545</v>
       </c>
       <c r="O17" t="s">
         <v>838</v>
@@ -12961,11 +12961,11 @@
         <v>840</v>
       </c>
       <c r="B19" s="34">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C19" s="34">
         <f t="shared" si="4"/>
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="D19" s="34">
         <v>0</v>
@@ -12984,19 +12984,19 @@
       </c>
       <c r="J19" s="36">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K19" s="36">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L19" s="36">
         <f t="shared" si="2"/>
-        <v>0.909090909090909</v>
+        <v>0.454545454545455</v>
       </c>
       <c r="M19" s="36">
         <f t="shared" si="3"/>
-        <v>5.45454545454545</v>
+        <v>5</v>
       </c>
       <c r="Q19">
         <v>0.9</v>
@@ -13019,11 +13019,11 @@
         <v>841</v>
       </c>
       <c r="B20">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C20">
         <f t="shared" si="4"/>
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -13045,19 +13045,19 @@
       </c>
       <c r="J20" s="35">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K20" s="35">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="L20" s="35">
         <f t="shared" si="2"/>
-        <v>1.81818181818182</v>
+        <v>0.909090909090909</v>
       </c>
       <c r="M20" s="35">
         <f t="shared" si="3"/>
-        <v>6.36363636363636</v>
+        <v>5.45454545454545</v>
       </c>
       <c r="O20" t="s">
         <v>843</v>
@@ -13083,11 +13083,11 @@
         <v>553</v>
       </c>
       <c r="B21">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="C21">
         <f t="shared" si="4"/>
-        <v>900</v>
+        <v>700</v>
       </c>
       <c r="D21">
         <v>7</v>
@@ -13109,19 +13109,19 @@
       </c>
       <c r="J21" s="35">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="K21" s="35">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="L21" s="35">
         <f t="shared" si="2"/>
-        <v>3.63636363636364</v>
+        <v>1.81818181818182</v>
       </c>
       <c r="M21" s="35">
         <f t="shared" si="3"/>
-        <v>8.18181818181818</v>
+        <v>6.36363636363636</v>
       </c>
       <c r="O21" t="s">
         <v>845</v>
@@ -13132,11 +13132,11 @@
         <v>846</v>
       </c>
       <c r="B22">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C22">
         <f t="shared" si="4"/>
-        <v>600</v>
+        <v>550</v>
       </c>
       <c r="D22">
         <v>6</v>
@@ -13158,19 +13158,19 @@
       </c>
       <c r="J22" s="35">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K22" s="35">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L22" s="35">
         <f t="shared" si="2"/>
-        <v>0.909090909090909</v>
+        <v>0.454545454545455</v>
       </c>
       <c r="M22" s="35">
         <f t="shared" si="3"/>
-        <v>5.45454545454545</v>
+        <v>5</v>
       </c>
       <c r="O22" t="s">
         <v>848</v>
@@ -13181,11 +13181,11 @@
         <v>849</v>
       </c>
       <c r="B23">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="C23">
         <f t="shared" si="4"/>
-        <v>550</v>
+        <v>525</v>
       </c>
       <c r="D23">
         <v>10</v>
@@ -13207,19 +13207,19 @@
       </c>
       <c r="J23" s="35">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K23" s="35">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="L23" s="35">
         <f t="shared" si="2"/>
-        <v>0.454545454545455</v>
+        <v>0.227272727272727</v>
       </c>
       <c r="M23" s="35">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>4.77272727272727</v>
       </c>
       <c r="O23" t="s">
         <v>851</v>
@@ -15873,7 +15873,7 @@
   <sheetPr/>
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
<Feature, Bugfix> Menu, Consumables
Consumables now provide permanent boost.
Added camera lock controller to menu.
Redesigned controls menus for easier reading.
Updated pause menu (not yet working).
Load is done based on most recent file between quicksave and manualsave.
Adrenaline gain modifier now used.
Added edge collider to region.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="5" activeTab="10"/>
+    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="5" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058">
   <si>
     <t>Type</t>
   </si>
@@ -2743,9 +2743,6 @@
     <t>Tainted Water</t>
   </si>
   <si>
-    <t>+</t>
-  </si>
-  <si>
     <t>Milk of the Earth</t>
   </si>
   <si>
@@ -2792,12 +2789,6 @@
   </si>
   <si>
     <t>Cinderberry</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>12</t>
   </si>
   <si>
     <t>Blightberry</t>
@@ -4411,6 +4402,9 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -4423,15 +4417,15 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -4442,9 +4436,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
@@ -11956,7 +11947,7 @@
   <sheetPr/>
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
@@ -14291,10 +14282,10 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S41"/>
+  <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -14302,21 +14293,20 @@
     <col min="1" max="1" width="22.1428571428571" style="5" customWidth="1"/>
     <col min="2" max="2" width="16.5714285714286" style="5" customWidth="1"/>
     <col min="3" max="3" width="26.8571428571429" style="5" customWidth="1"/>
-    <col min="4" max="5" width="9.42857142857143" style="5" customWidth="1"/>
-    <col min="6" max="6" width="13.4285714285714" style="5" customWidth="1"/>
-    <col min="7" max="7" width="6.28571428571429" style="5" customWidth="1"/>
-    <col min="8" max="8" width="7.85714285714286" style="5" customWidth="1"/>
-    <col min="9" max="9" width="6.42857142857143" style="5" customWidth="1"/>
-    <col min="10" max="10" width="8" style="5" customWidth="1"/>
-    <col min="11" max="11" width="11.2857142857143" style="5" customWidth="1"/>
-    <col min="12" max="14" width="9.14285714285714" style="5"/>
-    <col min="15" max="16" width="7.85714285714286" style="5" customWidth="1"/>
-    <col min="17" max="17" width="8.85714285714286" style="5" customWidth="1"/>
-    <col min="18" max="18" width="7.85714285714286" style="5" customWidth="1"/>
-    <col min="19" max="16384" width="9.14285714285714" style="5"/>
+    <col min="4" max="4" width="16.1428571428571" style="5" customWidth="1"/>
+    <col min="5" max="5" width="6.28571428571429" style="5" customWidth="1"/>
+    <col min="6" max="6" width="7.85714285714286" style="5" customWidth="1"/>
+    <col min="7" max="7" width="6.42857142857143" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8" style="5" customWidth="1"/>
+    <col min="9" max="9" width="11.2857142857143" style="5" customWidth="1"/>
+    <col min="10" max="12" width="9.14285714285714" style="5"/>
+    <col min="13" max="14" width="7.85714285714286" style="5" customWidth="1"/>
+    <col min="15" max="15" width="8.85714285714286" style="5" customWidth="1"/>
+    <col min="16" max="16" width="7.85714285714286" style="5" customWidth="1"/>
+    <col min="17" max="16384" width="9.14285714285714" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:17">
       <c r="A1" s="6" t="s">
         <v>119</v>
       </c>
@@ -14327,1232 +14317,1135 @@
         <v>661</v>
       </c>
       <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6" t="s">
-        <v>126</v>
-      </c>
-      <c r="G1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>900</v>
       </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
       <c r="H1" s="6"/>
       <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>901</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="17" t="s">
+      <c r="L1" s="11"/>
+      <c r="M1" s="18" t="s">
         <v>902</v>
       </c>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-    </row>
-    <row r="2" spans="1:19">
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="7" t="s">
         <v>767</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="E2" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>182</v>
+      </c>
       <c r="G2" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="J2" s="6"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="N2" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="O2" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="P2" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="Q2" s="19" t="s">
         <v>185</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q2" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="R2" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="S2" s="18" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="8" t="s">
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10">
+      <c r="D3" s="10"/>
+      <c r="E3" s="11">
         <v>0.9</v>
       </c>
-      <c r="H3" s="10">
+      <c r="F3" s="11">
         <v>0.7</v>
       </c>
-      <c r="I3" s="10">
+      <c r="G3" s="11">
         <v>0.5</v>
       </c>
-      <c r="J3" s="10">
+      <c r="H3" s="11">
         <v>0.3</v>
       </c>
-      <c r="K3" s="10">
+      <c r="I3" s="11">
         <v>0.1</v>
       </c>
-      <c r="L3" s="10">
-        <f t="shared" ref="L3:L22" si="0">SUM(G3:K3)</f>
+      <c r="J3" s="11">
+        <f t="shared" ref="J3:J22" si="0">SUM(E3:I3)</f>
         <v>2.5</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="L3" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="O3" s="10">
+      <c r="M3" s="11">
+        <f>SUM(E3:E6)</f>
+        <v>1</v>
+      </c>
+      <c r="N3" s="11">
+        <f>SUM(F3:F6)</f>
+        <v>1</v>
+      </c>
+      <c r="O3" s="11">
         <f>SUM(G3:G6)</f>
         <v>1</v>
       </c>
-      <c r="P3" s="10">
+      <c r="P3" s="11">
         <f>SUM(H3:H6)</f>
         <v>1</v>
       </c>
-      <c r="Q3" s="10">
+      <c r="Q3" s="11">
         <f>SUM(I3:I6)</f>
         <v>1</v>
       </c>
-      <c r="R3" s="10">
-        <f>SUM(J3:J6)</f>
-        <v>1</v>
-      </c>
-      <c r="S3" s="10">
-        <f>SUM(K3:K6)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19">
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="5" t="s">
         <v>903</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>123</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>541</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="12" t="s">
         <v>669</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>904</v>
-      </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="10">
+      <c r="E4" s="11">
         <v>0.1</v>
       </c>
-      <c r="H4" s="10">
+      <c r="F4" s="11">
         <v>0.2</v>
       </c>
-      <c r="I4" s="10">
+      <c r="G4" s="11">
         <v>0.3</v>
       </c>
-      <c r="J4" s="10">
+      <c r="H4" s="11">
         <v>0.5</v>
       </c>
-      <c r="K4" s="10">
+      <c r="I4" s="11">
         <v>0.5</v>
       </c>
-      <c r="L4" s="10">
+      <c r="J4" s="11">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="N4" s="17" t="s">
+      <c r="L4" s="18" t="s">
         <v>876</v>
       </c>
-      <c r="O4" s="10">
+      <c r="M4" s="11">
+        <f>SUM(E7:E9)</f>
+        <v>1</v>
+      </c>
+      <c r="N4" s="11">
+        <f>SUM(F7:F9)</f>
+        <v>1</v>
+      </c>
+      <c r="O4" s="11">
         <f>SUM(G7:G9)</f>
         <v>1</v>
       </c>
-      <c r="P4" s="10">
+      <c r="P4" s="11">
         <f>SUM(H7:H9)</f>
         <v>1</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="Q4" s="11">
         <f>SUM(I7:I9)</f>
         <v>1</v>
       </c>
-      <c r="R4" s="10">
-        <f>SUM(J7:J9)</f>
-        <v>1</v>
-      </c>
-      <c r="S4" s="10">
-        <f>SUM(K7:K9)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19">
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="5" t="s">
+        <v>904</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>905</v>
       </c>
-      <c r="B5" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>906</v>
-      </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="12" t="s">
         <v>669</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>904</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="10">
+      <c r="E5" s="11">
         <v>0</v>
       </c>
-      <c r="H5" s="10">
+      <c r="F5" s="11">
         <v>0.05</v>
       </c>
-      <c r="I5" s="10">
+      <c r="G5" s="11">
         <v>0.1</v>
       </c>
-      <c r="J5" s="19">
+      <c r="H5" s="13">
         <v>0.1</v>
       </c>
-      <c r="K5" s="10">
+      <c r="I5" s="11">
         <v>0.2</v>
       </c>
-      <c r="L5" s="10">
+      <c r="J5" s="11">
         <f t="shared" si="0"/>
         <v>0.45</v>
       </c>
-      <c r="N5" s="17" t="s">
+      <c r="L5" s="18" t="s">
+        <v>906</v>
+      </c>
+      <c r="M5" s="11">
+        <f>SUM(E10:E22)</f>
+        <v>1</v>
+      </c>
+      <c r="N5" s="11">
+        <f>SUM(F10:F22)</f>
+        <v>1</v>
+      </c>
+      <c r="O5" s="11">
+        <f>SUM(G10:G22)</f>
+        <v>1</v>
+      </c>
+      <c r="P5" s="11">
+        <f>SUM(H10:H22)</f>
+        <v>1</v>
+      </c>
+      <c r="Q5" s="11">
+        <f>SUM(I10:I22)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="5" t="s">
         <v>907</v>
       </c>
-      <c r="O5" s="10">
-        <f>SUM(G10:G22)</f>
-        <v>1</v>
-      </c>
-      <c r="P5" s="10">
-        <f>SUM(H10:H22)</f>
-        <v>1</v>
-      </c>
-      <c r="Q5" s="10">
-        <f>SUM(I10:I22)</f>
-        <v>1</v>
-      </c>
-      <c r="R5" s="10">
-        <f>SUM(J10:J22)</f>
-        <v>1</v>
-      </c>
-      <c r="S5" s="10">
-        <f>SUM(K10:K22)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="5" t="s">
-        <v>908</v>
-      </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="12" t="s">
         <v>123</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>906</v>
-      </c>
-      <c r="D6" s="11" t="s">
+        <v>905</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>484</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>904</v>
-      </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="10">
+      <c r="E6" s="11">
         <v>0</v>
       </c>
-      <c r="H6" s="10">
+      <c r="F6" s="11">
         <v>0.05</v>
       </c>
-      <c r="I6" s="10">
+      <c r="G6" s="11">
         <v>0.1</v>
       </c>
-      <c r="J6" s="19">
+      <c r="H6" s="13">
         <v>0.1</v>
       </c>
-      <c r="K6" s="10">
+      <c r="I6" s="11">
         <v>0.2</v>
       </c>
-      <c r="L6" s="10">
+      <c r="J6" s="11">
         <f t="shared" si="0"/>
         <v>0.45</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="L6" s="5" t="s">
+        <v>908</v>
+      </c>
+      <c r="M6" s="11">
+        <f>SUM(E23:E33)</f>
+        <v>1</v>
+      </c>
+      <c r="N6" s="11">
+        <f>SUM(F23:F33)</f>
+        <v>1</v>
+      </c>
+      <c r="O6" s="11">
+        <f>SUM(G23:G33)</f>
+        <v>1</v>
+      </c>
+      <c r="P6" s="11">
+        <f>SUM(H23:H33)</f>
+        <v>1</v>
+      </c>
+      <c r="Q6" s="11">
+        <f>SUM(I23:I33)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="5" t="s">
         <v>909</v>
       </c>
-      <c r="O6" s="10">
-        <f>SUM(G23:G33)</f>
-        <v>1</v>
-      </c>
-      <c r="P6" s="10">
-        <f>SUM(H23:H33)</f>
-        <v>1</v>
-      </c>
-      <c r="Q6" s="10">
-        <f>SUM(I23:I33)</f>
-        <v>1</v>
-      </c>
-      <c r="R6" s="10">
-        <f>SUM(J23:J33)</f>
-        <v>1</v>
-      </c>
-      <c r="S6" s="10">
-        <f>SUM(K23:K33)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" s="5" t="s">
-        <v>910</v>
-      </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="12" t="s">
         <v>876</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="12" t="s">
         <v>669</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>904</v>
-      </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="10">
+      <c r="E7" s="11">
         <v>0</v>
       </c>
-      <c r="H7" s="10">
+      <c r="F7" s="11">
         <v>0.1</v>
       </c>
-      <c r="I7" s="10">
+      <c r="G7" s="11">
         <v>0.2</v>
       </c>
-      <c r="J7" s="10">
+      <c r="H7" s="11">
         <v>0.3</v>
       </c>
-      <c r="K7" s="10">
+      <c r="I7" s="11">
         <v>0.4</v>
       </c>
-      <c r="L7" s="10">
+      <c r="J7" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:10">
       <c r="A8" s="5" t="s">
         <v>876</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="10" t="s">
         <v>876</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="10">
+      <c r="C8" s="9"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="11">
         <v>0.6</v>
       </c>
-      <c r="H8" s="10">
+      <c r="F8" s="11">
         <v>0.6</v>
       </c>
-      <c r="I8" s="10">
+      <c r="G8" s="11">
         <v>0.6</v>
       </c>
-      <c r="J8" s="10">
+      <c r="H8" s="11">
         <v>0.6</v>
       </c>
-      <c r="K8" s="10">
+      <c r="I8" s="11">
         <v>0.6</v>
       </c>
-      <c r="L8" s="10">
+      <c r="J8" s="11">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
-      <c r="A9" s="8" t="s">
-        <v>911</v>
-      </c>
-      <c r="B9" s="11" t="s">
+    <row r="9" spans="1:10">
+      <c r="A9" s="9" t="s">
+        <v>910</v>
+      </c>
+      <c r="B9" s="12" t="s">
         <v>876</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>540</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="12" t="s">
         <v>484</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>904</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="10">
+      <c r="E9" s="11">
         <v>0.4</v>
       </c>
-      <c r="H9" s="10">
+      <c r="F9" s="11">
         <v>0.3</v>
       </c>
-      <c r="I9" s="10">
+      <c r="G9" s="11">
         <v>0.2</v>
       </c>
-      <c r="J9" s="10">
+      <c r="H9" s="11">
         <v>0.1</v>
       </c>
-      <c r="K9" s="10">
+      <c r="I9" s="11">
         <v>0</v>
       </c>
-      <c r="L9" s="10">
+      <c r="J9" s="11">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:10">
       <c r="A10" s="7" t="s">
-        <v>912</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>907</v>
+        <v>911</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>906</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>540</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="12" t="s">
         <v>669</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>904</v>
-      </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="10">
+      <c r="E10" s="11">
         <v>0.1</v>
       </c>
-      <c r="H10" s="10">
+      <c r="F10" s="11">
         <v>0.1</v>
       </c>
-      <c r="I10" s="10">
+      <c r="G10" s="11">
         <v>0.1</v>
       </c>
-      <c r="J10" s="10">
+      <c r="H10" s="11">
         <v>0.1</v>
       </c>
-      <c r="K10" s="10">
+      <c r="I10" s="11">
         <v>0.2</v>
       </c>
-      <c r="L10" s="10">
+      <c r="J10" s="11">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:10">
       <c r="A11" s="7" t="s">
-        <v>913</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>907</v>
+        <v>912</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>906</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>541</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="12" t="s">
         <v>484</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>904</v>
-      </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="10">
+      <c r="E11" s="11">
         <v>0.1</v>
       </c>
-      <c r="H11" s="10">
+      <c r="F11" s="11">
         <v>0.1</v>
       </c>
-      <c r="I11" s="10">
+      <c r="G11" s="11">
         <v>0.1</v>
       </c>
-      <c r="J11" s="10">
+      <c r="H11" s="11">
         <v>0.15</v>
       </c>
-      <c r="K11" s="10">
+      <c r="I11" s="11">
         <v>0.1</v>
       </c>
-      <c r="L11" s="10">
+      <c r="J11" s="11">
         <f t="shared" si="0"/>
         <v>0.55</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:10">
       <c r="A12" s="7" t="s">
-        <v>914</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>907</v>
+        <v>913</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>906</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="12" t="s">
         <v>484</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>904</v>
-      </c>
-      <c r="F12" s="11"/>
-      <c r="G12" s="10">
+      <c r="E12" s="11">
         <v>0.3</v>
       </c>
-      <c r="H12" s="10">
+      <c r="F12" s="11">
         <v>0.2</v>
       </c>
-      <c r="I12" s="10">
+      <c r="G12" s="11">
         <v>0.1</v>
       </c>
-      <c r="J12" s="10">
+      <c r="H12" s="11">
         <v>0</v>
       </c>
-      <c r="K12" s="10">
+      <c r="I12" s="11">
         <v>0</v>
       </c>
-      <c r="L12" s="10">
+      <c r="J12" s="11">
         <f t="shared" si="0"/>
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:10">
       <c r="A13" s="5" t="s">
-        <v>915</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>907</v>
+        <v>914</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>906</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>542</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="12" t="s">
         <v>669</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>904</v>
-      </c>
-      <c r="F13" s="11"/>
-      <c r="G13" s="10">
+      <c r="E13" s="11">
         <v>0.1</v>
       </c>
-      <c r="H13" s="10">
+      <c r="F13" s="11">
         <v>0.15</v>
       </c>
-      <c r="I13" s="10">
+      <c r="G13" s="11">
         <v>0.1</v>
       </c>
-      <c r="J13" s="10">
+      <c r="H13" s="11">
         <v>0.1</v>
       </c>
-      <c r="K13" s="10">
+      <c r="I13" s="11">
         <v>0.1</v>
       </c>
-      <c r="L13" s="10">
+      <c r="J13" s="11">
         <f t="shared" si="0"/>
         <v>0.55</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:10">
       <c r="A14" s="5" t="s">
-        <v>916</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>907</v>
+        <v>915</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>906</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>542</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="12" t="s">
         <v>484</v>
       </c>
-      <c r="E14" s="11" t="s">
-        <v>904</v>
-      </c>
-      <c r="F14" s="11"/>
-      <c r="G14" s="10">
+      <c r="E14" s="11">
         <v>0.2</v>
       </c>
-      <c r="H14" s="10">
+      <c r="F14" s="11">
         <v>0.15</v>
       </c>
-      <c r="I14" s="10">
+      <c r="G14" s="11">
         <v>0.1</v>
       </c>
-      <c r="J14" s="10">
+      <c r="H14" s="11">
         <v>0.15</v>
       </c>
-      <c r="K14" s="10">
+      <c r="I14" s="11">
         <v>0.1</v>
       </c>
-      <c r="L14" s="10">
+      <c r="J14" s="11">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:10">
       <c r="A15" s="7" t="s">
+        <v>916</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>906</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>917</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>907</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>918</v>
-      </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="12" t="s">
         <v>484</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>904</v>
-      </c>
-      <c r="F15" s="11"/>
-      <c r="G15" s="10">
+      <c r="E15" s="11">
         <v>0.1</v>
       </c>
-      <c r="H15" s="10">
+      <c r="F15" s="11">
         <v>0</v>
       </c>
-      <c r="I15" s="10">
+      <c r="G15" s="11">
         <v>0.1</v>
       </c>
-      <c r="J15" s="10">
+      <c r="H15" s="11">
         <v>0.1</v>
       </c>
-      <c r="K15" s="10">
+      <c r="I15" s="11">
         <v>0.1</v>
       </c>
-      <c r="L15" s="10">
+      <c r="J15" s="11">
         <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:10">
       <c r="A16" s="7" t="s">
-        <v>919</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>907</v>
+        <v>918</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>906</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>918</v>
-      </c>
-      <c r="D16" s="11" t="s">
+        <v>917</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>669</v>
       </c>
-      <c r="E16" s="11" t="s">
-        <v>904</v>
-      </c>
-      <c r="F16" s="11"/>
-      <c r="G16" s="10">
+      <c r="E16" s="11">
         <v>0.1</v>
       </c>
-      <c r="H16" s="10">
+      <c r="F16" s="11">
         <v>0.15</v>
       </c>
-      <c r="I16" s="10">
+      <c r="G16" s="11">
         <v>0.1</v>
       </c>
-      <c r="J16" s="19">
+      <c r="H16" s="13">
         <v>0.1</v>
       </c>
-      <c r="K16" s="10">
+      <c r="I16" s="11">
         <v>0.1</v>
       </c>
-      <c r="L16" s="10">
+      <c r="J16" s="11">
         <f t="shared" si="0"/>
         <v>0.55</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:10">
       <c r="A17" s="7" t="s">
-        <v>920</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>907</v>
+        <v>919</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>906</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>780</v>
       </c>
-      <c r="D17" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="E17" s="12" t="s">
-        <v>921</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>922</v>
-      </c>
-      <c r="G17" s="10">
+      <c r="D17" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="E17" s="11">
         <v>0</v>
       </c>
-      <c r="H17" s="10">
+      <c r="F17" s="11">
         <v>0</v>
       </c>
-      <c r="I17" s="10">
+      <c r="G17" s="11">
         <v>0.05</v>
       </c>
-      <c r="J17" s="19">
+      <c r="H17" s="13">
         <v>0.05</v>
       </c>
-      <c r="K17" s="19">
+      <c r="I17" s="13">
         <v>0.05</v>
       </c>
-      <c r="L17" s="10">
+      <c r="J17" s="11">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:10">
       <c r="A18" s="7" t="s">
-        <v>923</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>907</v>
+        <v>920</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>906</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>784</v>
       </c>
-      <c r="D18" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>921</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>922</v>
-      </c>
-      <c r="G18" s="10">
+      <c r="D18" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="E18" s="11">
         <v>0</v>
       </c>
-      <c r="H18" s="10">
+      <c r="F18" s="11">
         <v>0</v>
       </c>
-      <c r="I18" s="10">
+      <c r="G18" s="11">
         <v>0.05</v>
       </c>
-      <c r="J18" s="19">
+      <c r="H18" s="13">
         <v>0.05</v>
       </c>
-      <c r="K18" s="19">
+      <c r="I18" s="13">
         <v>0.05</v>
       </c>
-      <c r="L18" s="10">
+      <c r="J18" s="11">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:10">
       <c r="A19" s="7" t="s">
-        <v>924</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>907</v>
+        <v>921</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>906</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>782</v>
       </c>
-      <c r="D19" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>921</v>
-      </c>
-      <c r="F19" s="11"/>
-      <c r="G19" s="10">
+      <c r="D19" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="E19" s="11">
         <v>0</v>
       </c>
-      <c r="H19" s="10">
+      <c r="F19" s="11">
         <v>0</v>
       </c>
-      <c r="I19" s="10">
+      <c r="G19" s="11">
         <v>0.05</v>
       </c>
-      <c r="J19" s="19">
+      <c r="H19" s="13">
         <v>0.05</v>
       </c>
-      <c r="K19" s="19">
+      <c r="I19" s="13">
         <v>0.05</v>
       </c>
-      <c r="L19" s="10">
+      <c r="J19" s="11">
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:10">
       <c r="A20" s="7" t="s">
-        <v>925</v>
-      </c>
-      <c r="B20" s="11" t="s">
-        <v>907</v>
+        <v>922</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>906</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>926</v>
-      </c>
-      <c r="D20" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="E20" s="12" t="s">
-        <v>921</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>922</v>
-      </c>
-      <c r="G20" s="10">
+        <v>923</v>
+      </c>
+      <c r="D20" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="E20" s="11">
         <v>0</v>
       </c>
-      <c r="H20" s="10">
+      <c r="F20" s="11">
         <v>0.05</v>
       </c>
-      <c r="I20" s="10">
+      <c r="G20" s="11">
         <v>0.05</v>
       </c>
-      <c r="J20" s="19">
+      <c r="H20" s="13">
         <v>0.05</v>
       </c>
-      <c r="K20" s="19">
+      <c r="I20" s="13">
         <v>0.05</v>
       </c>
-      <c r="L20" s="10">
+      <c r="J20" s="11">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:10">
       <c r="A21" s="7" t="s">
-        <v>927</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>907</v>
+        <v>924</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>906</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>928</v>
-      </c>
-      <c r="D21" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>921</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>922</v>
-      </c>
-      <c r="G21" s="10">
+        <v>925</v>
+      </c>
+      <c r="D21" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="E21" s="11">
         <v>0</v>
       </c>
-      <c r="H21" s="10">
+      <c r="F21" s="11">
         <v>0.05</v>
       </c>
-      <c r="I21" s="10">
+      <c r="G21" s="11">
         <v>0.05</v>
       </c>
-      <c r="J21" s="19">
+      <c r="H21" s="13">
         <v>0.05</v>
       </c>
-      <c r="K21" s="19">
+      <c r="I21" s="13">
         <v>0.05</v>
       </c>
-      <c r="L21" s="10">
+      <c r="J21" s="11">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:10">
       <c r="A22" s="7" t="s">
-        <v>929</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>907</v>
+        <v>926</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>906</v>
       </c>
       <c r="C22" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="E22" s="11">
+        <v>0</v>
+      </c>
+      <c r="F22" s="11">
         <v>0.05</v>
       </c>
-      <c r="E22" s="12" t="s">
-        <v>921</v>
-      </c>
-      <c r="F22" s="11" t="s">
-        <v>922</v>
-      </c>
-      <c r="G22" s="10">
-        <v>0</v>
-      </c>
-      <c r="H22" s="10">
+      <c r="G22" s="11">
         <v>0.05</v>
       </c>
-      <c r="I22" s="10">
+      <c r="H22" s="13">
         <v>0.05</v>
       </c>
-      <c r="J22" s="19">
+      <c r="I22" s="13">
         <v>0.05</v>
       </c>
-      <c r="K22" s="19">
-        <v>0.05</v>
-      </c>
-      <c r="L22" s="10">
+      <c r="J22" s="11">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:10">
       <c r="A23" s="5" t="s">
         <v>875</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>909</v>
-      </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="10">
-        <v>1</v>
-      </c>
-      <c r="H23" s="10">
+      <c r="B23" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="D23" s="15"/>
+      <c r="E23" s="11">
+        <v>1</v>
+      </c>
+      <c r="F23" s="11">
         <v>0.3</v>
       </c>
-      <c r="I23" s="10">
+      <c r="G23" s="11">
         <v>0.25</v>
       </c>
-      <c r="J23" s="19">
+      <c r="H23" s="13">
         <v>0.2</v>
       </c>
-      <c r="K23" s="10">
+      <c r="I23" s="11">
         <v>0.2</v>
       </c>
-      <c r="L23" s="10"/>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="J23" s="11"/>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24" s="5" t="s">
         <v>883</v>
       </c>
-      <c r="B24" s="9" t="s">
-        <v>909</v>
-      </c>
-      <c r="G24" s="10">
+      <c r="B24" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E24" s="11">
         <v>0</v>
       </c>
-      <c r="H24" s="10">
+      <c r="F24" s="11">
         <v>0.3</v>
       </c>
-      <c r="I24" s="10">
+      <c r="G24" s="11">
         <v>0.25</v>
       </c>
-      <c r="J24" s="19">
+      <c r="H24" s="13">
         <v>0.2</v>
       </c>
-      <c r="K24" s="10">
+      <c r="I24" s="11">
         <v>0.2</v>
       </c>
-      <c r="L24" s="10"/>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="J24" s="11"/>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="5" t="s">
         <v>880</v>
       </c>
-      <c r="B25" s="9" t="s">
-        <v>909</v>
-      </c>
-      <c r="G25" s="10">
+      <c r="B25" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E25" s="11">
         <v>0</v>
       </c>
-      <c r="H25" s="10">
+      <c r="F25" s="11">
         <v>0.2</v>
       </c>
-      <c r="I25" s="10">
+      <c r="G25" s="11">
         <v>0.2</v>
       </c>
-      <c r="J25" s="10">
+      <c r="H25" s="11">
         <v>0.1</v>
       </c>
-      <c r="K25" s="10">
+      <c r="I25" s="11">
         <v>0.1</v>
       </c>
-      <c r="L25" s="10"/>
-      <c r="O25" s="7"/>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="J25" s="11"/>
+      <c r="M25" s="7"/>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="7" t="s">
         <v>879</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>909</v>
-      </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="15">
+      <c r="B26" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E26" s="16">
         <v>0</v>
       </c>
-      <c r="H26" s="10">
+      <c r="F26" s="11">
         <v>0.1</v>
       </c>
-      <c r="I26" s="10">
+      <c r="G26" s="11">
         <v>0.1</v>
       </c>
-      <c r="J26" s="10">
+      <c r="H26" s="11">
         <v>0.1</v>
       </c>
-      <c r="K26" s="10">
+      <c r="I26" s="11">
         <v>0.1</v>
       </c>
-      <c r="L26" s="10"/>
-      <c r="O26"/>
-    </row>
-    <row r="27" spans="1:12">
-      <c r="A27" s="8" t="s">
+      <c r="J26" s="11"/>
+      <c r="M26"/>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27" s="9" t="s">
         <v>887</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>909</v>
-      </c>
-      <c r="G27" s="10">
+      <c r="B27" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E27" s="11">
         <v>0</v>
       </c>
-      <c r="H27" s="10">
+      <c r="F27" s="11">
         <v>0.1</v>
       </c>
-      <c r="I27" s="10">
+      <c r="G27" s="11">
         <v>0.1</v>
       </c>
-      <c r="J27" s="10">
+      <c r="H27" s="11">
         <v>0.1</v>
       </c>
-      <c r="K27" s="10">
+      <c r="I27" s="11">
         <v>0.1</v>
       </c>
-      <c r="L27" s="10"/>
-    </row>
-    <row r="28" spans="1:12">
+      <c r="J27" s="11"/>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28" s="7" t="s">
         <v>889</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>909</v>
-      </c>
-      <c r="G28" s="10">
+      <c r="B28" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E28" s="11">
         <v>0</v>
       </c>
-      <c r="H28" s="10">
+      <c r="F28" s="11">
         <v>0</v>
       </c>
-      <c r="I28" s="10">
+      <c r="G28" s="11">
         <v>0.1</v>
       </c>
-      <c r="J28" s="10">
+      <c r="H28" s="11">
         <v>0.1</v>
       </c>
-      <c r="K28" s="10">
+      <c r="I28" s="11">
         <v>0.1</v>
       </c>
-      <c r="L28" s="10"/>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="J28" s="11"/>
+    </row>
+    <row r="29" spans="1:13">
       <c r="A29" s="5" t="s">
         <v>893</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>909</v>
-      </c>
-      <c r="G29" s="10">
+      <c r="B29" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E29" s="11">
         <v>0</v>
       </c>
-      <c r="H29" s="10">
+      <c r="F29" s="11">
         <v>0</v>
       </c>
-      <c r="I29" s="10">
+      <c r="G29" s="11">
         <v>0</v>
       </c>
-      <c r="J29" s="10">
+      <c r="H29" s="11">
         <v>0.1</v>
       </c>
-      <c r="K29" s="10">
+      <c r="I29" s="11">
         <v>0.1</v>
       </c>
-      <c r="L29" s="10"/>
-      <c r="O29"/>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="J29" s="11"/>
+      <c r="M29"/>
+    </row>
+    <row r="30" spans="1:13">
       <c r="A30" s="7" t="s">
         <v>894</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>909</v>
-      </c>
-      <c r="G30" s="10">
+      <c r="B30" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E30" s="11">
         <v>0</v>
       </c>
-      <c r="H30" s="10">
+      <c r="F30" s="11">
         <v>0</v>
       </c>
-      <c r="I30" s="10">
+      <c r="G30" s="11">
         <v>0</v>
       </c>
-      <c r="J30" s="10">
+      <c r="H30" s="11">
         <v>0.1</v>
       </c>
-      <c r="K30" s="10">
+      <c r="I30" s="11">
         <v>0.1</v>
       </c>
-      <c r="L30" s="10"/>
-      <c r="O30"/>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="J30" s="11"/>
+      <c r="M30"/>
+    </row>
+    <row r="31" spans="1:13">
       <c r="A31" s="5" t="s">
         <v>898</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>909</v>
-      </c>
-      <c r="G31" s="10">
+      <c r="B31" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E31" s="11">
         <v>0</v>
       </c>
-      <c r="H31" s="10">
+      <c r="F31" s="11">
         <v>0</v>
       </c>
-      <c r="I31" s="10">
+      <c r="G31" s="11">
         <v>0</v>
       </c>
-      <c r="J31" s="10">
+      <c r="H31" s="11">
         <v>0</v>
       </c>
-      <c r="K31" s="10">
+      <c r="I31" s="11">
         <v>0</v>
       </c>
-      <c r="L31" s="10"/>
-      <c r="O31"/>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="J31" s="11"/>
+      <c r="M31"/>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32" s="5" t="s">
         <v>877</v>
       </c>
-      <c r="B32" s="9" t="s">
-        <v>909</v>
-      </c>
-      <c r="G32" s="10">
+      <c r="B32" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E32" s="11">
         <v>0</v>
       </c>
-      <c r="H32" s="10">
+      <c r="F32" s="11">
         <v>0</v>
       </c>
-      <c r="I32" s="10">
+      <c r="G32" s="11">
         <v>0</v>
       </c>
-      <c r="J32" s="10">
+      <c r="H32" s="11">
         <v>0</v>
       </c>
-      <c r="K32" s="10">
+      <c r="I32" s="11">
         <v>0</v>
       </c>
-      <c r="L32" s="10"/>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="J32" s="11"/>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B33" s="9" t="s">
-        <v>909</v>
-      </c>
-      <c r="G33" s="10">
+      <c r="B33" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E33" s="11">
         <v>0</v>
       </c>
-      <c r="H33" s="10">
+      <c r="F33" s="11">
         <v>0</v>
       </c>
-      <c r="I33" s="10">
+      <c r="G33" s="11">
         <v>0</v>
       </c>
-      <c r="J33" s="10">
+      <c r="H33" s="11">
         <v>0</v>
       </c>
-      <c r="K33" s="10">
+      <c r="I33" s="11">
         <v>0</v>
       </c>
-      <c r="L33" s="10"/>
-      <c r="O33" s="8"/>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="J33" s="11"/>
+      <c r="M33" s="9"/>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="5" t="s">
         <v>882</v>
       </c>
-      <c r="B34" s="9" t="s">
-        <v>909</v>
-      </c>
-      <c r="G34" s="16" t="s">
-        <v>930</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>930</v>
-      </c>
-      <c r="I34" s="16" t="s">
-        <v>930</v>
-      </c>
-      <c r="J34" s="16" t="s">
-        <v>930</v>
-      </c>
-      <c r="K34" s="16" t="s">
-        <v>930</v>
-      </c>
-      <c r="O34"/>
-    </row>
-    <row r="36" spans="15:15">
-      <c r="O36"/>
-    </row>
-    <row r="37" spans="15:15">
-      <c r="O37" s="7"/>
-    </row>
-    <row r="38" spans="15:15">
-      <c r="O38"/>
-    </row>
-    <row r="39" spans="15:15">
-      <c r="O39"/>
-    </row>
-    <row r="40" spans="15:15">
-      <c r="O40"/>
-    </row>
-    <row r="41" spans="15:15">
-      <c r="O41"/>
+      <c r="B34" s="10" t="s">
+        <v>908</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>927</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>927</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>927</v>
+      </c>
+      <c r="H34" s="17" t="s">
+        <v>927</v>
+      </c>
+      <c r="I34" s="17" t="s">
+        <v>927</v>
+      </c>
+      <c r="M34"/>
+    </row>
+    <row r="36" spans="13:13">
+      <c r="M36"/>
+    </row>
+    <row r="37" spans="13:13">
+      <c r="M37" s="7"/>
+    </row>
+    <row r="38" spans="13:13">
+      <c r="M38"/>
+    </row>
+    <row r="39" spans="13:13">
+      <c r="M39"/>
+    </row>
+    <row r="40" spans="13:13">
+      <c r="M40"/>
+    </row>
+    <row r="41" spans="13:13">
+      <c r="M41"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="O1:S1"/>
-    <mergeCell ref="D2:E2"/>
+  <mergeCells count="6">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:I1"/>
+    <mergeCell ref="M1:Q1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="J1:J2"/>
   </mergeCells>
-  <conditionalFormatting sqref="O3:S6">
+  <conditionalFormatting sqref="M3:Q6">
     <cfRule type="expression" dxfId="0" priority="2">
-      <formula>$O$3&gt;1</formula>
+      <formula>$M$3&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -15583,19 +15476,19 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="3" t="s">
-        <v>931</v>
+        <v>928</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3" t="s">
-        <v>932</v>
+        <v>929</v>
       </c>
       <c r="D1" s="3"/>
       <c r="E1" s="3" t="s">
-        <v>933</v>
+        <v>930</v>
       </c>
       <c r="F1" s="3"/>
       <c r="J1" s="3" t="s">
-        <v>934</v>
+        <v>931</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -15610,13 +15503,13 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="J2" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="K2" t="s">
-        <v>936</v>
+        <v>933</v>
       </c>
       <c r="L2" t="s">
-        <v>937</v>
+        <v>934</v>
       </c>
       <c r="M2" t="s">
         <v>184</v>
@@ -15627,22 +15520,22 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="3" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>938</v>
+        <v>935</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>939</v>
+        <v>936</v>
       </c>
       <c r="I3" t="s">
         <v>131</v>
@@ -15650,13 +15543,13 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>940</v>
+        <v>937</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>131</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
       <c r="I4" t="s">
         <v>134</v>
@@ -15664,13 +15557,13 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
       <c r="B5" t="s">
         <v>127</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>943</v>
+        <v>940</v>
       </c>
       <c r="I5" t="s">
         <v>146</v>
@@ -15678,13 +15571,13 @@
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="1" t="s">
-        <v>944</v>
+        <v>941</v>
       </c>
       <c r="B6" t="s">
-        <v>945</v>
+        <v>942</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>946</v>
+        <v>943</v>
       </c>
       <c r="I6" t="s">
         <v>143</v>
@@ -15692,94 +15585,94 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="B7" t="s">
+        <v>945</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="I7" t="s">
         <v>947</v>
-      </c>
-      <c r="B7" t="s">
-        <v>948</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>949</v>
-      </c>
-      <c r="I7" t="s">
-        <v>950</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>951</v>
+        <v>948</v>
       </c>
       <c r="B8" t="s">
-        <v>952</v>
+        <v>949</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>953</v>
+        <v>950</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
-        <v>954</v>
+        <v>951</v>
       </c>
       <c r="B9" t="s">
-        <v>955</v>
+        <v>952</v>
       </c>
       <c r="C9" t="s">
-        <v>956</v>
+        <v>953</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>957</v>
+        <v>954</v>
       </c>
       <c r="B10" t="s">
-        <v>958</v>
+        <v>955</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>959</v>
+        <v>956</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>960</v>
+        <v>957</v>
       </c>
       <c r="B11" t="s">
-        <v>961</v>
+        <v>958</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>962</v>
+        <v>959</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>963</v>
+        <v>960</v>
       </c>
       <c r="B12" t="s">
-        <v>964</v>
+        <v>961</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>965</v>
+        <v>962</v>
       </c>
       <c r="B13" t="s">
-        <v>966</v>
+        <v>963</v>
       </c>
     </row>
     <row r="14" spans="1:1">
       <c r="A14" t="s">
-        <v>967</v>
+        <v>964</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>968</v>
+        <v>965</v>
       </c>
       <c r="B15" t="s">
-        <v>969</v>
+        <v>966</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>970</v>
+        <v>967</v>
       </c>
       <c r="B16" t="s">
         <v>133</v>
@@ -15787,73 +15680,73 @@
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>971</v>
+        <v>968</v>
       </c>
       <c r="B17" t="s">
-        <v>972</v>
+        <v>969</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>973</v>
+        <v>970</v>
       </c>
       <c r="B18" t="s">
-        <v>974</v>
+        <v>971</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
-        <v>975</v>
+        <v>972</v>
       </c>
       <c r="B19" t="s">
-        <v>976</v>
+        <v>973</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
-        <v>977</v>
+        <v>974</v>
       </c>
       <c r="B20" t="s">
-        <v>978</v>
+        <v>975</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
-        <v>979</v>
+        <v>976</v>
       </c>
       <c r="B21" t="s">
-        <v>980</v>
+        <v>977</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
-        <v>981</v>
+        <v>978</v>
       </c>
       <c r="B22" t="s">
-        <v>982</v>
+        <v>979</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>983</v>
+        <v>980</v>
       </c>
       <c r="B23" t="s">
-        <v>984</v>
+        <v>981</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" t="s">
-        <v>985</v>
+        <v>982</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" t="s">
-        <v>950</v>
+        <v>947</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" t="s">
-        <v>986</v>
+        <v>983</v>
       </c>
     </row>
   </sheetData>
@@ -15885,19 +15778,19 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>987</v>
+        <v>984</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>988</v>
+        <v>985</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>989</v>
+        <v>986</v>
       </c>
       <c r="D1" s="1"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>990</v>
+        <v>987</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -15906,12 +15799,12 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>991</v>
+        <v>988</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>992</v>
+        <v>989</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -15920,12 +15813,12 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>993</v>
+        <v>990</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>994</v>
+        <v>991</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -15934,12 +15827,12 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>995</v>
+        <v>992</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>996</v>
+        <v>993</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -15948,12 +15841,12 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>997</v>
+        <v>994</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>998</v>
+        <v>995</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -15962,12 +15855,12 @@
         <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>999</v>
+        <v>996</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>1000</v>
+        <v>997</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -15976,12 +15869,12 @@
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>1001</v>
+        <v>998</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -15990,12 +15883,12 @@
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -16004,12 +15897,12 @@
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
       <c r="B10">
         <v>3</v>
@@ -16018,12 +15911,12 @@
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>1008</v>
+        <v>1005</v>
       </c>
       <c r="B11">
         <v>4</v>
@@ -16032,12 +15925,12 @@
         <v>1</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>1009</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>1010</v>
+        <v>1007</v>
       </c>
       <c r="B12">
         <v>5</v>
@@ -16046,12 +15939,12 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>1011</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="B13">
         <v>5</v>
@@ -16060,12 +15953,12 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="B14">
         <v>5</v>
@@ -16074,12 +15967,12 @@
         <v>3</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>1015</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>1016</v>
+        <v>1013</v>
       </c>
       <c r="B15">
         <v>5</v>
@@ -16088,12 +15981,12 @@
         <v>4</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>1017</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>1018</v>
+        <v>1015</v>
       </c>
       <c r="B16">
         <v>6</v>
@@ -16102,12 +15995,12 @@
         <v>1</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>1019</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="B17">
         <v>7</v>
@@ -16116,12 +16009,12 @@
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="B18">
         <v>8</v>
@@ -16130,12 +16023,12 @@
         <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
     </row>
     <row r="19" ht="15.75" spans="1:4">
       <c r="A19" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="B19">
         <v>9</v>
@@ -16144,12 +16037,12 @@
         <v>1</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="B20">
         <v>10</v>
@@ -16158,12 +16051,12 @@
         <v>1</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="B21">
         <v>11</v>
@@ -16172,12 +16065,12 @@
         <v>1</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="B22">
         <v>12</v>
@@ -16186,12 +16079,12 @@
         <v>1</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="B23">
         <v>13</v>
@@ -16200,12 +16093,12 @@
         <v>1</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="B24">
         <v>14</v>
@@ -16214,12 +16107,12 @@
         <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>1036</v>
+        <v>1033</v>
       </c>
       <c r="B25">
         <v>15</v>
@@ -16228,12 +16121,12 @@
         <v>1</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>1038</v>
+        <v>1035</v>
       </c>
       <c r="B26">
         <v>16</v>
@@ -16242,12 +16135,12 @@
         <v>1</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>1039</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>1040</v>
+        <v>1037</v>
       </c>
       <c r="B27">
         <v>17</v>
@@ -16256,12 +16149,12 @@
         <v>1</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>1041</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>1042</v>
+        <v>1039</v>
       </c>
       <c r="B28">
         <v>17</v>
@@ -16270,12 +16163,12 @@
         <v>2</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>1043</v>
+        <v>1040</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>1044</v>
+        <v>1041</v>
       </c>
       <c r="B29">
         <v>17</v>
@@ -16284,12 +16177,12 @@
         <v>3</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>1045</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>1046</v>
+        <v>1043</v>
       </c>
       <c r="B30">
         <v>17</v>
@@ -16298,12 +16191,12 @@
         <v>4</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="B31">
         <v>17</v>
@@ -16312,12 +16205,12 @@
         <v>5</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="B32">
         <v>18</v>
@@ -16326,12 +16219,12 @@
         <v>1</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="B33">
         <v>18</v>
@@ -16340,12 +16233,12 @@
         <v>2</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="B34">
         <v>18</v>
@@ -16354,12 +16247,12 @@
         <v>3</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="B35">
         <v>18</v>
@@ -16368,12 +16261,12 @@
         <v>4</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="1" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -16381,7 +16274,7 @@
         <v>1</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -16389,7 +16282,7 @@
         <v>2</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
     </row>
   </sheetData>
@@ -26201,16 +26094,16 @@
       <c r="C3" t="s">
         <v>545</v>
       </c>
-      <c r="D3" s="11">
-        <v>1</v>
-      </c>
-      <c r="E3" s="17">
+      <c r="D3" s="12">
+        <v>1</v>
+      </c>
+      <c r="E3" s="18">
         <v>4</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="18">
         <v>4</v>
       </c>
-      <c r="G3" s="11">
+      <c r="G3" s="12">
         <v>3</v>
       </c>
       <c r="H3" s="55">
@@ -26247,16 +26140,16 @@
       <c r="C4" t="s">
         <v>549</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="12">
         <v>4</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="12">
         <v>3</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="12">
         <v>3</v>
       </c>
-      <c r="G4" s="17">
+      <c r="G4" s="18">
         <v>2</v>
       </c>
       <c r="H4" s="55">
@@ -26291,16 +26184,16 @@
       <c r="C5" t="s">
         <v>551</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="12">
         <v>2</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="18">
         <v>6</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="12">
         <v>3</v>
       </c>
-      <c r="G5" s="11">
+      <c r="G5" s="12">
         <v>1</v>
       </c>
       <c r="H5" s="55">
@@ -26337,16 +26230,16 @@
       <c r="C6" t="s">
         <v>555</v>
       </c>
-      <c r="D6" s="11">
-        <v>1</v>
-      </c>
-      <c r="E6" s="11">
-        <v>1</v>
-      </c>
-      <c r="F6" s="11">
+      <c r="D6" s="12">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12">
+        <v>1</v>
+      </c>
+      <c r="F6" s="12">
         <v>4</v>
       </c>
-      <c r="G6" s="17">
+      <c r="G6" s="18">
         <v>6</v>
       </c>
       <c r="H6" s="55">
@@ -26381,16 +26274,16 @@
       <c r="C7" t="s">
         <v>558</v>
       </c>
-      <c r="D7" s="11">
+      <c r="D7" s="12">
         <v>4</v>
       </c>
-      <c r="E7" s="11">
-        <v>1</v>
-      </c>
-      <c r="F7" s="17">
+      <c r="E7" s="12">
+        <v>1</v>
+      </c>
+      <c r="F7" s="18">
         <v>3</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="12">
         <v>4</v>
       </c>
       <c r="H7" s="55">
@@ -26425,16 +26318,16 @@
       <c r="C8" t="s">
         <v>560</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="12">
         <v>3</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="18">
         <v>5</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="12">
         <v>2</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="12">
         <v>2</v>
       </c>
       <c r="H8" s="55">
@@ -26471,16 +26364,16 @@
       <c r="C9" t="s">
         <v>563</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="12">
         <v>6</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="12">
         <v>2</v>
       </c>
-      <c r="F9" s="11">
-        <v>1</v>
-      </c>
-      <c r="G9" s="11">
+      <c r="F9" s="12">
+        <v>1</v>
+      </c>
+      <c r="G9" s="12">
         <v>3</v>
       </c>
       <c r="H9" s="55">
@@ -26512,16 +26405,16 @@
       <c r="B10" t="s">
         <v>565</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="12">
         <v>3</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="12">
         <v>2</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="18">
         <v>4</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="18">
         <v>3</v>
       </c>
       <c r="H10" s="55">

</xml_diff>

<commit_message>
<Feature, Bugfix> Explosion, Skills
Updated explosion prefab to use fewer particles.
Explosion now has smoke.
Sickness is now area of effect.
Added sickness grenade.
Sniper no longer fires hundreds of shots.
Martyr explodes properly.
Rebalanced weapons.
Heart beat now plays correctly.
Added MagazineEffect particles for passive skills.
Added readytouse particles for skills.
Inscribing weapons now affects combat.
Updated medic behaviour (still needs work).
Added push behaviour to mountain (still needs work).
Warlords can no longer generate warlords.
Grenade now detonates when near target.
Shot now selects random condition to apply if multiple conditions can be
triggered.
Increased adrenaline gain rate.
Reduced dash cost.
Changed swarm to create area of effect burst.
Fixed bug where armour break clips wouldn't load.
Fixed bug where accessory and inscription templates couldn't be loaded.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="4" activeTab="4"/>
+    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="2" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -11998,8 +11998,8 @@
   <sheetPr/>
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -12133,11 +12133,11 @@
         <v>803</v>
       </c>
       <c r="B4">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C24" si="4">B4+500</f>
-        <v>600</v>
+        <v>575</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -12159,19 +12159,19 @@
       </c>
       <c r="J4" s="35">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K4" s="35">
         <f t="shared" si="1"/>
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L4" s="35">
         <f t="shared" si="2"/>
-        <v>0.909090909090909</v>
+        <v>0.681818181818182</v>
       </c>
       <c r="M4" s="35">
         <f t="shared" si="3"/>
-        <v>5.45454545454545</v>
+        <v>5.22727272727273</v>
       </c>
       <c r="O4" t="s">
         <v>804</v>
@@ -12182,11 +12182,11 @@
         <v>805</v>
       </c>
       <c r="B5">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="C5">
         <f t="shared" si="4"/>
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -12208,19 +12208,19 @@
       </c>
       <c r="J5" s="35">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K5" s="35">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L5" s="35">
         <f t="shared" si="2"/>
-        <v>2.72727272727273</v>
+        <v>2.27272727272727</v>
       </c>
       <c r="M5" s="35">
         <f t="shared" si="3"/>
-        <v>7.27272727272727</v>
+        <v>6.81818181818182</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>807</v>
@@ -12231,11 +12231,11 @@
         <v>808</v>
       </c>
       <c r="B6">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C6">
         <f t="shared" si="4"/>
-        <v>700</v>
+        <v>650</v>
       </c>
       <c r="D6">
         <v>4</v>
@@ -12257,19 +12257,19 @@
       </c>
       <c r="J6" s="35">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K6" s="35">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L6" s="35">
         <f t="shared" si="2"/>
-        <v>1.81818181818182</v>
+        <v>1.36363636363636</v>
       </c>
       <c r="M6" s="35">
         <f t="shared" si="3"/>
-        <v>6.36363636363636</v>
+        <v>5.90909090909091</v>
       </c>
       <c r="O6" t="s">
         <v>810</v>
@@ -12280,11 +12280,11 @@
         <v>811</v>
       </c>
       <c r="B7">
-        <v>400</v>
+        <v>300</v>
       </c>
       <c r="C7">
         <f t="shared" si="4"/>
-        <v>900</v>
+        <v>800</v>
       </c>
       <c r="D7">
         <v>4</v>
@@ -12306,19 +12306,19 @@
       </c>
       <c r="J7" s="35">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="K7" s="35">
         <f t="shared" si="1"/>
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="L7" s="35">
         <f t="shared" si="2"/>
-        <v>3.63636363636364</v>
+        <v>2.72727272727273</v>
       </c>
       <c r="M7" s="35">
         <f t="shared" si="3"/>
-        <v>8.18181818181818</v>
+        <v>7.27272727272727</v>
       </c>
       <c r="O7" t="s">
         <v>813</v>
@@ -12329,11 +12329,11 @@
         <v>814</v>
       </c>
       <c r="B8">
-        <v>600</v>
+        <v>400</v>
       </c>
       <c r="C8">
         <f t="shared" si="4"/>
-        <v>1100</v>
+        <v>900</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -12355,19 +12355,19 @@
       </c>
       <c r="J8" s="35">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="K8" s="35">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="L8" s="35">
         <f t="shared" si="2"/>
-        <v>5.45454545454545</v>
+        <v>3.63636363636364</v>
       </c>
       <c r="M8" s="35">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>8.18181818181818</v>
       </c>
       <c r="O8" t="s">
         <v>815</v>
@@ -12378,11 +12378,11 @@
         <v>816</v>
       </c>
       <c r="B9">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <f t="shared" si="4"/>
-        <v>550</v>
+        <v>530</v>
       </c>
       <c r="D9">
         <v>10</v>
@@ -12404,19 +12404,19 @@
       </c>
       <c r="J9" s="35">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="K9" s="35">
         <f t="shared" si="1"/>
-        <v>22</v>
+        <v>21.2</v>
       </c>
       <c r="L9" s="35">
         <f t="shared" si="2"/>
-        <v>0.454545454545455</v>
+        <v>0.272727272727273</v>
       </c>
       <c r="M9" s="35">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>4.81818181818182</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>817</v>
@@ -12433,11 +12433,11 @@
         <v>820</v>
       </c>
       <c r="B10">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C10">
         <f t="shared" si="4"/>
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -12459,19 +12459,19 @@
       </c>
       <c r="J10" s="35">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K10" s="35">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L10" s="35">
         <f t="shared" si="2"/>
-        <v>2.72727272727273</v>
+        <v>1.81818181818182</v>
       </c>
       <c r="M10" s="35">
         <f t="shared" si="3"/>
-        <v>7.27272727272727</v>
+        <v>6.36363636363636</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>821</v>
@@ -12561,11 +12561,11 @@
         <v>826</v>
       </c>
       <c r="B12" s="34">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="C12" s="34">
         <f t="shared" si="4"/>
-        <v>800</v>
+        <v>750</v>
       </c>
       <c r="D12" s="34">
         <v>3</v>
@@ -12587,19 +12587,19 @@
       </c>
       <c r="J12" s="36">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="K12" s="36">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L12" s="36">
         <f t="shared" si="2"/>
-        <v>2.72727272727273</v>
+        <v>2.27272727272727</v>
       </c>
       <c r="M12" s="36">
         <f t="shared" si="3"/>
-        <v>7.27272727272727</v>
+        <v>6.81818181818182</v>
       </c>
       <c r="O12" t="s">
         <v>828</v>
@@ -12625,11 +12625,11 @@
         <v>829</v>
       </c>
       <c r="B13" s="34">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="C13" s="34">
         <f t="shared" si="4"/>
-        <v>800</v>
+        <v>700</v>
       </c>
       <c r="D13" s="34">
         <v>5</v>
@@ -12651,19 +12651,19 @@
       </c>
       <c r="J13" s="36">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="K13" s="36">
         <f t="shared" si="1"/>
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="L13" s="36">
         <f t="shared" si="2"/>
-        <v>2.72727272727273</v>
+        <v>1.81818181818182</v>
       </c>
       <c r="M13" s="36">
         <f t="shared" si="3"/>
-        <v>7.27272727272727</v>
+        <v>6.36363636363636</v>
       </c>
       <c r="O13" t="s">
         <v>830</v>
@@ -12689,11 +12689,11 @@
         <v>831</v>
       </c>
       <c r="B14" s="34">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C14" s="34">
         <f t="shared" si="4"/>
-        <v>700</v>
+        <v>650</v>
       </c>
       <c r="D14" s="34">
         <v>5</v>
@@ -12715,19 +12715,19 @@
       </c>
       <c r="J14" s="36">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K14" s="36">
         <f t="shared" si="1"/>
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="L14" s="36">
         <f t="shared" si="2"/>
-        <v>1.81818181818182</v>
+        <v>1.36363636363636</v>
       </c>
       <c r="M14" s="36">
         <f t="shared" si="3"/>
-        <v>6.36363636363636</v>
+        <v>5.90909090909091</v>
       </c>
       <c r="O14" t="s">
         <v>833</v>
@@ -20755,7 +20755,7 @@
   <dimension ref="A1:Y38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R30" sqref="R30"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -20864,26 +20864,26 @@
         <v>23</v>
       </c>
       <c r="D3" s="128">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E3" s="129">
         <v>3</v>
       </c>
       <c r="F3" s="129">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
       <c r="G3" s="130">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="H3" s="131">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="I3" s="129">
         <v>10</v>
       </c>
       <c r="J3" s="158">
         <f>D3*1</f>
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K3" s="158">
         <f>I3/E3</f>
@@ -20891,19 +20891,19 @@
       </c>
       <c r="L3" s="158">
         <f>K3+F3</f>
-        <v>3.83333333333333</v>
+        <v>4.18333333333333</v>
       </c>
       <c r="M3" s="158">
         <f>J3*I3</f>
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="N3" s="159">
         <f>M3/L3</f>
-        <v>49.5652173913044</v>
+        <v>50.199203187251</v>
       </c>
       <c r="P3">
         <f>(J3/E3)/200</f>
-        <v>0.0316666666666667</v>
+        <v>0.035</v>
       </c>
       <c r="R3" t="s">
         <v>102</v>
@@ -20918,46 +20918,46 @@
         <v>24</v>
       </c>
       <c r="D4" s="133">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="E4" s="134">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F4" s="134">
-        <v>0.5</v>
+        <v>0.7</v>
       </c>
       <c r="G4" s="135">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H4" s="136">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="I4" s="134">
         <v>12</v>
       </c>
       <c r="J4" s="158">
-        <f>D4*2</f>
-        <v>14</v>
+        <f>D4</f>
+        <v>13</v>
       </c>
       <c r="K4" s="158">
         <f t="shared" ref="K4:K17" si="0">I4/E4</f>
-        <v>3</v>
+        <v>2.4</v>
       </c>
       <c r="L4" s="158">
         <f t="shared" ref="L4:L17" si="1">K4+F4</f>
-        <v>3.5</v>
+        <v>3.1</v>
       </c>
       <c r="M4" s="158">
         <f t="shared" ref="M4:M17" si="2">J4*I4</f>
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="N4" s="159">
         <f t="shared" ref="N4:N17" si="3">M4/L4</f>
-        <v>48</v>
+        <v>50.3225806451613</v>
       </c>
       <c r="P4">
         <f t="shared" ref="P4:P17" si="4">(J4/E4)/200</f>
-        <v>0.0175</v>
+        <v>0.013</v>
       </c>
       <c r="R4" t="s">
         <v>103</v>
@@ -20981,7 +20981,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="141">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="H5" s="142">
         <v>90</v>
@@ -21042,7 +21042,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="143">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="H6" s="136">
         <v>20</v>
@@ -21102,7 +21102,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="135">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="H7" s="136">
         <v>0</v>
@@ -21149,7 +21149,7 @@
         <v>34</v>
       </c>
       <c r="D8" s="139">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E8" s="140">
         <v>1</v>
@@ -21158,7 +21158,7 @@
         <v>5</v>
       </c>
       <c r="G8" s="141">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="H8" s="142">
         <v>20</v>
@@ -21168,7 +21168,7 @@
       </c>
       <c r="J8" s="160">
         <f t="shared" si="5"/>
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="K8" s="160">
         <f t="shared" si="0"/>
@@ -21180,15 +21180,15 @@
       </c>
       <c r="M8" s="160">
         <f t="shared" si="2"/>
-        <v>540</v>
+        <v>552</v>
       </c>
       <c r="N8" s="161">
         <f t="shared" si="3"/>
-        <v>49.0909090909091</v>
+        <v>50.1818181818182</v>
       </c>
       <c r="P8">
         <f t="shared" si="4"/>
-        <v>0.45</v>
+        <v>0.46</v>
       </c>
       <c r="R8" t="s">
         <v>107</v>
@@ -21213,7 +21213,7 @@
         <v>4</v>
       </c>
       <c r="F9" s="134">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="G9" s="135">
         <v>20</v>
@@ -21234,7 +21234,7 @@
       </c>
       <c r="L9" s="158">
         <f t="shared" si="1"/>
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="M9" s="158">
         <f t="shared" si="2"/>
@@ -21242,7 +21242,7 @@
       </c>
       <c r="N9" s="159">
         <f t="shared" si="3"/>
-        <v>51.4285714285714</v>
+        <v>50</v>
       </c>
       <c r="P9">
         <f t="shared" si="4"/>
@@ -21267,7 +21267,7 @@
         <v>1.5</v>
       </c>
       <c r="F10" s="134">
-        <v>3.5</v>
+        <v>3.3</v>
       </c>
       <c r="G10" s="135">
         <v>20</v>
@@ -21288,7 +21288,7 @@
       </c>
       <c r="L10" s="158">
         <f t="shared" si="1"/>
-        <v>10.1666666666667</v>
+        <v>9.96666666666667</v>
       </c>
       <c r="M10" s="158">
         <f t="shared" si="2"/>
@@ -21296,7 +21296,7 @@
       </c>
       <c r="N10" s="159">
         <f t="shared" si="3"/>
-        <v>49.1803278688525</v>
+        <v>50.1672240802676</v>
       </c>
       <c r="P10">
         <f t="shared" si="4"/>
@@ -21322,7 +21322,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="140">
-        <v>2.5</v>
+        <v>2.85</v>
       </c>
       <c r="G11" s="141">
         <v>20</v>
@@ -21343,7 +21343,7 @@
       </c>
       <c r="L11" s="160">
         <f t="shared" si="1"/>
-        <v>2.83333333333333</v>
+        <v>3.18333333333333</v>
       </c>
       <c r="M11" s="160">
         <f t="shared" si="2"/>
@@ -21351,7 +21351,7 @@
       </c>
       <c r="N11" s="161">
         <f t="shared" si="3"/>
-        <v>56.4705882352941</v>
+        <v>50.261780104712</v>
       </c>
       <c r="P11">
         <f t="shared" si="4"/>
@@ -21379,7 +21379,7 @@
         <v>12</v>
       </c>
       <c r="F12" s="134">
-        <v>1</v>
+        <v>1.1</v>
       </c>
       <c r="G12" s="143">
         <v>30</v>
@@ -21400,7 +21400,7 @@
       </c>
       <c r="L12" s="158">
         <f t="shared" si="1"/>
-        <v>3.5</v>
+        <v>3.6</v>
       </c>
       <c r="M12" s="158">
         <f t="shared" si="2"/>
@@ -21408,7 +21408,7 @@
       </c>
       <c r="N12" s="159">
         <f t="shared" si="3"/>
-        <v>51.4285714285714</v>
+        <v>50</v>
       </c>
       <c r="P12">
         <f t="shared" si="4"/>
@@ -21427,13 +21427,13 @@
         <v>45</v>
       </c>
       <c r="D13" s="133">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E13" s="134">
         <v>8</v>
       </c>
       <c r="F13" s="134">
-        <v>1.25</v>
+        <v>1.5</v>
       </c>
       <c r="G13" s="135">
         <v>30</v>
@@ -21446,7 +21446,7 @@
       </c>
       <c r="J13" s="158">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K13" s="158">
         <f t="shared" si="0"/>
@@ -21454,19 +21454,19 @@
       </c>
       <c r="L13" s="158">
         <f t="shared" si="1"/>
-        <v>3.75</v>
+        <v>4</v>
       </c>
       <c r="M13" s="158">
         <f t="shared" si="2"/>
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="N13" s="159">
         <f t="shared" si="3"/>
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="P13">
         <f t="shared" si="4"/>
-        <v>0.005625</v>
+        <v>0.00625</v>
       </c>
       <c r="R13" t="s">
         <v>105</v>
@@ -21487,7 +21487,7 @@
         <v>11</v>
       </c>
       <c r="F14" s="140">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G14" s="141">
         <v>30</v>
@@ -21508,7 +21508,7 @@
       </c>
       <c r="L14" s="160">
         <f t="shared" si="1"/>
-        <v>3.72727272727273</v>
+        <v>3.62727272727273</v>
       </c>
       <c r="M14" s="160">
         <f t="shared" si="2"/>
@@ -21516,7 +21516,7 @@
       </c>
       <c r="N14" s="161">
         <f t="shared" si="3"/>
-        <v>48.2926829268293</v>
+        <v>49.6240601503759</v>
       </c>
       <c r="P14">
         <f t="shared" si="4"/>
@@ -21540,10 +21540,10 @@
         <v>14</v>
       </c>
       <c r="E15" s="134">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="F15" s="134">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G15" s="143">
         <v>40</v>
@@ -21560,11 +21560,11 @@
       </c>
       <c r="K15" s="158">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>15.5555555555556</v>
       </c>
       <c r="L15" s="158">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>19.5555555555556</v>
       </c>
       <c r="M15" s="158">
         <f t="shared" si="2"/>
@@ -21572,12 +21572,12 @@
       </c>
       <c r="N15" s="159">
         <f t="shared" si="3"/>
-        <v>51.5789473684211</v>
+        <v>50.1136363636364</v>
       </c>
       <c r="O15" s="86"/>
       <c r="P15">
         <f t="shared" si="4"/>
-        <v>0.014</v>
+        <v>0.0155555555555556</v>
       </c>
       <c r="Q15"/>
       <c r="R15" t="s">
@@ -21599,7 +21599,7 @@
         <v>53</v>
       </c>
       <c r="D16" s="133">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E16" s="134">
         <v>5</v>
@@ -21618,7 +21618,7 @@
       </c>
       <c r="J16" s="158">
         <f t="shared" si="5"/>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K16" s="158">
         <f t="shared" si="0"/>
@@ -21630,15 +21630,15 @@
       </c>
       <c r="M16" s="158">
         <f t="shared" si="2"/>
-        <v>900</v>
+        <v>850</v>
       </c>
       <c r="N16" s="159">
         <f t="shared" si="3"/>
-        <v>52.9411764705882</v>
+        <v>50</v>
       </c>
       <c r="P16">
         <f t="shared" si="4"/>
-        <v>0.018</v>
+        <v>0.017</v>
       </c>
       <c r="R16" t="s">
         <v>105</v>
@@ -21659,7 +21659,7 @@
         <v>7</v>
       </c>
       <c r="F17" s="149">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="G17" s="150">
         <v>40</v>
@@ -21680,7 +21680,7 @@
       </c>
       <c r="L17" s="162">
         <f t="shared" si="1"/>
-        <v>12.1428571428571</v>
+        <v>11.9428571428571</v>
       </c>
       <c r="M17" s="162">
         <f t="shared" si="2"/>
@@ -21688,7 +21688,7 @@
       </c>
       <c r="N17" s="163">
         <f t="shared" si="3"/>
-        <v>49.4117647058824</v>
+        <v>50.2392344497608</v>
       </c>
       <c r="O17" s="86"/>
       <c r="P17">
@@ -21715,7 +21715,7 @@
         <v>115</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="4:7">
@@ -21735,19 +21735,19 @@
     <row r="21" spans="4:7">
       <c r="D21">
         <f>0.08*C19+1</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E21">
         <f>0.02*C19+1</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21">
         <f>1-0.01*C19</f>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="G21">
         <f>0.01*C19+1</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -21822,45 +21822,45 @@
       </c>
       <c r="D24" s="128">
         <f>D3*D$21</f>
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="E24" s="129">
         <f>E3*E$21</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F24" s="129">
         <f>F3*F$21</f>
-        <v>0.5</v>
+        <v>0.425</v>
       </c>
       <c r="G24" s="130">
         <f>G3*G$21</f>
-        <v>60</v>
+        <v>82.5</v>
       </c>
       <c r="H24" s="131">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="I24" s="129">
         <v>10</v>
       </c>
       <c r="J24" s="158">
         <f t="shared" ref="J24:J29" si="6">D24*1</f>
-        <v>19</v>
+        <v>105</v>
       </c>
       <c r="K24" s="158">
         <f t="shared" ref="K24:K38" si="7">I24/E24</f>
-        <v>3.33333333333333</v>
+        <v>1.66666666666667</v>
       </c>
       <c r="L24" s="158">
         <f t="shared" ref="L24:L38" si="8">K24+F24</f>
-        <v>3.83333333333333</v>
+        <v>2.09166666666667</v>
       </c>
       <c r="M24" s="158">
         <f t="shared" ref="M24:M38" si="9">J24*I24</f>
-        <v>190</v>
+        <v>1050</v>
       </c>
       <c r="N24" s="159">
         <f t="shared" ref="N24:N38" si="10">M24/L24</f>
-        <v>49.5652173913043</v>
+        <v>501.99203187251</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -21873,45 +21873,45 @@
       </c>
       <c r="D25" s="133">
         <f t="shared" ref="D25:D38" si="11">D4*D$21</f>
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="E25" s="134">
         <f t="shared" ref="E25:E38" si="12">E4*E$21</f>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F25" s="134">
         <f t="shared" ref="F25:F38" si="13">F4*F$21</f>
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
       <c r="G25" s="135">
         <f t="shared" ref="G25:G38" si="14">G4*G$21</f>
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="H25" s="136">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="I25" s="134">
         <v>12</v>
       </c>
       <c r="J25" s="158">
-        <f>D25*2</f>
-        <v>14</v>
+        <f>D25*1</f>
+        <v>65</v>
       </c>
       <c r="K25" s="158">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>1.2</v>
       </c>
       <c r="L25" s="158">
         <f t="shared" si="8"/>
-        <v>3.5</v>
+        <v>1.55</v>
       </c>
       <c r="M25" s="158">
         <f t="shared" si="9"/>
-        <v>168</v>
+        <v>780</v>
       </c>
       <c r="N25" s="159">
         <f t="shared" si="10"/>
-        <v>48</v>
+        <v>503.225806451613</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -21924,19 +21924,19 @@
       </c>
       <c r="D26" s="139">
         <f t="shared" si="11"/>
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="E26" s="140">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F26" s="140">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26" s="141">
         <f t="shared" si="14"/>
-        <v>75</v>
+        <v>97.5</v>
       </c>
       <c r="H26" s="142">
         <v>90</v>
@@ -21946,23 +21946,23 @@
       </c>
       <c r="J26" s="160">
         <f t="shared" si="6"/>
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="K26" s="160">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L26" s="160">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="M26" s="160">
         <f t="shared" si="9"/>
-        <v>150</v>
+        <v>750</v>
       </c>
       <c r="N26" s="161">
         <f t="shared" si="10"/>
-        <v>50</v>
+        <v>500</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -21977,19 +21977,19 @@
       </c>
       <c r="D27" s="133">
         <f t="shared" si="11"/>
-        <v>75</v>
+        <v>375</v>
       </c>
       <c r="E27" s="134">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" s="134">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="G27" s="143">
         <f t="shared" si="14"/>
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="H27" s="136">
         <v>20</v>
@@ -21999,23 +21999,23 @@
       </c>
       <c r="J27" s="158">
         <f t="shared" si="6"/>
-        <v>75</v>
+        <v>375</v>
       </c>
       <c r="K27" s="158">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L27" s="158">
         <f t="shared" si="8"/>
-        <v>9</v>
+        <v>4.5</v>
       </c>
       <c r="M27" s="158">
         <f t="shared" si="9"/>
-        <v>450</v>
+        <v>2250</v>
       </c>
       <c r="N27" s="159">
         <f t="shared" si="10"/>
-        <v>50</v>
+        <v>500</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -22028,19 +22028,19 @@
       </c>
       <c r="D28" s="133">
         <f t="shared" si="11"/>
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="E28" s="134">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F28" s="134">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="G28" s="135">
         <f t="shared" si="14"/>
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="H28" s="136">
         <v>0</v>
@@ -22050,23 +22050,23 @@
       </c>
       <c r="J28" s="158">
         <f t="shared" si="6"/>
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="K28" s="158">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>1.5</v>
       </c>
       <c r="L28" s="158">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M28" s="158">
         <f t="shared" si="9"/>
-        <v>300</v>
+        <v>1500</v>
       </c>
       <c r="N28" s="159">
         <f t="shared" si="10"/>
-        <v>50</v>
+        <v>500</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -22079,19 +22079,19 @@
       </c>
       <c r="D29" s="139">
         <f t="shared" si="11"/>
-        <v>90</v>
+        <v>460</v>
       </c>
       <c r="E29" s="140">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" s="140">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="G29" s="141">
         <f t="shared" si="14"/>
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="H29" s="142">
         <v>20</v>
@@ -22101,23 +22101,23 @@
       </c>
       <c r="J29" s="160">
         <f t="shared" si="6"/>
-        <v>90</v>
+        <v>460</v>
       </c>
       <c r="K29" s="160">
         <f t="shared" si="7"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L29" s="160">
         <f t="shared" si="8"/>
-        <v>11</v>
+        <v>5.5</v>
       </c>
       <c r="M29" s="160">
         <f t="shared" si="9"/>
-        <v>540</v>
+        <v>2760</v>
       </c>
       <c r="N29" s="161">
         <f t="shared" si="10"/>
-        <v>49.0909090909091</v>
+        <v>501.818181818182</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -22132,19 +22132,19 @@
       </c>
       <c r="D30" s="133">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="E30" s="134">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F30" s="134">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>1.05</v>
       </c>
       <c r="G30" s="135">
         <f t="shared" si="14"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H30" s="136">
         <v>35</v>
@@ -22154,23 +22154,23 @@
       </c>
       <c r="J30" s="158">
         <f t="shared" ref="J30:J32" si="15">D30*10</f>
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="K30" s="158">
         <f t="shared" si="7"/>
-        <v>1.5</v>
+        <v>0.75</v>
       </c>
       <c r="L30" s="158">
         <f t="shared" si="8"/>
-        <v>3.5</v>
+        <v>1.8</v>
       </c>
       <c r="M30" s="158">
         <f t="shared" si="9"/>
-        <v>180</v>
+        <v>900</v>
       </c>
       <c r="N30" s="159">
         <f t="shared" si="10"/>
-        <v>51.4285714285714</v>
+        <v>500</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -22183,19 +22183,19 @@
       </c>
       <c r="D31" s="133">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="E31" s="134">
         <f t="shared" si="12"/>
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="F31" s="134">
         <f t="shared" si="13"/>
-        <v>3.5</v>
+        <v>1.65</v>
       </c>
       <c r="G31" s="135">
         <f t="shared" si="14"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H31" s="136">
         <v>35</v>
@@ -22205,23 +22205,23 @@
       </c>
       <c r="J31" s="158">
         <f t="shared" si="15"/>
-        <v>50</v>
+        <v>250</v>
       </c>
       <c r="K31" s="158">
         <f t="shared" si="7"/>
-        <v>6.66666666666667</v>
+        <v>3.33333333333333</v>
       </c>
       <c r="L31" s="158">
         <f t="shared" si="8"/>
-        <v>10.1666666666667</v>
+        <v>4.98333333333333</v>
       </c>
       <c r="M31" s="158">
         <f t="shared" si="9"/>
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="N31" s="159">
         <f t="shared" si="10"/>
-        <v>49.1803278688525</v>
+        <v>501.672240802676</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -22234,19 +22234,19 @@
       </c>
       <c r="D32" s="139">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="E32" s="140">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F32" s="140">
         <f t="shared" si="13"/>
-        <v>2.5</v>
+        <v>1.425</v>
       </c>
       <c r="G32" s="141">
         <f t="shared" si="14"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H32" s="142">
         <v>35</v>
@@ -22256,23 +22256,23 @@
       </c>
       <c r="J32" s="160">
         <f t="shared" si="15"/>
-        <v>80</v>
+        <v>400</v>
       </c>
       <c r="K32" s="160">
         <f t="shared" si="7"/>
-        <v>0.333333333333333</v>
+        <v>0.166666666666667</v>
       </c>
       <c r="L32" s="160">
         <f t="shared" si="8"/>
-        <v>2.83333333333333</v>
+        <v>1.59166666666667</v>
       </c>
       <c r="M32" s="160">
         <f t="shared" si="9"/>
-        <v>160</v>
+        <v>800</v>
       </c>
       <c r="N32" s="161">
         <f t="shared" si="10"/>
-        <v>56.4705882352941</v>
+        <v>502.61780104712</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -22287,19 +22287,19 @@
       </c>
       <c r="D33" s="133">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E33" s="134">
         <f t="shared" si="12"/>
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="F33" s="134">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.55</v>
       </c>
       <c r="G33" s="143">
         <f t="shared" si="14"/>
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="H33" s="136">
         <v>98</v>
@@ -22309,23 +22309,23 @@
       </c>
       <c r="J33" s="158">
         <f t="shared" ref="J33:J38" si="16">D33*1</f>
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="K33" s="158">
         <f t="shared" si="7"/>
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
       <c r="L33" s="158">
         <f t="shared" si="8"/>
-        <v>3.5</v>
+        <v>1.8</v>
       </c>
       <c r="M33" s="158">
         <f t="shared" si="9"/>
-        <v>180</v>
+        <v>900</v>
       </c>
       <c r="N33" s="159">
         <f t="shared" si="10"/>
-        <v>51.4285714285714</v>
+        <v>500</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -22338,19 +22338,19 @@
       </c>
       <c r="D34" s="133">
         <f t="shared" si="11"/>
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="E34" s="134">
         <f t="shared" si="12"/>
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="F34" s="134">
         <f t="shared" si="13"/>
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="G34" s="135">
         <f t="shared" si="14"/>
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="H34" s="136">
         <v>95</v>
@@ -22360,23 +22360,23 @@
       </c>
       <c r="J34" s="158">
         <f t="shared" si="16"/>
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="K34" s="158">
         <f t="shared" si="7"/>
-        <v>2.5</v>
+        <v>1.25</v>
       </c>
       <c r="L34" s="158">
         <f t="shared" si="8"/>
-        <v>3.75</v>
+        <v>2</v>
       </c>
       <c r="M34" s="158">
         <f t="shared" si="9"/>
-        <v>180</v>
+        <v>1000</v>
       </c>
       <c r="N34" s="159">
         <f t="shared" si="10"/>
-        <v>48</v>
+        <v>500</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -22389,19 +22389,19 @@
       </c>
       <c r="D35" s="139">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="E35" s="140">
         <f t="shared" si="12"/>
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F35" s="140">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0.45</v>
       </c>
       <c r="G35" s="141">
         <f t="shared" si="14"/>
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="H35" s="142">
         <v>98</v>
@@ -22411,23 +22411,23 @@
       </c>
       <c r="J35" s="160">
         <f t="shared" si="16"/>
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="K35" s="160">
         <f t="shared" si="7"/>
-        <v>2.72727272727273</v>
+        <v>1.36363636363636</v>
       </c>
       <c r="L35" s="160">
         <f t="shared" si="8"/>
-        <v>3.72727272727273</v>
+        <v>1.81363636363636</v>
       </c>
       <c r="M35" s="160">
         <f t="shared" si="9"/>
-        <v>180</v>
+        <v>900</v>
       </c>
       <c r="N35" s="161">
         <f t="shared" si="10"/>
-        <v>48.2926829268293</v>
+        <v>496.240601503759</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -22442,19 +22442,19 @@
       </c>
       <c r="D36" s="133">
         <f t="shared" si="11"/>
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="E36" s="134">
         <f t="shared" si="12"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F36" s="134">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G36" s="143">
         <f t="shared" si="14"/>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="H36" s="136">
         <v>95</v>
@@ -22464,23 +22464,23 @@
       </c>
       <c r="J36" s="158">
         <f t="shared" si="16"/>
-        <v>14</v>
+        <v>70</v>
       </c>
       <c r="K36" s="158">
         <f t="shared" si="7"/>
-        <v>14</v>
+        <v>7.77777777777778</v>
       </c>
       <c r="L36" s="158">
         <f t="shared" si="8"/>
-        <v>19</v>
+        <v>9.77777777777778</v>
       </c>
       <c r="M36" s="158">
         <f t="shared" si="9"/>
-        <v>980</v>
+        <v>4900</v>
       </c>
       <c r="N36" s="159">
         <f t="shared" si="10"/>
-        <v>51.5789473684211</v>
+        <v>501.136363636364</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -22493,19 +22493,19 @@
       </c>
       <c r="D37" s="133">
         <f t="shared" si="11"/>
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="E37" s="134">
         <f t="shared" si="12"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F37" s="134">
         <f t="shared" si="13"/>
-        <v>7</v>
+        <v>3.5</v>
       </c>
       <c r="G37" s="135">
         <f t="shared" si="14"/>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="H37" s="136">
         <v>90</v>
@@ -22515,23 +22515,23 @@
       </c>
       <c r="J37" s="158">
         <f t="shared" si="16"/>
-        <v>18</v>
+        <v>85</v>
       </c>
       <c r="K37" s="158">
         <f t="shared" si="7"/>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="L37" s="158">
         <f t="shared" si="8"/>
-        <v>17</v>
+        <v>8.5</v>
       </c>
       <c r="M37" s="158">
         <f t="shared" si="9"/>
-        <v>900</v>
+        <v>4250</v>
       </c>
       <c r="N37" s="159">
         <f t="shared" si="10"/>
-        <v>52.9411764705882</v>
+        <v>500</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -22544,19 +22544,19 @@
       </c>
       <c r="D38" s="148">
         <f t="shared" si="11"/>
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="E38" s="149">
         <f t="shared" si="12"/>
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F38" s="149">
         <f t="shared" si="13"/>
-        <v>5</v>
+        <v>2.4</v>
       </c>
       <c r="G38" s="150">
         <f t="shared" si="14"/>
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="H38" s="151">
         <v>90</v>
@@ -22566,23 +22566,23 @@
       </c>
       <c r="J38" s="162">
         <f t="shared" si="16"/>
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="K38" s="162">
         <f t="shared" si="7"/>
-        <v>7.14285714285714</v>
+        <v>3.57142857142857</v>
       </c>
       <c r="L38" s="162">
         <f t="shared" si="8"/>
-        <v>12.1428571428571</v>
+        <v>5.97142857142857</v>
       </c>
       <c r="M38" s="162">
         <f t="shared" si="9"/>
-        <v>600</v>
+        <v>3000</v>
       </c>
       <c r="N38" s="163">
         <f t="shared" si="10"/>
-        <v>49.4117647058824</v>
+        <v>502.392344497608</v>
       </c>
     </row>
   </sheetData>
@@ -24128,7 +24128,7 @@
   <sheetPr/>
   <dimension ref="A1:AI80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
@@ -28336,7 +28336,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
<Optimisation, Bugfix> Pathing, Combat
Massively improved poisson sampling (not actually poisson sampling
anymore) generation.
Thunder audio now loaded at start.
Compass indicators now point to nearest thing in each 20 degree arc.
Reduced garbage collection impact for fastlight.
Improved fastlight performance.
Improved pathing grid performance.
Increased randomness of region generation.
Increased amount of rubble in region.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="2" activeTab="12"/>
+    <workbookView windowWidth="28695" windowHeight="13185" firstSheet="2" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -13954,8 +13954,8 @@
   <sheetPr/>
   <dimension ref="A1:J24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -14462,8 +14462,8 @@
   <sheetPr/>
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -20882,7 +20882,7 @@
   <dimension ref="A1:Y38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
<Bugfix, Feature> Rifle, Movement
Fixed enemy movement again, even more aggressive, plus added longer
reload time and pauses between firing.
Accessory modifier now gets applied to weapons and character.
Removed seek cover behaviour.
Increased rifle shot speed.
Improved rifle trail.
Changed some skill behaviours.
Updated push to work on enemies or player.
Fixed bug where martyr wouldn't detonate.
Removed shield for now.
Added sprite flash for taking condition damage.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18620" firstSheet="2" activeTab="15"/>
+    <workbookView windowHeight="18620" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -3231,14 +3231,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="0_ "/>
+    <numFmt numFmtId="178" formatCode="0.0_ "/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="0.00_ "/>
-    <numFmt numFmtId="177" formatCode="0_ "/>
-    <numFmt numFmtId="178" formatCode="0.0"/>
-    <numFmt numFmtId="179" formatCode="0.0_ "/>
+    <numFmt numFmtId="179" formatCode="0.0"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -3300,7 +3300,91 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3315,68 +3399,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3393,51 +3438,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3571,13 +3571,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3589,7 +3625,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3601,19 +3655,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3625,55 +3715,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3685,73 +3745,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4160,6 +4160,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
       </bottom>
@@ -4182,6 +4191,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -4196,46 +4220,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4254,12 +4243,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4277,130 +4277,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="37" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="37" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="41" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="41" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="52" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4510,10 +4510,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="179" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4717,7 +4717,7 @@
     <xf numFmtId="1" fontId="0" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="15" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
@@ -4735,7 +4735,7 @@
     <xf numFmtId="1" fontId="0" fillId="15" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -13279,8 +13279,8 @@
   <sheetPr/>
   <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>
@@ -13378,7 +13378,7 @@
         <v>775</v>
       </c>
       <c r="C4" s="28">
-        <v>0.1</v>
+        <v>-0.1</v>
       </c>
       <c r="D4" s="29" t="b">
         <v>0</v>
@@ -15914,7 +15914,7 @@
   <sheetPr/>
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
<Bugfix, Feature> Combat UI, Feedback Work
Simplified combat hud.
Moved and clarified pickup prompt.
FixeFixed bug where puddle had no select image.
Available compass pulses clearer.
Removed Armour and Health text.
Fixed bug where durability markers weren't showing.
Non-highlighted list elements are now 40% opacity.
Crafting fire now shows text.
Crafting menu even clearer.
Disabled buttons cannot be navigated to.
Fixed bug where toggling pause menu would break game.
Fixed bug where placeholder region text was shown at start of combat.
Fixed bug where inner ring of map wasn't being used.
Fixed bug where select image wasn't being shown when close enough to
container.
Fixed bug where container glow wouldn't fade.
Simplified armour, now takes a flat 5% damage reduction for each armour
piece.
Armour can only be damaged by shatter.
Fixed bug where resources were not saving if they had spaces or special
characters.
Fixed bug where colour pulse wouldn't work when timescale was 0.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -14775,8 +14775,8 @@
   <sheetPr/>
   <dimension ref="A1:S1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
<Feature, Bugfix> Tutorial, Needle, Push, More
Added Needle attack- accelerating projectile.
Rearranged character view to prioritise most used elements.
Swapped and improved sicken and vortex animations.
Added option to activate tutorial.
Updated push visuals (needs changing though).
Tutorial manager now shows tutorial sections, pausing game as necessary.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -3383,13 +3383,13 @@
     <t>Physical</t>
   </si>
   <si>
-    <t>Fettle- Increases your maximum health in combat.\nGrit- Determines how far you can travel on the map, as well as movement speed in combat.</t>
+    <t>Fettle- Increases your maximum health in combat. Grit- Determines how far you can travel on the map, as well as movement speed in combat.</t>
   </si>
   <si>
     <t>Mental</t>
   </si>
   <si>
-    <t>Focus- Increases your total compass charges, and your adrenaline recharge rate.\nWill- Can be used to restore other attributes, and reduces the cooldown of your skills.</t>
+    <t>Focus- Increases your total compass charges, and your adrenaline recharge rate. Will- Can be used to restore other attributes, and reduces the cooldown of your skills.</t>
   </si>
   <si>
     <t>Restoring Attributes</t>
@@ -14884,7 +14884,7 @@
   <sheetPr/>
   <dimension ref="A1:S1048576"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
@@ -17169,7 +17169,7 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="7"/>
@@ -17220,24 +17220,27 @@
         <v>1096</v>
       </c>
       <c r="D2">
-        <v>785</v>
+        <v>865</v>
       </c>
       <c r="E2">
-        <v>730</v>
+        <v>505</v>
       </c>
       <c r="F2">
-        <v>785</v>
+        <v>865</v>
       </c>
       <c r="G2">
-        <v>250</v>
+        <v>480</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>1097</v>
       </c>
     </row>
-    <row r="3" spans="2:8">
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>2</v>
+      </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
         <v>1098</v>
@@ -17258,9 +17261,12 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="4" spans="2:8">
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>2</v>
+      </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
         <v>1100</v>
@@ -17283,7 +17289,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -17307,7 +17313,10 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>3</v>
+      </c>
       <c r="B6">
         <v>2</v>
       </c>
@@ -17330,7 +17339,10 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>3</v>
+      </c>
       <c r="B7">
         <v>3</v>
       </c>
@@ -17353,7 +17365,10 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>3</v>
+      </c>
       <c r="B8">
         <v>4</v>
       </c>
@@ -17376,7 +17391,10 @@
         <v>1107</v>
       </c>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>3</v>
+      </c>
       <c r="B9">
         <v>5</v>
       </c>
@@ -17404,7 +17422,7 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
         <v>1110</v>
@@ -17427,10 +17445,10 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>1112</v>
@@ -17453,7 +17471,7 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -17477,7 +17495,10 @@
         <v>1115</v>
       </c>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>4</v>
+      </c>
       <c r="B13">
         <v>2</v>
       </c>
@@ -17500,7 +17521,10 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>4</v>
+      </c>
       <c r="B14">
         <v>3</v>
       </c>
@@ -17523,7 +17547,10 @@
         <v>1119</v>
       </c>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>4</v>
+      </c>
       <c r="B15">
         <v>4</v>
       </c>
@@ -17546,7 +17573,10 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>4</v>
+      </c>
       <c r="B16">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
<Feature, Bugfix> Explosions, Tutorial
Added impact to fire and shatter effects.
Updated fire behaviours to allow for explosion, trail, and simple fire.
Added more tutorial sections.
Modified condition chance by magazine size.
Changed Erupt skill behaviour to have a cluster bomb effect.
Game won't start until all audioclips loaded.
Tutorial window now hidden if given zero bounds.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157">
   <si>
     <t>Type</t>
   </si>
@@ -3323,7 +3323,7 @@
     <t>Exploration</t>
   </si>
   <si>
-    <t>Survival in the world of Beyond The Veil relies on constant exploration of your environment, both to survive, and to carry out the Necromancer’s commands. Select the Explore action to find a new destination to exploit.</t>
+    <t>Beyond The Veil requires constant exploration of your environment, both to survive, and to carry out the Necromancer’s commands. The Explore action allows you to access the map, where you can discover and exploit new destinations.</t>
   </si>
   <si>
     <t>The Map</t>
@@ -3374,6 +3374,9 @@
     <t>If you have fully explored a region, or you need to escape an overpowering encounter, you can leave by travelling to the ring around the region’s edge.</t>
   </si>
   <si>
+    <t>Finally, there are 4 types of damage in Beyond The Veil. Physical damage is the most basic, is dealt by all weapons, and can reduced by armour. Shatter damage causes damage to armour, increasing the amount of physical damage dealt. Fire damage causes small amounts of direct damage over time. Void damage builds up over time, and upon reaching a critical level, causes large amounts of damage directly to health.</t>
+  </si>
+  <si>
     <t>Attributes</t>
   </si>
   <si>
@@ -3402,6 +3405,102 @@
   </si>
   <si>
     <t>Your Hunger and Thirst will decrease over time, eventually killing you if allowed to fully deplete. Eat food and drink water to stave them off. Hot weather will cause you to dehydrate, whilst Cold weather increases your Hunger.</t>
+  </si>
+  <si>
+    <t>Progress</t>
+  </si>
+  <si>
+    <t>Progress is saved automatically at the dawn of every day. If a character starves, dehydrates, or loses all their health in combat, they will die. If the Wanderer dies, it is game over, and you must either reload at the dawn of the last day, or start a new game. The day can be restarted at any time from the pause menu.</t>
+  </si>
+  <si>
+    <t>Gear</t>
+  </si>
+  <si>
+    <t>The gear section shows your currently equipped Weapon, Armour, and Accessory. To learn more about each gear type, select the relevant element.</t>
+  </si>
+  <si>
+    <t>Crafting</t>
+  </si>
+  <si>
+    <t>The resources you find in the world can be used to craft a variety of different items. As you find resources, recipes will be unlocked that can make your journey through the world easier.</t>
+  </si>
+  <si>
+    <t>Some resources are always dropped by enemies, some can be found scattered throughout the world, and some can only be crafted.</t>
+  </si>
+  <si>
+    <t>Salt is dropped by enemies, and can be used to craft one of the most useful resources in the game- Radiance. Radiance can be used to claim a region. Over time, claimed regions will generate either food, water, or resources. These resources are automatically added to your inventory.</t>
+  </si>
+  <si>
+    <t>Weapons</t>
+  </si>
+  <si>
+    <t>Weapons come in a number of different varieties, all of which with unique firing behaviours.</t>
+  </si>
+  <si>
+    <t>Weapon power affects the damage output of a weapon. Lower power reduces the effectiveness of your weapons, whilst higher power increases it. The current weapon power is shown on this bar.</t>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>A weapon’s quality affects it’s maximum power, and is represented by the width of the power bar. Weapons of equal power will have similar damage outputs, regardless of their quality. For this reason it is important to maintain their power level.</t>
+  </si>
+  <si>
+    <t>Chanelling</t>
+  </si>
+  <si>
+    <t>Using your weapon slowly drains it of power, thereby decreasing the damage you deal in combat. You can offset this either by using a different weapon, or by channelling essence into it to increase it’s Power. Finding this essence, however, may be easier said than done.</t>
+  </si>
+  <si>
+    <t>Infusions</t>
+  </si>
+  <si>
+    <t>Weapons can also be infused with the last words of the dying. These infusions grant larger, passive bonuses to weapons, allowing you to customise them further to your playstyle. Infusing can only be performed using Essence, and new Infusions will replace any existing ones.</t>
+  </si>
+  <si>
+    <t>Armour can be equipped to reduce incoming damage. All characters have two armour slots for Chest and Head armour respectively.</t>
+  </si>
+  <si>
+    <t>Protection</t>
+  </si>
+  <si>
+    <t>Armour offers varying levels of protection, with higher quality armour offering more protection. Each point of protection offers a 5% reduction in damage, up to a maximum of 50%.</t>
+  </si>
+  <si>
+    <t>The Shatter effect causes damage to armour. When enough Shatter damage is taken, armour will lose a point of protection. If a piece of armour loses all it’s protection, it will break, and be lost.</t>
+  </si>
+  <si>
+    <t>Sources</t>
+  </si>
+  <si>
+    <t>Armour cannot be repaired, and so must be replaced, either through crafting, or found as loot. Instead of a health boost, consider armour an expendable source of protection, destined to be damaged and eventually destroyed.</t>
+  </si>
+  <si>
+    <t>Accessories</t>
+  </si>
+  <si>
+    <t>Accessories are small trinkets that can further modify the power of your weapon, either by increasing the chance of inflicting conditions, or by increasing the stats of your weapons. Only one accessory can be equipped at a time.</t>
+  </si>
+  <si>
+    <t>Skills</t>
+  </si>
+  <si>
+    <t>Skills can have a large impact on how a battle plays out. In total there are 4 skill slots available during combat.</t>
+  </si>
+  <si>
+    <t>Character Skills</t>
+  </si>
+  <si>
+    <t>2 skills are linked to the character’s class. These skills are unlocked over time, and are generally geared towards survival.</t>
+  </si>
+  <si>
+    <t>Weapon Skills</t>
+  </si>
+  <si>
+    <t>The remaining 2 skills are linked to the currently equipped weapon. Weapon skills unlocked by dealing damage with the relevant weapon. Weapon skills have an offensive focus, and are complement the play style of each weapon.</t>
+  </si>
+  <si>
+    <t>The cost of a skill is shown above its name. Activating any skill will reset the cooldown period of all your skills, regardless of their cost.</t>
   </si>
 </sst>
 </file>
@@ -17166,10 +17265,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="7"/>
@@ -17223,13 +17322,13 @@
         <v>865</v>
       </c>
       <c r="E2">
-        <v>505</v>
+        <v>495</v>
       </c>
       <c r="F2">
         <v>865</v>
       </c>
       <c r="G2">
-        <v>480</v>
+        <v>465</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>1097</v>
@@ -17471,28 +17570,28 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>1114</v>
-      </c>
-      <c r="D12">
-        <v>645</v>
-      </c>
-      <c r="E12">
-        <v>320</v>
-      </c>
-      <c r="F12">
-        <v>645</v>
-      </c>
-      <c r="G12">
-        <v>645</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>1115</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -17500,10 +17599,10 @@
         <v>4</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="D13">
         <v>645</v>
@@ -17512,13 +17611,13 @@
         <v>320</v>
       </c>
       <c r="F13">
-        <v>960</v>
+        <v>645</v>
       </c>
       <c r="G13">
         <v>645</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -17526,25 +17625,25 @@
         <v>4</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="D14">
-        <v>960</v>
+        <v>645</v>
       </c>
       <c r="E14">
         <v>320</v>
       </c>
       <c r="F14">
-        <v>645</v>
+        <v>960</v>
       </c>
       <c r="G14">
         <v>645</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="15" spans="1:8">
@@ -17552,25 +17651,25 @@
         <v>4</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15" t="s">
+        <v>1119</v>
+      </c>
+      <c r="D15">
+        <v>960</v>
+      </c>
+      <c r="E15">
+        <v>320</v>
+      </c>
+      <c r="F15">
+        <v>645</v>
+      </c>
+      <c r="G15">
+        <v>645</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>1120</v>
-      </c>
-      <c r="D15">
-        <v>840</v>
-      </c>
-      <c r="E15">
-        <v>840</v>
-      </c>
-      <c r="F15">
-        <v>840</v>
-      </c>
-      <c r="G15">
-        <v>115</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>1121</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -17578,25 +17677,545 @@
         <v>4</v>
       </c>
       <c r="B16">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1121</v>
+      </c>
+      <c r="D16">
+        <v>840</v>
+      </c>
+      <c r="E16">
+        <v>840</v>
+      </c>
+      <c r="F16">
+        <v>840</v>
+      </c>
+      <c r="G16">
+        <v>115</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>1122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
         <v>5</v>
       </c>
-      <c r="C16" t="s">
-        <v>1122</v>
-      </c>
-      <c r="D16">
+      <c r="C17" t="s">
+        <v>1123</v>
+      </c>
+      <c r="D17">
         <v>635</v>
       </c>
-      <c r="E16">
+      <c r="E17">
         <v>375</v>
       </c>
-      <c r="F16">
+      <c r="F17">
         <v>635</v>
       </c>
-      <c r="G16">
+      <c r="G17">
         <v>605</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>1123</v>
+      <c r="H17" s="1" t="s">
+        <v>1124</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1125</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1127</v>
+      </c>
+      <c r="D19">
+        <v>745</v>
+      </c>
+      <c r="E19">
+        <v>707</v>
+      </c>
+      <c r="F19">
+        <v>745</v>
+      </c>
+      <c r="G19">
+        <v>160</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>1128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>1129</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20">
+        <v>10</v>
+      </c>
+      <c r="F20">
+        <v>20</v>
+      </c>
+      <c r="G20">
+        <v>970</v>
+      </c>
+      <c r="H20" t="s">
+        <v>1130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>791</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>5</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>883</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>6</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>1133</v>
+      </c>
+      <c r="D23">
+        <v>620</v>
+      </c>
+      <c r="E23">
+        <v>300</v>
+      </c>
+      <c r="F23">
+        <v>620</v>
+      </c>
+      <c r="G23">
+        <v>640</v>
+      </c>
+      <c r="H23" t="s">
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>656</v>
+      </c>
+      <c r="D24">
+        <v>745</v>
+      </c>
+      <c r="E24">
+        <v>370</v>
+      </c>
+      <c r="F24">
+        <v>745</v>
+      </c>
+      <c r="G24">
+        <v>600</v>
+      </c>
+      <c r="H24" t="s">
+        <v>1135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>6</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1136</v>
+      </c>
+      <c r="D25">
+        <v>745</v>
+      </c>
+      <c r="E25">
+        <v>370</v>
+      </c>
+      <c r="F25">
+        <v>745</v>
+      </c>
+      <c r="G25">
+        <v>600</v>
+      </c>
+      <c r="H25" t="s">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26">
+        <v>6</v>
+      </c>
+      <c r="B26">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1138</v>
+      </c>
+      <c r="D26">
+        <v>1190</v>
+      </c>
+      <c r="E26">
+        <v>700</v>
+      </c>
+      <c r="F26">
+        <v>565</v>
+      </c>
+      <c r="G26">
+        <v>275</v>
+      </c>
+      <c r="H26" t="s">
+        <v>1139</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27">
+        <v>6</v>
+      </c>
+      <c r="B27">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>1140</v>
+      </c>
+      <c r="D27">
+        <v>565</v>
+      </c>
+      <c r="E27">
+        <v>700</v>
+      </c>
+      <c r="F27">
+        <v>1190</v>
+      </c>
+      <c r="G27">
+        <v>275</v>
+      </c>
+      <c r="H27" t="s">
+        <v>1141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>793</v>
+      </c>
+      <c r="D28">
+        <v>505</v>
+      </c>
+      <c r="E28">
+        <v>305</v>
+      </c>
+      <c r="F28">
+        <v>505</v>
+      </c>
+      <c r="G28">
+        <v>660</v>
+      </c>
+      <c r="H28" t="s">
+        <v>1142</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>7</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1143</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29" t="s">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>7</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30" t="s">
+        <v>1145</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>7</v>
+      </c>
+      <c r="B31">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1146</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
+        <v>1147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1150</v>
+      </c>
+      <c r="D33">
+        <v>525</v>
+      </c>
+      <c r="E33">
+        <v>900</v>
+      </c>
+      <c r="F33">
+        <v>525</v>
+      </c>
+      <c r="G33">
+        <v>55</v>
+      </c>
+      <c r="H33" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D34">
+        <v>570</v>
+      </c>
+      <c r="E34">
+        <v>900</v>
+      </c>
+      <c r="F34">
+        <v>1020</v>
+      </c>
+      <c r="G34">
+        <v>55</v>
+      </c>
+      <c r="H34" t="s">
+        <v>1153</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <v>9</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1154</v>
+      </c>
+      <c r="D35">
+        <v>1020</v>
+      </c>
+      <c r="E35">
+        <v>900</v>
+      </c>
+      <c r="F35">
+        <v>570</v>
+      </c>
+      <c r="G35">
+        <v>55</v>
+      </c>
+      <c r="H35" t="s">
+        <v>1155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36">
+        <v>9</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>574</v>
+      </c>
+      <c r="D36">
+        <v>585</v>
+      </c>
+      <c r="E36">
+        <v>900</v>
+      </c>
+      <c r="F36">
+        <v>1195</v>
+      </c>
+      <c r="G36">
+        <v>110</v>
+      </c>
+      <c r="H36" t="s">
+        <v>1156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
<Feature, Bugfix, Story> Main Story 4th pass
Added shelter player icon.
Fixed bug where water icon wasn't displaying.
Added support for mouse aiming.
Fixed null reference exception when trying to get a dismantle reward
when none available.
Added shelter character event text.
Better enemy spawning when shelter character event triggered.
Added battle music layer 4.
Added default weapon for all new characters.
Removed character in shelter regions after death/discovery.
Changed lmg knockback ability to autospool ability.
Fixed map node audio not fading when map closed.
Fixed pause menu causing game to freeze when used in combat.
Fixed null reference on cooldown controller when skill is null.
Updated main story lore (parts 1-4).
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18620" firstSheet="2" activeTab="16"/>
+    <workbookView windowHeight="18620" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -1793,7 +1793,7 @@
     <t>Compel</t>
   </si>
   <si>
-    <t>Shots release a small shockwave, pushing enemies back</t>
+    <t>Can fire without spooling up</t>
   </si>
   <si>
     <t>Hairpin</t>
@@ -17284,7 +17284,7 @@
   <sheetPr/>
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
@@ -31671,8 +31671,8 @@
   <sheetPr/>
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>
@@ -31828,7 +31828,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="65">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7" s="66" t="s">
         <v>587</v>

</xml_diff>

<commit_message>
<Bugfix, Audio> Journal, Combat Audio
Resource UI now glows/flashes on change.
MapNode claim particles toned down.
Radiance drop audio softened.
Footstep audio muffled.
More audiopoolcontroller functionality.
Added brawler slash audio.
Reduced inscription and channel cost.
Fixed food/water count in resource tab.
Updated inventory audio.
Added journal close audio.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18620" firstSheet="2" activeTab="12"/>
+    <workbookView windowHeight="18620" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -14247,8 +14247,8 @@
   <sheetPr/>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="$A14:$XFD14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>
@@ -25191,8 +25191,8 @@
   <sheetPr/>
   <dimension ref="A1:V102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
<Feature, Bugfix> Combat UI, Tutorial
Added adaptive mouse/keyboard input.
Added gear background to gear menu.
Added save indicator when saving.
Fixed overlap bug on pistol trail.
Made enemy bullet trails red.
Added selected indicator to map node.
Added more tutorial parts, broke some into smaller parts.
First few regions now have no enemies to ease into the game better.
Removing last element in listcontroller no longer breaks it.
List controller gains focus better.
Added reason for death on game over menu.
Simplified weapon list view.
Simplified story skipping.
Added combat HUD fade in out.
Possibly fixed bug where large rocks weren't being placed with the
correct radius.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18620" firstSheet="2" activeTab="2"/>
+    <workbookView windowHeight="18620" firstSheet="2" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251">
   <si>
     <t>Type</t>
   </si>
@@ -3569,6 +3569,39 @@
     <t>Travelling to regions requires grit, shown below the region name. Returning to the gate never consumes grit. The further the region, the more grit required to travel.</t>
   </si>
   <si>
+    <t>This bar shows your remaining Grit. Each point of Grit allows you to travel a distance of 1 additional region.</t>
+  </si>
+  <si>
+    <t>The Compass</t>
+  </si>
+  <si>
+    <t>You can consume compass charges to find hidden resources, enemies, and other nearby points of interest.</t>
+  </si>
+  <si>
+    <t>Charges and Focus</t>
+  </si>
+  <si>
+    <t>The number of times you can use your compass is dictated by your current Focus level. Each use of the compass will consume 1 focus.</t>
+  </si>
+  <si>
+    <t>Search for Resources</t>
+  </si>
+  <si>
+    <t>Try using the compass to explore this region (press [E]).</t>
+  </si>
+  <si>
+    <t>Meditating</t>
+  </si>
+  <si>
+    <t>When an attribute is exhausted any related actions cannot be performed. Meditating can be done at any time to restore attributes by consuming Will.</t>
+  </si>
+  <si>
+    <t>Restore Grit</t>
+  </si>
+  <si>
+    <t>As your Grit is currently exhausted, try restoring it by meditating. By doing this you can continue to explore without returning home to Sleep. Press [I] to open the inventory and navigate to the Meditate tab.</t>
+  </si>
+  <si>
     <t>This is your health bar. When it reaches zero, your current character dies. Other characters are expendable, but the Wanderer is not.</t>
   </si>
   <si>
@@ -3587,12 +3620,6 @@
     <t>This bar shows the remaining ammunition in your weapon. Although weapons have infinite ammunition, you still need to reload at the end of a clip.</t>
   </si>
   <si>
-    <t>Compass</t>
-  </si>
-  <si>
-    <t>You can consume compass charges to find hidden resources, enemies, and other locations of interest. The compass will show the direction of nearby points of interest.</t>
-  </si>
-  <si>
     <t>Enemies</t>
   </si>
   <si>
@@ -3645,9 +3672,6 @@
   </si>
   <si>
     <t>The sleep action will restore all your attributes over time. Sleeping can only be done at home, and character can be woken from sleep at any time.</t>
-  </si>
-  <si>
-    <t>Meditating</t>
   </si>
   <si>
     <t>The Meditate action allows you to consume Will to restore your other attributes instantly. Meditating can be done anywhere whilst your character still has Will.</t>
@@ -18618,10 +18642,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="7"/>
@@ -18819,25 +18843,25 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" t="s">
         <v>1177</v>
       </c>
       <c r="D8">
-        <v>650</v>
+        <v>780</v>
       </c>
       <c r="E8">
-        <v>905</v>
+        <v>425</v>
       </c>
       <c r="F8">
-        <v>650</v>
+        <v>780</v>
       </c>
       <c r="G8">
-        <v>25</v>
+        <v>360</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>1178</v>
@@ -18848,22 +18872,22 @@
         <v>3</v>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>810</v>
+        <v>560</v>
       </c>
       <c r="D9">
-        <v>1020</v>
+        <v>650</v>
       </c>
       <c r="E9">
-        <v>950</v>
+        <v>905</v>
       </c>
       <c r="F9">
-        <v>10</v>
+        <v>650</v>
       </c>
       <c r="G9">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>1179</v>
@@ -18871,351 +18895,351 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>822</v>
+        <v>1180</v>
       </c>
       <c r="D10">
+        <v>1010</v>
+      </c>
+      <c r="E10">
+        <v>1025</v>
+      </c>
+      <c r="F10">
+        <v>750</v>
+      </c>
+      <c r="G10">
         <v>10</v>
       </c>
-      <c r="E10">
-        <v>950</v>
-      </c>
-      <c r="F10">
-        <v>1020</v>
-      </c>
-      <c r="G10">
-        <v>35</v>
-      </c>
       <c r="H10" s="2" t="s">
-        <v>1180</v>
+        <v>1181</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>1181</v>
+        <v>1182</v>
       </c>
       <c r="D11">
-        <v>895</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>935</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>895</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>1182</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12">
         <v>3</v>
       </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
       <c r="C12" t="s">
-        <v>1183</v>
+        <v>1184</v>
       </c>
       <c r="D12">
-        <v>785</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>1010</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>1184</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>1185</v>
+        <v>1186</v>
       </c>
       <c r="D13">
-        <v>1010</v>
+        <v>0</v>
       </c>
       <c r="E13">
-        <v>1025</v>
+        <v>0</v>
       </c>
       <c r="F13">
-        <v>750</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>1186</v>
+        <v>1187</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>1187</v>
+        <v>1188</v>
       </c>
       <c r="D14">
-        <v>530</v>
+        <v>0</v>
       </c>
       <c r="E14">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F14">
-        <v>530</v>
+        <v>0</v>
       </c>
       <c r="G14">
-        <v>960</v>
+        <v>0</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>1188</v>
+        <v>1189</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>810</v>
       </c>
       <c r="D15">
-        <v>890</v>
+        <v>1020</v>
       </c>
       <c r="E15">
-        <v>45</v>
+        <v>950</v>
       </c>
       <c r="F15">
-        <v>890</v>
+        <v>10</v>
       </c>
       <c r="G15">
-        <v>915</v>
+        <v>35</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>1189</v>
+        <v>1190</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>822</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>950</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1020</v>
       </c>
       <c r="G16">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>1190</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="17" spans="1:8">
       <c r="A17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>1191</v>
+        <v>1192</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>895</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>935</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>895</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>1192</v>
+        <v>1193</v>
       </c>
     </row>
     <row r="18" spans="1:8">
       <c r="A18">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>823</v>
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1194</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>785</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1025</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>1010</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>1193</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="19" spans="1:8">
       <c r="A19">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C19" t="s">
-        <v>903</v>
+        <v>1196</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>530</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>530</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>960</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>1194</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="20" spans="1:8">
       <c r="A20">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>1195</v>
+        <v>4</v>
       </c>
       <c r="D20">
-        <v>650</v>
+        <v>890</v>
       </c>
       <c r="E20">
-        <v>315</v>
+        <v>45</v>
       </c>
       <c r="F20">
-        <v>650</v>
+        <v>890</v>
       </c>
       <c r="G20">
-        <v>640</v>
+        <v>915</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>1196</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="21" spans="1:8">
       <c r="A21">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>1197</v>
+        <v>3</v>
       </c>
       <c r="D21">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="E21">
-        <v>315</v>
+        <v>0</v>
       </c>
       <c r="F21">
-        <v>960</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>640</v>
+        <v>0</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>1199</v>
+        <v>1200</v>
       </c>
       <c r="D22">
-        <v>960</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>315</v>
+        <v>0</v>
       </c>
       <c r="F22">
-        <v>650</v>
+        <v>0</v>
       </c>
       <c r="G22">
-        <v>640</v>
+        <v>0</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>1200</v>
+        <v>1201</v>
       </c>
     </row>
     <row r="23" spans="1:8">
       <c r="A23">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B23">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
-        <v>1201</v>
+        <v>1</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>823</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -19229,109 +19253,109 @@
       <c r="G23">
         <v>0</v>
       </c>
-      <c r="H23" s="1" t="s">
+      <c r="H23" s="2" t="s">
         <v>1202</v>
       </c>
     </row>
     <row r="24" spans="1:8">
       <c r="A24">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
+        <v>903</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>1203</v>
-      </c>
-      <c r="D24">
-        <v>860</v>
-      </c>
-      <c r="E24">
-        <v>650</v>
-      </c>
-      <c r="F24">
-        <v>860</v>
-      </c>
-      <c r="G24">
-        <v>330</v>
-      </c>
-      <c r="H24" t="s">
-        <v>1204</v>
       </c>
     </row>
     <row r="25" spans="1:8">
       <c r="A25">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B25">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C25" t="s">
+        <v>1204</v>
+      </c>
+      <c r="D25">
+        <v>650</v>
+      </c>
+      <c r="E25">
+        <v>315</v>
+      </c>
+      <c r="F25">
+        <v>650</v>
+      </c>
+      <c r="G25">
+        <v>640</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>1205</v>
-      </c>
-      <c r="D25">
-        <v>860</v>
-      </c>
-      <c r="E25">
-        <v>615</v>
-      </c>
-      <c r="F25">
-        <v>860</v>
-      </c>
-      <c r="G25">
-        <v>370</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>1206</v>
       </c>
     </row>
     <row r="26" spans="1:8">
       <c r="A26">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>754</v>
+        <v>1206</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>650</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>960</v>
       </c>
       <c r="G26">
-        <v>0</v>
-      </c>
-      <c r="H26" t="s">
+        <v>640</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>1207</v>
       </c>
     </row>
     <row r="27" spans="1:8">
       <c r="A27">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B27">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
         <v>1208</v>
       </c>
       <c r="D27">
-        <v>645</v>
+        <v>960</v>
       </c>
       <c r="E27">
-        <v>385</v>
+        <v>315</v>
       </c>
       <c r="F27">
-        <v>645</v>
+        <v>650</v>
       </c>
       <c r="G27">
-        <v>600</v>
+        <v>640</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>1209</v>
@@ -19339,51 +19363,51 @@
     </row>
     <row r="28" spans="1:8">
       <c r="A28">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B28">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
         <v>1210</v>
       </c>
       <c r="D28">
-        <v>645</v>
+        <v>0</v>
       </c>
       <c r="E28">
-        <v>705</v>
+        <v>0</v>
       </c>
       <c r="F28">
-        <v>645</v>
+        <v>0</v>
       </c>
       <c r="G28">
-        <v>160</v>
-      </c>
-      <c r="H28" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>1211</v>
       </c>
     </row>
     <row r="29" spans="1:8">
       <c r="A29">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B29">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C29" t="s">
         <v>1212</v>
       </c>
       <c r="D29">
-        <v>20</v>
+        <v>860</v>
       </c>
       <c r="E29">
-        <v>10</v>
+        <v>650</v>
       </c>
       <c r="F29">
-        <v>20</v>
+        <v>860</v>
       </c>
       <c r="G29">
-        <v>970</v>
+        <v>330</v>
       </c>
       <c r="H29" t="s">
         <v>1213</v>
@@ -19391,129 +19415,129 @@
     </row>
     <row r="30" spans="1:8">
       <c r="A30">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>820</v>
+        <v>1186</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>860</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>615</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>860</v>
       </c>
       <c r="G30">
-        <v>0</v>
-      </c>
-      <c r="H30" t="s">
+        <v>370</v>
+      </c>
+      <c r="H30" s="2" t="s">
         <v>1214</v>
       </c>
     </row>
     <row r="31" spans="1:8">
       <c r="A31">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C31" t="s">
+        <v>754</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31" t="s">
         <v>1215</v>
-      </c>
-      <c r="D31">
-        <v>650</v>
-      </c>
-      <c r="E31">
-        <v>305</v>
-      </c>
-      <c r="F31">
-        <v>650</v>
-      </c>
-      <c r="G31">
-        <v>620</v>
-      </c>
-      <c r="H31" t="s">
-        <v>1216</v>
       </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32">
+        <v>9</v>
+      </c>
+      <c r="B32">
         <v>8</v>
       </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
       <c r="C32" t="s">
-        <v>672</v>
+        <v>1216</v>
       </c>
       <c r="D32">
-        <v>825</v>
+        <v>645</v>
       </c>
       <c r="E32">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F32">
-        <v>825</v>
+        <v>645</v>
       </c>
       <c r="G32">
-        <v>590</v>
-      </c>
-      <c r="H32" t="s">
+        <v>600</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>1217</v>
       </c>
     </row>
     <row r="33" spans="1:8">
       <c r="A33">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C33" t="s">
         <v>1218</v>
       </c>
       <c r="D33">
-        <v>825</v>
+        <v>645</v>
       </c>
       <c r="E33">
-        <v>390</v>
+        <v>705</v>
       </c>
       <c r="F33">
-        <v>825</v>
+        <v>645</v>
       </c>
       <c r="G33">
-        <v>590</v>
-      </c>
-      <c r="H33" t="s">
+        <v>160</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>1219</v>
       </c>
     </row>
     <row r="34" spans="1:8">
       <c r="A34">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B34">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
         <v>1220</v>
       </c>
       <c r="D34">
-        <v>1190</v>
+        <v>20</v>
       </c>
       <c r="E34">
-        <v>680</v>
+        <v>10</v>
       </c>
       <c r="F34">
-        <v>570</v>
+        <v>20</v>
       </c>
       <c r="G34">
-        <v>285</v>
+        <v>970</v>
       </c>
       <c r="H34" t="s">
         <v>1221</v>
@@ -19521,51 +19545,51 @@
     </row>
     <row r="35" spans="1:8">
       <c r="A35">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B35">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C35" t="s">
+        <v>820</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35" t="s">
         <v>1222</v>
-      </c>
-      <c r="D35">
-        <v>570</v>
-      </c>
-      <c r="E35">
-        <v>680</v>
-      </c>
-      <c r="F35">
-        <v>1190</v>
-      </c>
-      <c r="G35">
-        <v>285</v>
-      </c>
-      <c r="H35" t="s">
-        <v>1223</v>
       </c>
     </row>
     <row r="36" spans="1:8">
       <c r="A36">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
       <c r="C36" t="s">
-        <v>822</v>
+        <v>1223</v>
       </c>
       <c r="D36">
-        <v>460</v>
+        <v>650</v>
       </c>
       <c r="E36">
-        <v>300</v>
+        <v>305</v>
       </c>
       <c r="F36">
-        <v>460</v>
+        <v>650</v>
       </c>
       <c r="G36">
-        <v>615</v>
+        <v>620</v>
       </c>
       <c r="H36" t="s">
         <v>1224</v>
@@ -19573,51 +19597,51 @@
     </row>
     <row r="37" spans="1:8">
       <c r="A37">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37" t="s">
+        <v>672</v>
+      </c>
+      <c r="D37">
+        <v>825</v>
+      </c>
+      <c r="E37">
+        <v>390</v>
+      </c>
+      <c r="F37">
+        <v>825</v>
+      </c>
+      <c r="G37">
+        <v>590</v>
+      </c>
+      <c r="H37" t="s">
         <v>1225</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37" t="s">
-        <v>1226</v>
       </c>
     </row>
     <row r="38" spans="1:8">
       <c r="A38">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B38">
         <v>3</v>
       </c>
       <c r="C38" t="s">
-        <v>3</v>
+        <v>1226</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>825</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>825</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>590</v>
       </c>
       <c r="H38" t="s">
         <v>1227</v>
@@ -19625,7 +19649,7 @@
     </row>
     <row r="39" spans="1:8">
       <c r="A39">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B39">
         <v>4</v>
@@ -19634,16 +19658,16 @@
         <v>1228</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1190</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>680</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>570</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>285</v>
       </c>
       <c r="H39" t="s">
         <v>1229</v>
@@ -19651,25 +19675,25 @@
     </row>
     <row r="40" spans="1:8">
       <c r="A40">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
         <v>1230</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>570</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>680</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>1190</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>285</v>
       </c>
       <c r="H40" t="s">
         <v>1231</v>
@@ -19677,158 +19701,288 @@
     </row>
     <row r="41" spans="1:8">
       <c r="A41">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41" t="s">
+        <v>822</v>
+      </c>
+      <c r="D41">
+        <v>460</v>
+      </c>
+      <c r="E41">
+        <v>300</v>
+      </c>
+      <c r="F41">
+        <v>460</v>
+      </c>
+      <c r="G41">
+        <v>615</v>
+      </c>
+      <c r="H41" t="s">
         <v>1232</v>
-      </c>
-      <c r="D41">
-        <v>525</v>
-      </c>
-      <c r="E41">
-        <v>900</v>
-      </c>
-      <c r="F41">
-        <v>525</v>
-      </c>
-      <c r="G41">
-        <v>55</v>
-      </c>
-      <c r="H41" t="s">
-        <v>1233</v>
       </c>
     </row>
     <row r="42" spans="1:8">
       <c r="A42">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B42">
         <v>2</v>
       </c>
       <c r="C42" t="s">
+        <v>1233</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42" t="s">
         <v>1234</v>
-      </c>
-      <c r="D42">
-        <v>570</v>
-      </c>
-      <c r="E42">
-        <v>900</v>
-      </c>
-      <c r="F42">
-        <v>1020</v>
-      </c>
-      <c r="G42">
-        <v>55</v>
-      </c>
-      <c r="H42" t="s">
-        <v>1235</v>
       </c>
     </row>
     <row r="43" spans="1:8">
       <c r="A43">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B43">
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>1236</v>
+        <v>3</v>
       </c>
       <c r="D43">
-        <v>1020</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>570</v>
+        <v>0</v>
       </c>
       <c r="G43">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="H43" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="44" spans="1:8">
       <c r="A44">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B44">
         <v>4</v>
       </c>
       <c r="C44" t="s">
-        <v>589</v>
+        <v>1236</v>
       </c>
       <c r="D44">
-        <v>585</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>900</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>1195</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>110</v>
+        <v>0</v>
       </c>
       <c r="H44" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="45" spans="1:8">
       <c r="A45">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" t="s">
+        <v>1238</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45" t="s">
         <v>1239</v>
-      </c>
-      <c r="D45">
-        <v>0</v>
-      </c>
-      <c r="E45">
-        <v>0</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45" t="s">
-        <v>1240</v>
       </c>
     </row>
     <row r="46" spans="1:8">
       <c r="A46">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>1240</v>
+      </c>
+      <c r="D46">
+        <v>525</v>
+      </c>
+      <c r="E46">
+        <v>900</v>
+      </c>
+      <c r="F46">
+        <v>525</v>
+      </c>
+      <c r="G46">
+        <v>55</v>
+      </c>
+      <c r="H46" t="s">
+        <v>1241</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47">
+        <v>14</v>
+      </c>
+      <c r="B47">
         <v>2</v>
       </c>
-      <c r="C46" s="4" t="s">
-        <v>1241</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46" t="s">
+      <c r="C47" t="s">
         <v>1242</v>
+      </c>
+      <c r="D47">
+        <v>570</v>
+      </c>
+      <c r="E47">
+        <v>900</v>
+      </c>
+      <c r="F47">
+        <v>1020</v>
+      </c>
+      <c r="G47">
+        <v>55</v>
+      </c>
+      <c r="H47" t="s">
+        <v>1243</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48">
+        <v>14</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>1244</v>
+      </c>
+      <c r="D48">
+        <v>1020</v>
+      </c>
+      <c r="E48">
+        <v>900</v>
+      </c>
+      <c r="F48">
+        <v>570</v>
+      </c>
+      <c r="G48">
+        <v>55</v>
+      </c>
+      <c r="H48" t="s">
+        <v>1245</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="A49">
+        <v>14</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49" t="s">
+        <v>589</v>
+      </c>
+      <c r="D49">
+        <v>585</v>
+      </c>
+      <c r="E49">
+        <v>900</v>
+      </c>
+      <c r="F49">
+        <v>1195</v>
+      </c>
+      <c r="G49">
+        <v>110</v>
+      </c>
+      <c r="H49" t="s">
+        <v>1246</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="A50">
+        <v>15</v>
+      </c>
+      <c r="B50">
+        <v>1</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>1247</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50" t="s">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="A51">
+        <v>15</v>
+      </c>
+      <c r="B51">
+        <v>2</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>1249</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51" t="s">
+        <v>1250</v>
       </c>
     </row>
   </sheetData>
@@ -24249,7 +24403,7 @@
   <sheetPr/>
   <dimension ref="A1:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
<UI> Improved user experience
Enlarged close buttons.
Merged close buttons and ui background into prefabs.
Removed left, right, centre backgrounds, now just uses background.
Changed accept to space.
Changed button prompts to esc and spc.
Changed control scheme in menu.
Added rmb and drag to aim.
Improved readability of text in journals, etc.
Added MMB to use as well as T.
Added simple easy/hard difficulty setting and ui.
Fixed bullet trail returning to origin if it didn't hit anything.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -3438,14 +3438,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="0_ "/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="0_ "/>
-    <numFmt numFmtId="178" formatCode="0.0"/>
-    <numFmt numFmtId="179" formatCode="0.0_ "/>
+    <numFmt numFmtId="178" formatCode="0.0_ "/>
+    <numFmt numFmtId="179" formatCode="0.0"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -3514,15 +3514,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3543,17 +3542,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3566,7 +3559,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3596,24 +3589,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3643,8 +3620,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3773,7 +3773,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3791,25 +3929,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3821,139 +3953,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4349,8 +4349,38 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4374,22 +4404,27 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4408,47 +4443,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -4466,130 +4466,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="35" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="38" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="45" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="45" borderId="37" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="36" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="35" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4714,10 +4714,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="179" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4897,7 +4897,7 @@
     <xf numFmtId="1" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
@@ -4915,7 +4915,7 @@
     <xf numFmtId="1" fontId="0" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -30661,7 +30661,7 @@
   <dimension ref="A1:Q49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
<Feature, Bugfix, Audio> Bullets, Effects
Fixed weather appearing in front of screen fader.
Fixed pause button height.
Fixed blood spatter layer order.
Fixed grenade radius.
Fixed bug where loading travel action would cause enemies to not spawn.
Slightly changed ghast movement behaviour.
Added rite portal audio.
Added enemy/player/shield hit sounds.
Added gate transit audio.
Essence clouds disappear faster.
Increased recoil recovery rate.
Added music fade in main menu.
Fixed dismantle menu showing armour.
Dismantle menu responds to button clicks.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18620" firstSheet="2" activeTab="15"/>
+    <workbookView windowHeight="18620" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -17464,7 +17464,7 @@
   <sheetPr/>
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
@@ -24013,8 +24013,8 @@
   <sheetPr/>
   <dimension ref="A1:V102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>
@@ -24927,7 +24927,7 @@
         <v>0.05</v>
       </c>
       <c r="C21" s="106">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="D21" s="106">
         <v>0.15</v>
@@ -24936,21 +24936,21 @@
         <v>0.1</v>
       </c>
       <c r="F21" s="106">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="G21" s="106">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H21" s="106">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="I21">
         <f>SUM(B21:H21)</f>
-        <v>0.95</v>
+        <v>0.7</v>
       </c>
       <c r="J21" s="109">
         <f>I21/(SUM(I$21:I$27))</f>
-        <v>0.135714285714286</v>
+        <v>0.1</v>
       </c>
       <c r="K21" s="31"/>
       <c r="L21" s="31"/>
@@ -24961,7 +24961,7 @@
         <v>139</v>
       </c>
       <c r="B22" s="105">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="C22" s="106">
         <v>0.05</v>
@@ -24983,11 +24983,11 @@
       </c>
       <c r="I22">
         <f t="shared" ref="I22:I28" si="2">SUM(B22:H22)</f>
-        <v>0.8</v>
+        <v>0.75</v>
       </c>
       <c r="J22" s="109">
         <f t="shared" ref="J22:J27" si="3">I22/(SUM(I$21:I$27))</f>
-        <v>0.114285714285714</v>
+        <v>0.107142857142857</v>
       </c>
       <c r="K22" s="31"/>
       <c r="L22" s="31"/>
@@ -24998,7 +24998,7 @@
         <v>141</v>
       </c>
       <c r="B23" s="105">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="C23" s="106">
         <v>0.1</v>
@@ -25016,15 +25016,15 @@
         <v>0.1</v>
       </c>
       <c r="H23" s="106">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="I23">
         <f t="shared" si="2"/>
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="J23" s="109">
         <f t="shared" si="3"/>
-        <v>0.114285714285714</v>
+        <v>0.1</v>
       </c>
       <c r="K23" s="31"/>
       <c r="L23" s="31"/>
@@ -25035,7 +25035,7 @@
         <v>122</v>
       </c>
       <c r="B24" s="105">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="C24" s="106">
         <v>0.1</v>
@@ -25057,11 +25057,11 @@
       </c>
       <c r="I24">
         <f t="shared" si="2"/>
-        <v>0.7</v>
+        <v>0.75</v>
       </c>
       <c r="J24" s="109">
         <f t="shared" si="3"/>
-        <v>0.1</v>
+        <v>0.107142857142857</v>
       </c>
       <c r="K24" s="31"/>
       <c r="L24" s="31"/>
@@ -25072,10 +25072,10 @@
         <v>144</v>
       </c>
       <c r="B25" s="105">
+        <v>0.2</v>
+      </c>
+      <c r="C25" s="106">
         <v>0.25</v>
-      </c>
-      <c r="C25" s="106">
-        <v>0.2</v>
       </c>
       <c r="D25" s="106">
         <v>0.15</v>
@@ -25084,21 +25084,21 @@
         <v>0.2</v>
       </c>
       <c r="F25" s="106">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="G25" s="106">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="H25" s="106">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="I25">
         <f t="shared" si="2"/>
-        <v>1.25</v>
+        <v>1.4</v>
       </c>
       <c r="J25" s="109">
         <f t="shared" si="3"/>
-        <v>0.178571428571429</v>
+        <v>0.2</v>
       </c>
       <c r="K25" s="31"/>
       <c r="L25" s="31"/>
@@ -25109,7 +25109,7 @@
         <v>146</v>
       </c>
       <c r="B26" s="105">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="C26" s="106">
         <v>0.2</v>
@@ -25127,15 +25127,15 @@
         <v>0.1</v>
       </c>
       <c r="H26" s="106">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="I26">
         <f t="shared" si="2"/>
-        <v>1.25</v>
+        <v>1.35</v>
       </c>
       <c r="J26" s="109">
         <f t="shared" si="3"/>
-        <v>0.178571428571429</v>
+        <v>0.192857142857143</v>
       </c>
       <c r="K26" s="31"/>
       <c r="L26" s="31"/>
@@ -25146,7 +25146,7 @@
         <v>148</v>
       </c>
       <c r="B27" s="105">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="C27" s="106">
         <v>0.2</v>
@@ -25161,18 +25161,18 @@
         <v>0.2</v>
       </c>
       <c r="G27" s="106">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="H27" s="106">
         <v>0.05</v>
       </c>
       <c r="I27">
         <f t="shared" si="2"/>
-        <v>1.25</v>
+        <v>1.35</v>
       </c>
       <c r="J27" s="109">
         <f t="shared" si="3"/>
-        <v>0.178571428571429</v>
+        <v>0.192857142857143</v>
       </c>
       <c r="K27" s="31"/>
       <c r="L27" s="31"/>

</xml_diff>

<commit_message>
<Feature, Bugfix> Starfish, Claim
Claiming regions is permanent.
Claimed regions provide their bonus every 6 hours.
Improved claim visuals in combat and map.
Improved maelstrom shot visibility and animation.
Improved starfish animation.
Fixed starfish prewarm.
Added health to tomb, must be broken before boss spawns.
Fixed pause menu opening when invisible.
Fixed campfire not lighting.
Fixed autosave not being selected.
Most recent designation now given to save chronologically recent.
Fixed nightmare enemies not being pushed back.
Added pathing blocker to fountain/rite shrine/monument.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -15081,7 +15081,7 @@
   <dimension ref="A1:T69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>
@@ -16381,7 +16381,7 @@
       </c>
       <c r="O24" s="22">
         <f t="shared" ref="O24:O30" si="2">O$50*H25</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P24" s="22">
         <f t="shared" ref="P24:P30" si="3">P$50*I25</f>
@@ -16393,11 +16393,11 @@
       </c>
       <c r="R24" s="22">
         <f t="shared" ref="R24:R30" si="5">R$50*K25</f>
-        <v>6.25</v>
+        <v>7.5</v>
       </c>
       <c r="S24" s="22">
         <f t="shared" ref="S24:S30" si="6">SUM(N24:R24)</f>
-        <v>34.25</v>
+        <v>36.5</v>
       </c>
       <c r="T24" s="22"/>
     </row>
@@ -16419,7 +16419,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="12">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="I25" s="12">
         <v>0.2</v>
@@ -16428,7 +16428,7 @@
         <v>0.15</v>
       </c>
       <c r="K25" s="12">
-        <v>0.125</v>
+        <v>0.15</v>
       </c>
       <c r="M25" s="12"/>
       <c r="N25" s="22">
@@ -16437,11 +16437,11 @@
       </c>
       <c r="O25" s="22">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="P25" s="22">
         <f t="shared" si="3"/>
-        <v>6</v>
+        <v>7.5</v>
       </c>
       <c r="Q25" s="22">
         <f t="shared" si="4"/>
@@ -16449,11 +16449,11 @@
       </c>
       <c r="R25" s="22">
         <f t="shared" si="5"/>
-        <v>6.25</v>
+        <v>7.5</v>
       </c>
       <c r="S25" s="22">
         <f t="shared" si="6"/>
-        <v>24.25</v>
+        <v>28</v>
       </c>
       <c r="T25" s="22"/>
     </row>
@@ -16474,16 +16474,16 @@
         <v>0</v>
       </c>
       <c r="H26" s="12">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="I26" s="12">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="J26" s="20">
         <v>0.15</v>
       </c>
       <c r="K26" s="12">
-        <v>0.125</v>
+        <v>0.15</v>
       </c>
       <c r="M26" s="12"/>
       <c r="N26" s="22">
@@ -16504,11 +16504,11 @@
       </c>
       <c r="R26" s="22">
         <f t="shared" si="5"/>
-        <v>6.25</v>
+        <v>5</v>
       </c>
       <c r="S26" s="22">
         <f t="shared" si="6"/>
-        <v>22.25</v>
+        <v>21</v>
       </c>
       <c r="T26" s="22"/>
     </row>
@@ -16538,7 +16538,7 @@
         <v>0.15</v>
       </c>
       <c r="K27" s="12">
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="M27" s="12"/>
       <c r="N27" s="22">
@@ -16551,7 +16551,7 @@
       </c>
       <c r="P27" s="22">
         <f t="shared" si="3"/>
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="Q27" s="22">
         <f t="shared" si="4"/>
@@ -16559,11 +16559,11 @@
       </c>
       <c r="R27" s="22">
         <f t="shared" si="5"/>
-        <v>6.25</v>
+        <v>7.5</v>
       </c>
       <c r="S27" s="22">
         <f t="shared" si="6"/>
-        <v>18.75</v>
+        <v>18.5</v>
       </c>
       <c r="T27" s="22"/>
     </row>
@@ -16587,13 +16587,13 @@
         <v>0.1</v>
       </c>
       <c r="I28" s="12">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="J28" s="12">
         <v>0.15</v>
       </c>
       <c r="K28" s="12">
-        <v>0.125</v>
+        <v>0.15</v>
       </c>
       <c r="M28" s="12"/>
       <c r="N28" s="22">
@@ -16606,19 +16606,19 @@
       </c>
       <c r="P28" s="22">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>7.5</v>
       </c>
       <c r="Q28" s="22">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="R28" s="22">
         <f t="shared" si="5"/>
-        <v>6.25</v>
+        <v>7.5</v>
       </c>
       <c r="S28" s="22">
         <f t="shared" si="6"/>
-        <v>15.25</v>
+        <v>23</v>
       </c>
       <c r="T28" s="22"/>
     </row>
@@ -16642,13 +16642,13 @@
         <v>0</v>
       </c>
       <c r="I29" s="12">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="J29" s="12">
+        <v>0.2</v>
+      </c>
+      <c r="K29" s="12">
         <v>0.15</v>
-      </c>
-      <c r="K29" s="12">
-        <v>0.125</v>
       </c>
       <c r="M29" s="12"/>
       <c r="N29" s="22">
@@ -16665,15 +16665,15 @@
       </c>
       <c r="Q29" s="22">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="R29" s="22">
         <f t="shared" si="5"/>
-        <v>6.25</v>
+        <v>7.5</v>
       </c>
       <c r="S29" s="22">
         <f t="shared" si="6"/>
-        <v>8.25</v>
+        <v>13.5</v>
       </c>
       <c r="T29" s="22"/>
     </row>
@@ -16700,10 +16700,10 @@
         <v>0</v>
       </c>
       <c r="J30" s="12">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="K30" s="12">
-        <v>0.125</v>
+        <v>0.15</v>
       </c>
       <c r="M30" s="12"/>
       <c r="N30" s="22">
@@ -16724,11 +16724,11 @@
       </c>
       <c r="R30" s="22">
         <f t="shared" si="5"/>
-        <v>6.25</v>
+        <v>7.5</v>
       </c>
       <c r="S30" s="22">
         <f t="shared" si="6"/>
-        <v>8.25</v>
+        <v>9.5</v>
       </c>
       <c r="T30" s="22"/>
     </row>
@@ -16758,7 +16758,7 @@
         <v>0.05</v>
       </c>
       <c r="K31" s="12">
-        <v>0.125</v>
+        <v>0.15</v>
       </c>
       <c r="M31" s="12"/>
       <c r="N31" s="12"/>
@@ -17489,19 +17489,19 @@
       </c>
       <c r="N58" s="12">
         <f>SUM(H25:H34)</f>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="O58" s="12">
         <f>SUM(I25:I34)</f>
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="P58" s="12">
         <f>SUM(J25:J34)</f>
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="Q58" s="12">
         <f>SUM(K25:K34)</f>
-        <v>0.875</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="12:13">

</xml_diff>

<commit_message>
<Feature, Bugfix> Starfish, Audio
Ensured nightmare enemy works.
Added maelstrom shot audio.
Added starfish boss audio.
</commit_message>
<xml_diff>
--- a/Desolation Balance Files.xlsx
+++ b/Desolation Balance Files.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="18620" firstSheet="2" activeTab="4"/>
+    <workbookView windowHeight="18620" firstSheet="2" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Weapon Data v1" sheetId="2" state="hidden" r:id="rId1"/>
@@ -3306,14 +3306,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="8">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
     <numFmt numFmtId="177" formatCode="0_ "/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="0.0_ "/>
-    <numFmt numFmtId="179" formatCode="0.0"/>
+    <numFmt numFmtId="178" formatCode="0.0"/>
+    <numFmt numFmtId="179" formatCode="0.0_ "/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -3381,8 +3381,86 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3396,52 +3474,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3456,15 +3489,15 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3472,31 +3505,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3509,17 +3518,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3648,7 +3648,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3660,7 +3720,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3672,19 +3780,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3696,121 +3810,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3822,13 +3822,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4221,17 +4221,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4240,7 +4234,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4255,30 +4249,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -4299,6 +4269,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -4313,8 +4313,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -4323,148 +4323,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="37" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="42" borderId="39" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="42" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="36" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="41" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="46" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="34" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="37" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="47" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="48" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="50" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="51" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="45" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="49" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4559,10 +4559,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="178" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
@@ -4766,7 +4766,7 @@
     <xf numFmtId="1" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="0" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1">
@@ -4784,7 +4784,7 @@
     <xf numFmtId="1" fontId="0" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -12696,8 +12696,8 @@
   <sheetPr/>
   <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14545454545454" defaultRowHeight="14.5"/>
@@ -13609,7 +13609,7 @@
         <v>900</v>
       </c>
       <c r="D16" s="29">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E16" s="29">
         <v>4</v>
@@ -27338,7 +27338,7 @@
   <sheetPr/>
   <dimension ref="A1:X65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -29755,23 +29755,23 @@
         <v>2</v>
       </c>
       <c r="F3" s="64">
-        <f>SUM(B3:E3)</f>
+        <f t="shared" ref="F3:F8" si="0">SUM(B3:E3)</f>
         <v>12</v>
       </c>
       <c r="G3" s="64">
-        <f>C3*50</f>
+        <f t="shared" ref="G3:G8" si="1">C3*50</f>
         <v>150</v>
       </c>
       <c r="H3" s="71">
-        <f>-0.025*D3+1</f>
+        <f t="shared" ref="H3:H8" si="2">-0.025*D3+1</f>
         <v>0.875</v>
       </c>
       <c r="I3" s="71">
-        <f>0.1*E3+1</f>
+        <f t="shared" ref="I3:I8" si="3">0.1*E3+1</f>
         <v>1.2</v>
       </c>
       <c r="J3" s="71">
-        <f>5+B3*0.25</f>
+        <f t="shared" ref="J3:J8" si="4">5+B3*0.25</f>
         <v>5.5</v>
       </c>
       <c r="K3" s="74"/>
@@ -29793,23 +29793,23 @@
         <v>3</v>
       </c>
       <c r="F4" s="64">
-        <f>SUM(B4:E4)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="G4" s="64">
-        <f>C4*50</f>
+        <f t="shared" si="1"/>
         <v>250</v>
       </c>
       <c r="H4" s="71">
-        <f>-0.025*D4+1</f>
+        <f t="shared" si="2"/>
         <v>0.95</v>
       </c>
       <c r="I4" s="71">
-        <f>0.1*E4+1</f>
+        <f t="shared" si="3"/>
         <v>1.3</v>
       </c>
       <c r="J4" s="71">
-        <f>5+B4*0.25</f>
+        <f t="shared" si="4"/>
         <v>5.5</v>
       </c>
       <c r="K4" s="74"/>
@@ -29831,23 +29831,23 @@
         <v>2</v>
       </c>
       <c r="F5" s="64">
-        <f>SUM(B5:E5)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="G5" s="64">
-        <f>C5*50</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="H5" s="71">
-        <f>-0.025*D5+1</f>
+        <f t="shared" si="2"/>
         <v>0.9</v>
       </c>
       <c r="I5" s="71">
-        <f>0.1*E5+1</f>
+        <f t="shared" si="3"/>
         <v>1.2</v>
       </c>
       <c r="J5" s="71">
-        <f>5+B5*0.25</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="K5" s="75"/>
@@ -29869,23 +29869,23 @@
         <v>2</v>
       </c>
       <c r="F6" s="64">
-        <f>SUM(B6:E6)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="G6" s="64">
-        <f>C6*50</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="H6" s="71">
-        <f>-0.025*D6+1</f>
+        <f t="shared" si="2"/>
         <v>0.925</v>
       </c>
       <c r="I6" s="71">
-        <f>0.1*E6+1</f>
+        <f t="shared" si="3"/>
         <v>1.2</v>
       </c>
       <c r="J6" s="71">
-        <f>5+B6*0.25</f>
+        <f t="shared" si="4"/>
         <v>5.75</v>
       </c>
       <c r="K6" s="74"/>
@@ -29907,23 +29907,23 @@
         <v>3</v>
       </c>
       <c r="F7" s="64">
-        <f>SUM(B7:E7)</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="G7" s="64">
-        <f>C7*50</f>
+        <f t="shared" si="1"/>
         <v>100</v>
       </c>
       <c r="H7" s="71">
-        <f>-0.025*D7+1</f>
+        <f t="shared" si="2"/>
         <v>0.95</v>
       </c>
       <c r="I7" s="71">
-        <f>0.1*E7+1</f>
+        <f t="shared" si="3"/>
         <v>1.3</v>
       </c>
       <c r="J7" s="71">
-        <f>5+B7*0.25</f>
+        <f t="shared" si="4"/>
         <v>6.25</v>
       </c>
       <c r="K7" s="75"/>
@@ -29945,23 +29945,23 @@
         <v>4</v>
       </c>
       <c r="F8" s="64">
-        <f>SUM(B8:E8)</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="G8" s="64">
-        <f>C8*50</f>
+        <f t="shared" si="1"/>
         <v>200</v>
       </c>
       <c r="H8" s="71">
-        <f>-0.025*D8+1</f>
+        <f t="shared" si="2"/>
         <v>0.9</v>
       </c>
       <c r="I8" s="71">
-        <f>0.1*E8+1</f>
+        <f t="shared" si="3"/>
         <v>1.4</v>
       </c>
       <c r="J8" s="71">
-        <f>5+B8*0.25</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="K8" s="74"/>
@@ -30046,39 +30046,39 @@
         <v>603</v>
       </c>
       <c r="B16" s="64">
-        <f>B3+9</f>
+        <f t="shared" ref="B16:B21" si="5">B3+9</f>
         <v>11</v>
       </c>
       <c r="C16" s="64">
-        <f>C3+9</f>
+        <f t="shared" ref="C16:C21" si="6">C3+9</f>
         <v>12</v>
       </c>
       <c r="D16" s="64">
-        <f>D3+9</f>
+        <f t="shared" ref="D16:D21" si="7">D3+9</f>
         <v>14</v>
       </c>
       <c r="E16" s="64">
-        <f>E3+9</f>
+        <f t="shared" ref="E16:E21" si="8">E3+9</f>
         <v>11</v>
       </c>
       <c r="F16" s="64">
-        <f>SUM(B16:E16)</f>
+        <f t="shared" ref="F16:F21" si="9">SUM(B16:E16)</f>
         <v>48</v>
       </c>
       <c r="G16" s="64">
-        <f>C16*50</f>
+        <f t="shared" ref="G16:G21" si="10">C16*50</f>
         <v>600</v>
       </c>
       <c r="H16" s="71">
-        <f>-0.025*D16+1</f>
+        <f t="shared" ref="H16:H21" si="11">-0.025*D16+1</f>
         <v>0.65</v>
       </c>
       <c r="I16" s="71">
-        <f>0.1*E16+1</f>
+        <f t="shared" ref="I16:I21" si="12">0.1*E16+1</f>
         <v>2.1</v>
       </c>
       <c r="J16" s="71">
-        <f>5+B16*0.25</f>
+        <f t="shared" ref="J16:J21" si="13">5+B16*0.25</f>
         <v>7.75</v>
       </c>
     </row>
@@ -30087,39 +30087,39 @@
         <v>414</v>
       </c>
       <c r="B17" s="64">
-        <f>B4+9</f>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="C17" s="64">
-        <f>C4+9</f>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
       <c r="D17" s="64">
-        <f>D4+9</f>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="E17" s="64">
-        <f>E4+9</f>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="F17" s="64">
-        <f>SUM(B17:E17)</f>
+        <f t="shared" si="9"/>
         <v>48</v>
       </c>
       <c r="G17" s="64">
-        <f>C17*50</f>
+        <f t="shared" si="10"/>
         <v>700</v>
       </c>
       <c r="H17" s="71">
-        <f>-0.025*D17+1</f>
+        <f t="shared" si="11"/>
         <v>0.725</v>
       </c>
       <c r="I17" s="71">
-        <f>0.1*E17+1</f>
+        <f t="shared" si="12"/>
         <v>2.2</v>
       </c>
       <c r="J17" s="71">
-        <f>5+B17*0.25</f>
+        <f t="shared" si="13"/>
         <v>7.75</v>
       </c>
     </row>
@@ -30128,39 +30128,39 @@
         <v>604</v>
       </c>
       <c r="B18" s="64">
-        <f>B5+9</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="C18" s="64">
-        <f>C5+9</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="D18" s="64">
-        <f>D5+9</f>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="E18" s="64">
-        <f>E5+9</f>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="F18" s="64">
-        <f>SUM(B18:E18)</f>
+        <f t="shared" si="9"/>
         <v>48</v>
       </c>
       <c r="G18" s="64">
-        <f>C18*50</f>
+        <f t="shared" si="10"/>
         <v>550</v>
       </c>
       <c r="H18" s="71">
-        <f>-0.025*D18+1</f>
+        <f t="shared" si="11"/>
         <v>0.675</v>
       </c>
       <c r="I18" s="71">
-        <f>0.1*E18+1</f>
+        <f t="shared" si="12"/>
         <v>2.1</v>
       </c>
       <c r="J18" s="71">
-        <f>5+B18*0.25</f>
+        <f t="shared" si="13"/>
         <v>8.25</v>
       </c>
     </row>
@@ -30169,39 +30169,39 @@
         <v>605</v>
       </c>
       <c r="B19" s="64">
-        <f>B6+9</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="C19" s="64">
-        <f>C6+9</f>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="D19" s="64">
-        <f>D6+9</f>
+        <f t="shared" si="7"/>
         <v>12</v>
       </c>
       <c r="E19" s="64">
-        <f>E6+9</f>
+        <f t="shared" si="8"/>
         <v>11</v>
       </c>
       <c r="F19" s="64">
-        <f>SUM(B19:E19)</f>
+        <f t="shared" si="9"/>
         <v>48</v>
       </c>
       <c r="G19" s="64">
-        <f>C19*50</f>
+        <f t="shared" si="10"/>
         <v>650</v>
       </c>
       <c r="H19" s="71">
-        <f>-0.025*D19+1</f>
+        <f t="shared" si="11"/>
         <v>0.7</v>
       </c>
       <c r="I19" s="71">
-        <f>0.1*E19+1</f>
+        <f t="shared" si="12"/>
         <v>2.1</v>
       </c>
       <c r="J19" s="71">
-        <f>5+B19*0.25</f>
+        <f t="shared" si="13"/>
         <v>8</v>
       </c>
     </row>
@@ -30210,39 +30210,39 @@
         <v>269</v>
       </c>
       <c r="B20" s="64">
-        <f>B7+9</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="C20" s="64">
-        <f>C7+9</f>
+        <f t="shared" si="6"/>
         <v>11</v>
       </c>
       <c r="D20" s="64">
-        <f>D7+9</f>
+        <f t="shared" si="7"/>
         <v>11</v>
       </c>
       <c r="E20" s="64">
-        <f>E7+9</f>
+        <f t="shared" si="8"/>
         <v>12</v>
       </c>
       <c r="F20" s="64">
-        <f>SUM(B20:E20)</f>
+        <f t="shared" si="9"/>
         <v>48</v>
       </c>
       <c r="G20" s="64">
-        <f>C20*50</f>
+        <f t="shared" si="10"/>
         <v>550</v>
       </c>
       <c r="H20" s="71">
-        <f>-0.025*D20+1</f>
+        <f t="shared" si="11"/>
         <v>0.725</v>
       </c>
       <c r="I20" s="71">
-        <f>0.1*E20+1</f>
+        <f t="shared" si="12"/>
         <v>2.2</v>
       </c>
       <c r="J20" s="71">
-        <f>5+B20*0.25</f>
+        <f t="shared" si="13"/>
         <v>8.5</v>
       </c>
     </row>
@@ -30251,39 +30251,39 @@
         <v>606</v>
       </c>
       <c r="B21" s="64">
-        <f>B8+9</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="C21" s="64">
-        <f>C8+9</f>
+        <f t="shared" si="6"/>
         <v>13</v>
       </c>
       <c r="D21" s="64">
-        <f>D8+9</f>
+        <f t="shared" si="7"/>
         <v>13</v>
       </c>
       <c r="E21" s="64">
-        <f>E8+9</f>
+        <f t="shared" si="8"/>
         <v>13</v>
       </c>
       <c r="F21" s="64">
-        <f>SUM(B21:E21)</f>
+        <f t="shared" si="9"/>
         <v>52</v>
       </c>
       <c r="G21" s="64">
-        <f>C21*50</f>
+        <f t="shared" si="10"/>
         <v>650</v>
       </c>
       <c r="H21" s="71">
-        <f>-0.025*D21+1</f>
+        <f t="shared" si="11"/>
         <v>0.675</v>
       </c>
       <c r="I21" s="71">
-        <f>0.1*E21+1</f>
+        <f t="shared" si="12"/>
         <v>2.3</v>
       </c>
       <c r="J21" s="71">
-        <f>5+B21*0.25</f>
+        <f t="shared" si="13"/>
         <v>8.25</v>
       </c>
     </row>

</xml_diff>